<commit_message>
QC code and plot updates
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="15600" activeTab="1"/>
+    <workbookView xWindow="7540" yWindow="0" windowWidth="24500" windowHeight="15360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="treatments.csv" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="48">
   <si>
     <t>Treatment</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Time_set_start_UTC</t>
+  </si>
+  <si>
+    <t>Ambient4</t>
+  </si>
+  <si>
+    <t>Ambient22</t>
   </si>
 </sst>
 </file>
@@ -820,11 +826,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -850,35 +856,29 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C3">
-        <v>22</v>
-      </c>
-      <c r="D3">
-        <v>1162.7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>22</v>
       </c>
-      <c r="D4">
-        <v>1253.8</v>
-      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
@@ -887,12 +887,12 @@
         <v>22</v>
       </c>
       <c r="D5">
-        <v>1139.9000000000001</v>
+        <v>1162.7</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
@@ -901,12 +901,12 @@
         <v>22</v>
       </c>
       <c r="D6">
-        <v>1185.5</v>
+        <v>1253.8</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>32</v>
@@ -915,12 +915,12 @@
         <v>22</v>
       </c>
       <c r="D7">
-        <v>1231</v>
+        <v>1139.9000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
@@ -934,35 +934,35 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>22</v>
       </c>
       <c r="D9">
-        <v>1162.7</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10">
         <v>22</v>
       </c>
       <c r="D10">
-        <v>1071.5</v>
+        <v>1185.5</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -971,12 +971,12 @@
         <v>22</v>
       </c>
       <c r="D11">
-        <v>1048.7</v>
+        <v>1162.7</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
@@ -985,12 +985,12 @@
         <v>22</v>
       </c>
       <c r="D12">
-        <v>1299.4000000000001</v>
+        <v>1071.5</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>33</v>
@@ -999,12 +999,12 @@
         <v>22</v>
       </c>
       <c r="D13">
-        <v>1139.9000000000001</v>
+        <v>1048.7</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
@@ -1013,40 +1013,40 @@
         <v>22</v>
       </c>
       <c r="D14">
-        <v>1094.3</v>
+        <v>1299.4000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C15">
         <v>22</v>
       </c>
       <c r="D15">
-        <v>1025.9000000000001</v>
+        <v>1139.9000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16">
         <v>22</v>
       </c>
       <c r="D16">
-        <v>1162.7</v>
+        <v>1094.3</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
@@ -1055,12 +1055,12 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>1299.4000000000001</v>
+        <v>1025.9000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
@@ -1069,12 +1069,12 @@
         <v>22</v>
       </c>
       <c r="D18">
-        <v>957.5</v>
+        <v>1162.7</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
@@ -1083,12 +1083,12 @@
         <v>22</v>
       </c>
       <c r="D19">
-        <v>1253.8</v>
+        <v>1299.4000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>35</v>
@@ -1097,40 +1097,40 @@
         <v>22</v>
       </c>
       <c r="D20">
-        <v>1094.3</v>
+        <v>957.5</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D21">
-        <v>957.5</v>
+        <v>1253.8</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D22">
-        <v>1185.5</v>
+        <v>1094.3</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
@@ -1139,12 +1139,12 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>1094.3</v>
+        <v>957.5</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
@@ -1153,12 +1153,12 @@
         <v>4</v>
       </c>
       <c r="D24">
-        <v>1139.9000000000001</v>
+        <v>1185.5</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
         <v>32</v>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
@@ -1181,40 +1181,40 @@
         <v>4</v>
       </c>
       <c r="D26">
-        <v>1185.5</v>
+        <v>1139.9000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27">
         <v>4</v>
       </c>
       <c r="D27">
-        <v>1242.4000000000001</v>
+        <v>1094.3</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
       <c r="D28">
-        <v>1048.7</v>
+        <v>1185.5</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
         <v>33</v>
@@ -1223,12 +1223,12 @@
         <v>4</v>
       </c>
       <c r="D29">
-        <v>1162.7</v>
+        <v>1242.4000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
@@ -1237,12 +1237,12 @@
         <v>4</v>
       </c>
       <c r="D30">
-        <v>1139.9000000000001</v>
+        <v>1048.7</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
         <v>33</v>
@@ -1251,12 +1251,12 @@
         <v>4</v>
       </c>
       <c r="D31">
-        <v>1231</v>
+        <v>1162.7</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -1265,6 +1265,34 @@
         <v>4</v>
       </c>
       <c r="D32">
+        <v>1139.9000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
         <v>1162.7</v>
       </c>
     </row>
@@ -1285,7 +1313,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1336,7 +1364,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1473,7 +1501,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1610,7 +1638,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1747,7 +1775,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1884,7 +1912,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2021,7 +2049,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2158,7 +2186,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2295,7 +2323,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2432,7 +2460,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2569,7 +2597,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -2706,7 +2734,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2843,7 +2871,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2980,7 +3008,7 @@
         <v>10</v>
       </c>
       <c r="E87" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -3117,7 +3145,7 @@
         <v>10</v>
       </c>
       <c r="E94" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3254,7 +3282,7 @@
         <v>10</v>
       </c>
       <c r="E101" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -3391,7 +3419,7 @@
         <v>10</v>
       </c>
       <c r="E108" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -3528,7 +3556,7 @@
         <v>10</v>
       </c>
       <c r="E115" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -3665,7 +3693,7 @@
         <v>10</v>
       </c>
       <c r="E122" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -3802,7 +3830,7 @@
         <v>10</v>
       </c>
       <c r="E129" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3939,7 +3967,7 @@
         <v>10</v>
       </c>
       <c r="E136" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="137" spans="1:6">

</xml_diff>

<commit_message>
Sep 8 and Sep 11 data update
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7540" yWindow="0" windowWidth="24500" windowHeight="15360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="treatments.csv" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="50">
   <si>
     <t>Treatment</t>
   </si>
@@ -165,13 +165,19 @@
   <si>
     <t>Ambient22</t>
   </si>
+  <si>
+    <t xml:space="preserve">10ml water added 9/10/2015 accidental </t>
+  </si>
+  <si>
+    <t xml:space="preserve">30ml water added 9/10/2015 accidental </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -234,7 +240,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="141">
+  <cellStyleXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -376,17 +382,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="141">
+  <cellStyles count="155">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -457,6 +476,13 @@
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -527,6 +553,13 @@
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -835,8 +868,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="18">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="18">
+      <c r="A1" s="3" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1309,21 +1342,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:G214"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <pane ySplit="2" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A215" sqref="A215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="18">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="18">
+      <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1334,7 +1367,7 @@
       <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D2" t="s">
@@ -1351,13 +1384,13 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>42247</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="5">
         <v>0.72083333333333333</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3">
@@ -1368,13 +1401,13 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>42247</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>0.75</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4">
@@ -1388,13 +1421,13 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>42247</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="5">
         <v>0.75</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5">
@@ -1408,13 +1441,13 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>42247</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
         <v>0.75</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6">
@@ -1428,13 +1461,13 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>42247</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <v>0.75</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7">
@@ -1448,13 +1481,13 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>42247</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="5">
         <v>0.75</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8">
@@ -1468,13 +1501,13 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>42247</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <v>0.75</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="D9">
@@ -1488,13 +1521,13 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>42247</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="5">
         <v>0.77083333333333326</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>2</v>
       </c>
       <c r="D10">
@@ -1505,13 +1538,13 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>42247</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>2</v>
       </c>
       <c r="D11">
@@ -1525,13 +1558,13 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>42247</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>2</v>
       </c>
       <c r="D12">
@@ -1545,13 +1578,13 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>42247</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>2</v>
       </c>
       <c r="D13">
@@ -1565,13 +1598,13 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>42247</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>2</v>
       </c>
       <c r="D14">
@@ -1585,13 +1618,13 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>42247</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>2</v>
       </c>
       <c r="D15">
@@ -1605,13 +1638,13 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>42247</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>2</v>
       </c>
       <c r="D16">
@@ -1625,13 +1658,13 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>42247</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="5">
         <v>0.84375</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>3</v>
       </c>
       <c r="D17">
@@ -1642,13 +1675,13 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>42247</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="5">
         <v>0.85069444444444442</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>3</v>
       </c>
       <c r="D18">
@@ -1662,13 +1695,13 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>42247</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="5">
         <v>0.85069444444444442</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>3</v>
       </c>
       <c r="D19">
@@ -1682,13 +1715,13 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>42247</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="5">
         <v>0.85069444444444442</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>3</v>
       </c>
       <c r="D20">
@@ -1702,13 +1735,13 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>42247</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="5">
         <v>0.85069444444444442</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>3</v>
       </c>
       <c r="D21">
@@ -1722,13 +1755,13 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>42247</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="5">
         <v>0.85069444444444442</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>3</v>
       </c>
       <c r="D22">
@@ -1742,13 +1775,13 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>42247</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="5">
         <v>0.85069444444444442</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>3</v>
       </c>
       <c r="D23">
@@ -1762,13 +1795,13 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>42247</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="5">
         <v>0.875</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>4</v>
       </c>
       <c r="D24">
@@ -1779,13 +1812,13 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>42247</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>4</v>
       </c>
       <c r="D25">
@@ -1799,13 +1832,13 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>42247</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2">
         <v>4</v>
       </c>
       <c r="D26">
@@ -1819,13 +1852,13 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>42247</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>4</v>
       </c>
       <c r="D27">
@@ -1839,13 +1872,13 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>42247</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>4</v>
       </c>
       <c r="D28">
@@ -1859,13 +1892,13 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>42247</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>4</v>
       </c>
       <c r="D29">
@@ -1879,13 +1912,13 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>42247</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>4</v>
       </c>
       <c r="D30">
@@ -1899,13 +1932,13 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>42247</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>5</v>
       </c>
       <c r="D31">
@@ -1916,13 +1949,13 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>42247</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2">
         <v>5</v>
       </c>
       <c r="D32">
@@ -1936,13 +1969,13 @@
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>42247</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2">
         <v>5</v>
       </c>
       <c r="D33">
@@ -1956,13 +1989,13 @@
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>42247</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <v>5</v>
       </c>
       <c r="D34">
@@ -1976,13 +2009,13 @@
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>42247</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2">
         <v>5</v>
       </c>
       <c r="D35">
@@ -1996,13 +2029,13 @@
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>42247</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2">
         <v>5</v>
       </c>
       <c r="D36">
@@ -2016,13 +2049,13 @@
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>42247</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="5">
         <v>0.93055555555555558</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2">
         <v>5</v>
       </c>
       <c r="D37">
@@ -2036,13 +2069,13 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>42248</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="5">
         <v>0.78055555555555545</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2">
         <v>1</v>
       </c>
       <c r="D38">
@@ -2053,13 +2086,13 @@
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <v>42248</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="2">
         <v>3</v>
       </c>
       <c r="D39">
@@ -2073,13 +2106,13 @@
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>42248</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="2">
         <v>3</v>
       </c>
       <c r="D40">
@@ -2093,13 +2126,13 @@
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="2">
+      <c r="A41" s="1">
         <v>42248</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="2">
         <v>3</v>
       </c>
       <c r="D41">
@@ -2113,13 +2146,13 @@
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>42248</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="2">
         <v>3</v>
       </c>
       <c r="D42">
@@ -2133,13 +2166,13 @@
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="2">
+      <c r="A43" s="1">
         <v>42248</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="2">
         <v>3</v>
       </c>
       <c r="D43">
@@ -2153,13 +2186,13 @@
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>42248</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="5">
         <v>0.8125</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="2">
         <v>3</v>
       </c>
       <c r="D44">
@@ -2173,13 +2206,13 @@
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>42248</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="5">
         <v>0.84305555555555545</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2">
         <v>1</v>
       </c>
       <c r="D45">
@@ -2190,13 +2223,13 @@
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="2">
+      <c r="A46" s="1">
         <v>42248</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="5">
         <v>0.84722222222222232</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="2">
         <v>4</v>
       </c>
       <c r="D46">
@@ -2210,13 +2243,13 @@
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="2">
+      <c r="A47" s="1">
         <v>42248</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="5">
         <v>0.84722222222222232</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="2">
         <v>4</v>
       </c>
       <c r="D47">
@@ -2230,13 +2263,13 @@
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>42248</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="5">
         <v>0.84722222222222232</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="2">
         <v>4</v>
       </c>
       <c r="D48">
@@ -2250,13 +2283,13 @@
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>42248</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="5">
         <v>0.84722222222222232</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="2">
         <v>4</v>
       </c>
       <c r="D49">
@@ -2270,13 +2303,13 @@
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>42248</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="5">
         <v>0.84722222222222232</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="2">
         <v>4</v>
       </c>
       <c r="D50">
@@ -2290,13 +2323,13 @@
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="2">
+      <c r="A51" s="1">
         <v>42248</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="5">
         <v>0.84722222222222232</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="2">
         <v>4</v>
       </c>
       <c r="D51">
@@ -2310,13 +2343,13 @@
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="2">
+      <c r="A52" s="1">
         <v>42248</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="5">
         <v>0.875</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="2">
         <v>1</v>
       </c>
       <c r="D52">
@@ -2327,13 +2360,13 @@
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="2">
+      <c r="A53" s="1">
         <v>42248</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="5">
         <v>0.90625</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="2">
         <v>5</v>
       </c>
       <c r="D53">
@@ -2347,13 +2380,13 @@
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="2">
+      <c r="A54" s="1">
         <v>42248</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="5">
         <v>0.90625</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="2">
         <v>5</v>
       </c>
       <c r="D54">
@@ -2367,13 +2400,13 @@
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="2">
+      <c r="A55" s="1">
         <v>42248</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="5">
         <v>0.90625</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="2">
         <v>5</v>
       </c>
       <c r="D55">
@@ -2387,13 +2420,13 @@
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="2">
+      <c r="A56" s="1">
         <v>42248</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="5">
         <v>0.90625</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="2">
         <v>5</v>
       </c>
       <c r="D56">
@@ -2407,13 +2440,13 @@
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="2">
+      <c r="A57" s="1">
         <v>42248</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="5">
         <v>0.90625</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="2">
         <v>5</v>
       </c>
       <c r="D57">
@@ -2427,13 +2460,13 @@
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="2">
+      <c r="A58" s="1">
         <v>42248</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="5">
         <v>0.90625</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="2">
         <v>5</v>
       </c>
       <c r="D58">
@@ -2447,13 +2480,13 @@
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="2">
+      <c r="A59" s="1">
         <v>42248</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="5">
         <v>0.71875</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59" s="2">
         <v>1</v>
       </c>
       <c r="D59">
@@ -2464,13 +2497,13 @@
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="2">
+      <c r="A60" s="1">
         <v>42248</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="5">
         <v>0.71875</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="2">
         <v>1</v>
       </c>
       <c r="D60">
@@ -2484,13 +2517,13 @@
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="2">
+      <c r="A61" s="1">
         <v>42248</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="5">
         <v>0.71875</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="2">
         <v>1</v>
       </c>
       <c r="D61">
@@ -2504,13 +2537,13 @@
       </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="2">
+      <c r="A62" s="1">
         <v>42248</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="5">
         <v>0.71875</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C62" s="2">
         <v>1</v>
       </c>
       <c r="D62">
@@ -2524,13 +2557,13 @@
       </c>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="2">
+      <c r="A63" s="1">
         <v>42248</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="5">
         <v>0.71875</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C63" s="2">
         <v>1</v>
       </c>
       <c r="D63">
@@ -2544,13 +2577,13 @@
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="2">
+      <c r="A64" s="1">
         <v>42248</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64" s="5">
         <v>0.71875</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64" s="2">
         <v>1</v>
       </c>
       <c r="D64">
@@ -2564,13 +2597,13 @@
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="2">
+      <c r="A65" s="1">
         <v>42248</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65" s="5">
         <v>0.71875</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C65" s="2">
         <v>1</v>
       </c>
       <c r="D65">
@@ -2584,13 +2617,13 @@
       </c>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="2">
+      <c r="A66" s="1">
         <v>42248</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="5">
         <v>0.74305555555555558</v>
       </c>
-      <c r="C66" s="3">
+      <c r="C66" s="2">
         <v>1</v>
       </c>
       <c r="D66">
@@ -2601,13 +2634,13 @@
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="2">
+      <c r="A67" s="1">
         <v>42248</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="5">
         <v>0.75</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67" s="2">
         <v>2</v>
       </c>
       <c r="D67">
@@ -2621,13 +2654,13 @@
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="2">
+      <c r="A68" s="1">
         <v>42248</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="5">
         <v>0.75</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68" s="2">
         <v>2</v>
       </c>
       <c r="D68">
@@ -2641,13 +2674,13 @@
       </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="2">
+      <c r="A69" s="1">
         <v>42248</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69" s="5">
         <v>0.75</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C69" s="2">
         <v>2</v>
       </c>
       <c r="D69">
@@ -2661,13 +2694,13 @@
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="2">
+      <c r="A70" s="1">
         <v>42248</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="5">
         <v>0.75</v>
       </c>
-      <c r="C70" s="3">
+      <c r="C70" s="2">
         <v>2</v>
       </c>
       <c r="D70">
@@ -2681,13 +2714,13 @@
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="2">
+      <c r="A71" s="1">
         <v>42248</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="5">
         <v>0.75</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C71" s="2">
         <v>2</v>
       </c>
       <c r="D71">
@@ -2701,13 +2734,13 @@
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="2">
+      <c r="A72" s="1">
         <v>42248</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="5">
         <v>0.75</v>
       </c>
-      <c r="C72" s="3">
+      <c r="C72" s="2">
         <v>2</v>
       </c>
       <c r="D72">
@@ -2721,13 +2754,13 @@
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="2">
+      <c r="A73" s="1">
         <v>42250</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73" s="5">
         <v>0.75</v>
       </c>
-      <c r="C73" s="3">
+      <c r="C73" s="2">
         <v>1</v>
       </c>
       <c r="D73">
@@ -2738,13 +2771,13 @@
       </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="2">
+      <c r="A74" s="1">
         <v>42250</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="5">
         <v>0.77500000000000002</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C74" s="2">
         <v>1</v>
       </c>
       <c r="D74">
@@ -2758,13 +2791,13 @@
       </c>
     </row>
     <row r="75" spans="1:6">
-      <c r="A75" s="2">
+      <c r="A75" s="1">
         <v>42250</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75" s="5">
         <v>0.77500000000000002</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C75" s="2">
         <v>1</v>
       </c>
       <c r="D75">
@@ -2778,13 +2811,13 @@
       </c>
     </row>
     <row r="76" spans="1:6">
-      <c r="A76" s="2">
+      <c r="A76" s="1">
         <v>42250</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="5">
         <v>0.77500000000000002</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C76" s="2">
         <v>1</v>
       </c>
       <c r="D76">
@@ -2798,13 +2831,13 @@
       </c>
     </row>
     <row r="77" spans="1:6">
-      <c r="A77" s="2">
+      <c r="A77" s="1">
         <v>42250</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B77" s="5">
         <v>0.77500000000000002</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C77" s="2">
         <v>1</v>
       </c>
       <c r="D77">
@@ -2818,13 +2851,13 @@
       </c>
     </row>
     <row r="78" spans="1:6">
-      <c r="A78" s="2">
+      <c r="A78" s="1">
         <v>42250</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="5">
         <v>0.77500000000000002</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C78" s="2">
         <v>1</v>
       </c>
       <c r="D78">
@@ -2838,13 +2871,13 @@
       </c>
     </row>
     <row r="79" spans="1:6">
-      <c r="A79" s="2">
+      <c r="A79" s="1">
         <v>42250</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B79" s="5">
         <v>0.77500000000000002</v>
       </c>
-      <c r="C79" s="3">
+      <c r="C79" s="2">
         <v>1</v>
       </c>
       <c r="D79">
@@ -2858,13 +2891,13 @@
       </c>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="2">
+      <c r="A80" s="1">
         <v>42250</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B80" s="5">
         <v>0.79236111111111107</v>
       </c>
-      <c r="C80" s="3">
+      <c r="C80" s="2">
         <v>2</v>
       </c>
       <c r="D80">
@@ -2875,13 +2908,13 @@
       </c>
     </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="2">
+      <c r="A81" s="1">
         <v>42250</v>
       </c>
-      <c r="B81" s="6">
+      <c r="B81" s="5">
         <v>0.79861111111111116</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C81" s="2">
         <v>2</v>
       </c>
       <c r="D81">
@@ -2895,13 +2928,13 @@
       </c>
     </row>
     <row r="82" spans="1:6">
-      <c r="A82" s="2">
+      <c r="A82" s="1">
         <v>42250</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="5">
         <v>0.79861111111111116</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C82" s="2">
         <v>2</v>
       </c>
       <c r="D82">
@@ -2915,13 +2948,13 @@
       </c>
     </row>
     <row r="83" spans="1:6">
-      <c r="A83" s="2">
+      <c r="A83" s="1">
         <v>42250</v>
       </c>
-      <c r="B83" s="6">
+      <c r="B83" s="5">
         <v>0.79861111111111116</v>
       </c>
-      <c r="C83" s="3">
+      <c r="C83" s="2">
         <v>2</v>
       </c>
       <c r="D83">
@@ -2935,13 +2968,13 @@
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="2">
+      <c r="A84" s="1">
         <v>42250</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="5">
         <v>0.79861111111111116</v>
       </c>
-      <c r="C84" s="3">
+      <c r="C84" s="2">
         <v>2</v>
       </c>
       <c r="D84">
@@ -2955,13 +2988,13 @@
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="2">
+      <c r="A85" s="1">
         <v>42250</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85" s="5">
         <v>0.79861111111111116</v>
       </c>
-      <c r="C85" s="3">
+      <c r="C85" s="2">
         <v>2</v>
       </c>
       <c r="D85">
@@ -2975,13 +3008,13 @@
       </c>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="2">
+      <c r="A86" s="1">
         <v>42250</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="5">
         <v>0.79861111111111116</v>
       </c>
-      <c r="C86" s="3">
+      <c r="C86" s="2">
         <v>2</v>
       </c>
       <c r="D86">
@@ -2995,13 +3028,13 @@
       </c>
     </row>
     <row r="87" spans="1:6">
-      <c r="A87" s="2">
+      <c r="A87" s="1">
         <v>42250</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="5">
         <v>0.81666666666666676</v>
       </c>
-      <c r="C87" s="3">
+      <c r="C87" s="2">
         <v>3</v>
       </c>
       <c r="D87">
@@ -3012,13 +3045,13 @@
       </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="2">
+      <c r="A88" s="1">
         <v>42250</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B88" s="5">
         <v>0.85763888888888884</v>
       </c>
-      <c r="C88" s="3">
+      <c r="C88" s="2">
         <v>3</v>
       </c>
       <c r="D88">
@@ -3032,13 +3065,13 @@
       </c>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="2">
+      <c r="A89" s="1">
         <v>42250</v>
       </c>
-      <c r="B89" s="6">
+      <c r="B89" s="5">
         <v>0.85763888888888884</v>
       </c>
-      <c r="C89" s="3">
+      <c r="C89" s="2">
         <v>3</v>
       </c>
       <c r="D89">
@@ -3052,13 +3085,13 @@
       </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="2">
+      <c r="A90" s="1">
         <v>42250</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B90" s="5">
         <v>0.85763888888888884</v>
       </c>
-      <c r="C90" s="3">
+      <c r="C90" s="2">
         <v>3</v>
       </c>
       <c r="D90">
@@ -3072,13 +3105,13 @@
       </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="2">
+      <c r="A91" s="1">
         <v>42250</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B91" s="5">
         <v>0.85763888888888884</v>
       </c>
-      <c r="C91" s="3">
+      <c r="C91" s="2">
         <v>3</v>
       </c>
       <c r="D91">
@@ -3092,13 +3125,13 @@
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="2">
+      <c r="A92" s="1">
         <v>42250</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="5">
         <v>0.85763888888888884</v>
       </c>
-      <c r="C92" s="3">
+      <c r="C92" s="2">
         <v>3</v>
       </c>
       <c r="D92">
@@ -3112,13 +3145,13 @@
       </c>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="2">
+      <c r="A93" s="1">
         <v>42250</v>
       </c>
-      <c r="B93" s="6">
+      <c r="B93" s="5">
         <v>0.85763888888888884</v>
       </c>
-      <c r="C93" s="3">
+      <c r="C93" s="2">
         <v>3</v>
       </c>
       <c r="D93">
@@ -3132,13 +3165,13 @@
       </c>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="2">
+      <c r="A94" s="1">
         <v>42250</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B94" s="5">
         <v>0.87638888888888899</v>
       </c>
-      <c r="C94" s="3">
+      <c r="C94" s="2">
         <v>4</v>
       </c>
       <c r="D94">
@@ -3149,13 +3182,13 @@
       </c>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="2">
+      <c r="A95" s="1">
         <v>42250</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B95" s="5">
         <v>0.93263888888888891</v>
       </c>
-      <c r="C95" s="3">
+      <c r="C95" s="2">
         <v>4</v>
       </c>
       <c r="D95">
@@ -3169,13 +3202,13 @@
       </c>
     </row>
     <row r="96" spans="1:6">
-      <c r="A96" s="2">
+      <c r="A96" s="1">
         <v>42250</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B96" s="5">
         <v>0.93263888888888891</v>
       </c>
-      <c r="C96" s="3">
+      <c r="C96" s="2">
         <v>4</v>
       </c>
       <c r="D96">
@@ -3189,13 +3222,13 @@
       </c>
     </row>
     <row r="97" spans="1:6">
-      <c r="A97" s="2">
+      <c r="A97" s="1">
         <v>42250</v>
       </c>
-      <c r="B97" s="6">
+      <c r="B97" s="5">
         <v>0.93263888888888891</v>
       </c>
-      <c r="C97" s="3">
+      <c r="C97" s="2">
         <v>4</v>
       </c>
       <c r="D97">
@@ -3209,13 +3242,13 @@
       </c>
     </row>
     <row r="98" spans="1:6">
-      <c r="A98" s="2">
+      <c r="A98" s="1">
         <v>42250</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98" s="5">
         <v>0.93263888888888891</v>
       </c>
-      <c r="C98" s="3">
+      <c r="C98" s="2">
         <v>4</v>
       </c>
       <c r="D98">
@@ -3229,13 +3262,13 @@
       </c>
     </row>
     <row r="99" spans="1:6">
-      <c r="A99" s="2">
+      <c r="A99" s="1">
         <v>42250</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B99" s="5">
         <v>0.93263888888888891</v>
       </c>
-      <c r="C99" s="3">
+      <c r="C99" s="2">
         <v>4</v>
       </c>
       <c r="D99">
@@ -3249,13 +3282,13 @@
       </c>
     </row>
     <row r="100" spans="1:6">
-      <c r="A100" s="2">
+      <c r="A100" s="1">
         <v>42250</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100" s="5">
         <v>0.93263888888888891</v>
       </c>
-      <c r="C100" s="3">
+      <c r="C100" s="2">
         <v>4</v>
       </c>
       <c r="D100">
@@ -3269,13 +3302,13 @@
       </c>
     </row>
     <row r="101" spans="1:6">
-      <c r="A101" s="2">
+      <c r="A101" s="1">
         <v>42250</v>
       </c>
-      <c r="B101" s="6">
+      <c r="B101" s="5">
         <v>0.95000000000000007</v>
       </c>
-      <c r="C101" s="3">
+      <c r="C101" s="2">
         <v>5</v>
       </c>
       <c r="D101">
@@ -3286,13 +3319,13 @@
       </c>
     </row>
     <row r="102" spans="1:6">
-      <c r="A102" s="2">
+      <c r="A102" s="1">
         <v>42250</v>
       </c>
-      <c r="B102" s="6">
+      <c r="B102" s="5">
         <v>0.95763888888888893</v>
       </c>
-      <c r="C102" s="3">
+      <c r="C102" s="2">
         <v>5</v>
       </c>
       <c r="D102">
@@ -3306,13 +3339,13 @@
       </c>
     </row>
     <row r="103" spans="1:6">
-      <c r="A103" s="2">
+      <c r="A103" s="1">
         <v>42250</v>
       </c>
-      <c r="B103" s="6">
+      <c r="B103" s="5">
         <v>0.95763888888888893</v>
       </c>
-      <c r="C103" s="3">
+      <c r="C103" s="2">
         <v>5</v>
       </c>
       <c r="D103">
@@ -3326,13 +3359,13 @@
       </c>
     </row>
     <row r="104" spans="1:6">
-      <c r="A104" s="2">
+      <c r="A104" s="1">
         <v>42250</v>
       </c>
-      <c r="B104" s="6">
+      <c r="B104" s="5">
         <v>0.95763888888888893</v>
       </c>
-      <c r="C104" s="3">
+      <c r="C104" s="2">
         <v>5</v>
       </c>
       <c r="D104">
@@ -3346,13 +3379,13 @@
       </c>
     </row>
     <row r="105" spans="1:6">
-      <c r="A105" s="2">
+      <c r="A105" s="1">
         <v>42250</v>
       </c>
-      <c r="B105" s="6">
+      <c r="B105" s="5">
         <v>0.95763888888888893</v>
       </c>
-      <c r="C105" s="3">
+      <c r="C105" s="2">
         <v>5</v>
       </c>
       <c r="D105">
@@ -3366,13 +3399,13 @@
       </c>
     </row>
     <row r="106" spans="1:6">
-      <c r="A106" s="2">
+      <c r="A106" s="1">
         <v>42250</v>
       </c>
-      <c r="B106" s="6">
+      <c r="B106" s="5">
         <v>0.95763888888888893</v>
       </c>
-      <c r="C106" s="3">
+      <c r="C106" s="2">
         <v>5</v>
       </c>
       <c r="D106">
@@ -3386,13 +3419,13 @@
       </c>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="2">
+      <c r="A107" s="1">
         <v>42250</v>
       </c>
-      <c r="B107" s="6">
+      <c r="B107" s="5">
         <v>0.95763888888888893</v>
       </c>
-      <c r="C107" s="3">
+      <c r="C107" s="2">
         <v>5</v>
       </c>
       <c r="D107">
@@ -3406,13 +3439,13 @@
       </c>
     </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="2">
+      <c r="A108" s="1">
         <v>42251</v>
       </c>
-      <c r="B108" s="6">
+      <c r="B108" s="5">
         <v>0.71527777777777779</v>
       </c>
-      <c r="C108" s="3">
+      <c r="C108" s="2">
         <v>1</v>
       </c>
       <c r="D108">
@@ -3423,13 +3456,13 @@
       </c>
     </row>
     <row r="109" spans="1:6">
-      <c r="A109" s="2">
+      <c r="A109" s="1">
         <v>42251</v>
       </c>
-      <c r="B109" s="6">
+      <c r="B109" s="5">
         <v>0.73819444444444438</v>
       </c>
-      <c r="C109" s="3">
+      <c r="C109" s="2">
         <v>1</v>
       </c>
       <c r="D109">
@@ -3443,13 +3476,13 @@
       </c>
     </row>
     <row r="110" spans="1:6">
-      <c r="A110" s="2">
+      <c r="A110" s="1">
         <v>42251</v>
       </c>
-      <c r="B110" s="6">
+      <c r="B110" s="5">
         <v>0.73819444444444438</v>
       </c>
-      <c r="C110" s="3">
+      <c r="C110" s="2">
         <v>1</v>
       </c>
       <c r="D110">
@@ -3463,13 +3496,13 @@
       </c>
     </row>
     <row r="111" spans="1:6">
-      <c r="A111" s="2">
+      <c r="A111" s="1">
         <v>42251</v>
       </c>
-      <c r="B111" s="6">
+      <c r="B111" s="5">
         <v>0.73819444444444438</v>
       </c>
-      <c r="C111" s="3">
+      <c r="C111" s="2">
         <v>1</v>
       </c>
       <c r="D111">
@@ -3483,13 +3516,13 @@
       </c>
     </row>
     <row r="112" spans="1:6">
-      <c r="A112" s="2">
+      <c r="A112" s="1">
         <v>42251</v>
       </c>
-      <c r="B112" s="6">
+      <c r="B112" s="5">
         <v>0.73819444444444438</v>
       </c>
-      <c r="C112" s="3">
+      <c r="C112" s="2">
         <v>1</v>
       </c>
       <c r="D112">
@@ -3503,13 +3536,13 @@
       </c>
     </row>
     <row r="113" spans="1:6">
-      <c r="A113" s="2">
+      <c r="A113" s="1">
         <v>42251</v>
       </c>
-      <c r="B113" s="6">
+      <c r="B113" s="5">
         <v>0.73819444444444438</v>
       </c>
-      <c r="C113" s="3">
+      <c r="C113" s="2">
         <v>1</v>
       </c>
       <c r="D113">
@@ -3523,13 +3556,13 @@
       </c>
     </row>
     <row r="114" spans="1:6">
-      <c r="A114" s="2">
+      <c r="A114" s="1">
         <v>42251</v>
       </c>
-      <c r="B114" s="6">
+      <c r="B114" s="5">
         <v>0.73819444444444438</v>
       </c>
-      <c r="C114" s="3">
+      <c r="C114" s="2">
         <v>1</v>
       </c>
       <c r="D114">
@@ -3543,13 +3576,13 @@
       </c>
     </row>
     <row r="115" spans="1:6">
-      <c r="A115" s="2">
+      <c r="A115" s="1">
         <v>42251</v>
       </c>
-      <c r="B115" s="6">
+      <c r="B115" s="5">
         <v>0.75624999999999998</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C115" s="2">
         <v>2</v>
       </c>
       <c r="D115">
@@ -3560,13 +3593,13 @@
       </c>
     </row>
     <row r="116" spans="1:6">
-      <c r="A116" s="2">
+      <c r="A116" s="1">
         <v>42251</v>
       </c>
-      <c r="B116" s="6">
+      <c r="B116" s="5">
         <v>0.76180555555555562</v>
       </c>
-      <c r="C116" s="3">
+      <c r="C116" s="2">
         <v>2</v>
       </c>
       <c r="D116">
@@ -3580,13 +3613,13 @@
       </c>
     </row>
     <row r="117" spans="1:6">
-      <c r="A117" s="2">
+      <c r="A117" s="1">
         <v>42251</v>
       </c>
-      <c r="B117" s="6">
+      <c r="B117" s="5">
         <v>0.76180555555555562</v>
       </c>
-      <c r="C117" s="3">
+      <c r="C117" s="2">
         <v>2</v>
       </c>
       <c r="D117">
@@ -3600,13 +3633,13 @@
       </c>
     </row>
     <row r="118" spans="1:6">
-      <c r="A118" s="2">
+      <c r="A118" s="1">
         <v>42251</v>
       </c>
-      <c r="B118" s="6">
+      <c r="B118" s="5">
         <v>0.76180555555555562</v>
       </c>
-      <c r="C118" s="3">
+      <c r="C118" s="2">
         <v>2</v>
       </c>
       <c r="D118">
@@ -3620,13 +3653,13 @@
       </c>
     </row>
     <row r="119" spans="1:6">
-      <c r="A119" s="2">
+      <c r="A119" s="1">
         <v>42251</v>
       </c>
-      <c r="B119" s="6">
+      <c r="B119" s="5">
         <v>0.76180555555555562</v>
       </c>
-      <c r="C119" s="3">
+      <c r="C119" s="2">
         <v>2</v>
       </c>
       <c r="D119">
@@ -3640,13 +3673,13 @@
       </c>
     </row>
     <row r="120" spans="1:6">
-      <c r="A120" s="2">
+      <c r="A120" s="1">
         <v>42251</v>
       </c>
-      <c r="B120" s="6">
+      <c r="B120" s="5">
         <v>0.76180555555555562</v>
       </c>
-      <c r="C120" s="3">
+      <c r="C120" s="2">
         <v>2</v>
       </c>
       <c r="D120">
@@ -3660,13 +3693,13 @@
       </c>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="2">
+      <c r="A121" s="1">
         <v>42251</v>
       </c>
-      <c r="B121" s="6">
+      <c r="B121" s="5">
         <v>0.76180555555555562</v>
       </c>
-      <c r="C121" s="3">
+      <c r="C121" s="2">
         <v>2</v>
       </c>
       <c r="D121">
@@ -3680,13 +3713,13 @@
       </c>
     </row>
     <row r="122" spans="1:6">
-      <c r="A122" s="2">
+      <c r="A122" s="1">
         <v>42251</v>
       </c>
-      <c r="B122" s="6">
+      <c r="B122" s="5">
         <v>0.77847222222222223</v>
       </c>
-      <c r="C122" s="3">
+      <c r="C122" s="2">
         <v>3</v>
       </c>
       <c r="D122">
@@ -3697,13 +3730,13 @@
       </c>
     </row>
     <row r="123" spans="1:6">
-      <c r="A123" s="2">
+      <c r="A123" s="1">
         <v>42251</v>
       </c>
-      <c r="B123" s="6">
+      <c r="B123" s="5">
         <v>0.81508101851851855</v>
       </c>
-      <c r="C123" s="3">
+      <c r="C123" s="2">
         <v>3</v>
       </c>
       <c r="D123">
@@ -3717,13 +3750,13 @@
       </c>
     </row>
     <row r="124" spans="1:6">
-      <c r="A124" s="2">
+      <c r="A124" s="1">
         <v>42251</v>
       </c>
-      <c r="B124" s="6">
+      <c r="B124" s="5">
         <v>0.81508101851851855</v>
       </c>
-      <c r="C124" s="3">
+      <c r="C124" s="2">
         <v>3</v>
       </c>
       <c r="D124">
@@ -3737,13 +3770,13 @@
       </c>
     </row>
     <row r="125" spans="1:6">
-      <c r="A125" s="2">
+      <c r="A125" s="1">
         <v>42251</v>
       </c>
-      <c r="B125" s="6">
+      <c r="B125" s="5">
         <v>0.81508101851851855</v>
       </c>
-      <c r="C125" s="3">
+      <c r="C125" s="2">
         <v>3</v>
       </c>
       <c r="D125">
@@ -3757,13 +3790,13 @@
       </c>
     </row>
     <row r="126" spans="1:6">
-      <c r="A126" s="2">
+      <c r="A126" s="1">
         <v>42251</v>
       </c>
-      <c r="B126" s="6">
+      <c r="B126" s="5">
         <v>0.81508101851851855</v>
       </c>
-      <c r="C126" s="3">
+      <c r="C126" s="2">
         <v>3</v>
       </c>
       <c r="D126">
@@ -3777,13 +3810,13 @@
       </c>
     </row>
     <row r="127" spans="1:6">
-      <c r="A127" s="2">
+      <c r="A127" s="1">
         <v>42251</v>
       </c>
-      <c r="B127" s="6">
+      <c r="B127" s="5">
         <v>0.81508101851851855</v>
       </c>
-      <c r="C127" s="3">
+      <c r="C127" s="2">
         <v>3</v>
       </c>
       <c r="D127">
@@ -3797,13 +3830,13 @@
       </c>
     </row>
     <row r="128" spans="1:6">
-      <c r="A128" s="2">
+      <c r="A128" s="1">
         <v>42251</v>
       </c>
-      <c r="B128" s="6">
+      <c r="B128" s="5">
         <v>0.81508101851851855</v>
       </c>
-      <c r="C128" s="3">
+      <c r="C128" s="2">
         <v>3</v>
       </c>
       <c r="D128">
@@ -3817,13 +3850,13 @@
       </c>
     </row>
     <row r="129" spans="1:6">
-      <c r="A129" s="2">
+      <c r="A129" s="1">
         <v>42251</v>
       </c>
-      <c r="B129" s="6">
+      <c r="B129" s="5">
         <v>0.83225694444444442</v>
       </c>
-      <c r="C129" s="3">
+      <c r="C129" s="2">
         <v>4</v>
       </c>
       <c r="D129">
@@ -3834,13 +3867,13 @@
       </c>
     </row>
     <row r="130" spans="1:6">
-      <c r="A130" s="2">
+      <c r="A130" s="1">
         <v>42251</v>
       </c>
-      <c r="B130" s="6">
+      <c r="B130" s="5">
         <v>0.8386689814814815</v>
       </c>
-      <c r="C130" s="3">
+      <c r="C130" s="2">
         <v>4</v>
       </c>
       <c r="D130">
@@ -3854,13 +3887,13 @@
       </c>
     </row>
     <row r="131" spans="1:6">
-      <c r="A131" s="2">
+      <c r="A131" s="1">
         <v>42251</v>
       </c>
-      <c r="B131" s="6">
+      <c r="B131" s="5">
         <v>0.8386689814814815</v>
       </c>
-      <c r="C131" s="3">
+      <c r="C131" s="2">
         <v>4</v>
       </c>
       <c r="D131">
@@ -3874,13 +3907,13 @@
       </c>
     </row>
     <row r="132" spans="1:6">
-      <c r="A132" s="2">
+      <c r="A132" s="1">
         <v>42251</v>
       </c>
-      <c r="B132" s="6">
+      <c r="B132" s="5">
         <v>0.8386689814814815</v>
       </c>
-      <c r="C132" s="3">
+      <c r="C132" s="2">
         <v>4</v>
       </c>
       <c r="D132">
@@ -3894,13 +3927,13 @@
       </c>
     </row>
     <row r="133" spans="1:6">
-      <c r="A133" s="2">
+      <c r="A133" s="1">
         <v>42251</v>
       </c>
-      <c r="B133" s="6">
+      <c r="B133" s="5">
         <v>0.8386689814814815</v>
       </c>
-      <c r="C133" s="3">
+      <c r="C133" s="2">
         <v>4</v>
       </c>
       <c r="D133">
@@ -3914,13 +3947,13 @@
       </c>
     </row>
     <row r="134" spans="1:6">
-      <c r="A134" s="2">
+      <c r="A134" s="1">
         <v>42251</v>
       </c>
-      <c r="B134" s="6">
+      <c r="B134" s="5">
         <v>0.8386689814814815</v>
       </c>
-      <c r="C134" s="3">
+      <c r="C134" s="2">
         <v>4</v>
       </c>
       <c r="D134">
@@ -3934,13 +3967,13 @@
       </c>
     </row>
     <row r="135" spans="1:6">
-      <c r="A135" s="2">
+      <c r="A135" s="1">
         <v>42251</v>
       </c>
-      <c r="B135" s="6">
+      <c r="B135" s="5">
         <v>0.8386689814814815</v>
       </c>
-      <c r="C135" s="3">
+      <c r="C135" s="2">
         <v>4</v>
       </c>
       <c r="D135">
@@ -3954,13 +3987,13 @@
       </c>
     </row>
     <row r="136" spans="1:6">
-      <c r="A136" s="2">
+      <c r="A136" s="1">
         <v>42251</v>
       </c>
-      <c r="B136" s="6">
+      <c r="B136" s="5">
         <v>0.85541666666666671</v>
       </c>
-      <c r="C136" s="3">
+      <c r="C136" s="2">
         <v>5</v>
       </c>
       <c r="D136">
@@ -3971,13 +4004,13 @@
       </c>
     </row>
     <row r="137" spans="1:6">
-      <c r="A137" s="2">
+      <c r="A137" s="1">
         <v>42251</v>
       </c>
-      <c r="B137" s="6">
+      <c r="B137" s="5">
         <v>0.88888888888888884</v>
       </c>
-      <c r="C137" s="3">
+      <c r="C137" s="2">
         <v>5</v>
       </c>
       <c r="D137">
@@ -3991,13 +4024,13 @@
       </c>
     </row>
     <row r="138" spans="1:6">
-      <c r="A138" s="2">
+      <c r="A138" s="1">
         <v>42251</v>
       </c>
-      <c r="B138" s="6">
+      <c r="B138" s="5">
         <v>0.88888888888888884</v>
       </c>
-      <c r="C138" s="3">
+      <c r="C138" s="2">
         <v>5</v>
       </c>
       <c r="D138">
@@ -4011,13 +4044,13 @@
       </c>
     </row>
     <row r="139" spans="1:6">
-      <c r="A139" s="2">
+      <c r="A139" s="1">
         <v>42251</v>
       </c>
-      <c r="B139" s="6">
+      <c r="B139" s="5">
         <v>0.88888888888888884</v>
       </c>
-      <c r="C139" s="3">
+      <c r="C139" s="2">
         <v>5</v>
       </c>
       <c r="D139">
@@ -4031,13 +4064,13 @@
       </c>
     </row>
     <row r="140" spans="1:6">
-      <c r="A140" s="2">
+      <c r="A140" s="1">
         <v>42251</v>
       </c>
-      <c r="B140" s="6">
+      <c r="B140" s="5">
         <v>0.88888888888888884</v>
       </c>
-      <c r="C140" s="3">
+      <c r="C140" s="2">
         <v>5</v>
       </c>
       <c r="D140">
@@ -4051,13 +4084,13 @@
       </c>
     </row>
     <row r="141" spans="1:6">
-      <c r="A141" s="2">
+      <c r="A141" s="1">
         <v>42251</v>
       </c>
-      <c r="B141" s="6">
+      <c r="B141" s="5">
         <v>0.88888888888888884</v>
       </c>
-      <c r="C141" s="3">
+      <c r="C141" s="2">
         <v>5</v>
       </c>
       <c r="D141">
@@ -4071,13 +4104,13 @@
       </c>
     </row>
     <row r="142" spans="1:6">
-      <c r="A142" s="2">
+      <c r="A142" s="1">
         <v>42251</v>
       </c>
-      <c r="B142" s="6">
+      <c r="B142" s="5">
         <v>0.88888888888888884</v>
       </c>
-      <c r="C142" s="3">
+      <c r="C142" s="2">
         <v>5</v>
       </c>
       <c r="D142">
@@ -4088,6 +4121,1209 @@
       </c>
       <c r="F142">
         <v>1185.5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B143" s="5">
+        <v>0.70624999999999993</v>
+      </c>
+      <c r="D143">
+        <v>10</v>
+      </c>
+      <c r="E143" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B144" s="5">
+        <v>0.74513888888888891</v>
+      </c>
+      <c r="D144">
+        <v>6</v>
+      </c>
+      <c r="E144" t="s">
+        <v>18</v>
+      </c>
+      <c r="F144">
+        <v>1619.1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B145" s="5">
+        <v>0.74513888888888891</v>
+      </c>
+      <c r="D145">
+        <v>16</v>
+      </c>
+      <c r="E145" t="s">
+        <v>19</v>
+      </c>
+      <c r="F145">
+        <v>2016.8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B146" s="5">
+        <v>0.74513888888888891</v>
+      </c>
+      <c r="D146">
+        <v>13</v>
+      </c>
+      <c r="E146" t="s">
+        <v>20</v>
+      </c>
+      <c r="F146">
+        <v>2207.6999999999998</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B147" s="5">
+        <v>0.74513888888888891</v>
+      </c>
+      <c r="D147">
+        <v>14</v>
+      </c>
+      <c r="E147" t="s">
+        <v>21</v>
+      </c>
+      <c r="F147">
+        <v>1491.8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B148" s="5">
+        <v>0.74513888888888891</v>
+      </c>
+      <c r="D148">
+        <v>11</v>
+      </c>
+      <c r="E148" t="s">
+        <v>22</v>
+      </c>
+      <c r="F148">
+        <v>2243.6999999999998</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B149" s="5">
+        <v>0.74513888888888891</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149" t="s">
+        <v>23</v>
+      </c>
+      <c r="F149">
+        <v>1720.4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B150" s="5">
+        <v>0.76180555555555562</v>
+      </c>
+      <c r="D150">
+        <v>10</v>
+      </c>
+      <c r="E150" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B151" s="5">
+        <v>0.76874999999999993</v>
+      </c>
+      <c r="D151">
+        <v>4</v>
+      </c>
+      <c r="E151" t="s">
+        <v>9</v>
+      </c>
+      <c r="F151">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B152" s="5">
+        <v>0.76874999999999993</v>
+      </c>
+      <c r="D152">
+        <v>2</v>
+      </c>
+      <c r="E152" t="s">
+        <v>11</v>
+      </c>
+      <c r="F152">
+        <v>1758.3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B153" s="5">
+        <v>0.76874999999999993</v>
+      </c>
+      <c r="D153">
+        <v>12</v>
+      </c>
+      <c r="E153" t="s">
+        <v>13</v>
+      </c>
+      <c r="F153">
+        <v>1726.9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B154" s="5">
+        <v>0.76874999999999993</v>
+      </c>
+      <c r="D154">
+        <v>8</v>
+      </c>
+      <c r="E154" t="s">
+        <v>15</v>
+      </c>
+      <c r="F154">
+        <v>2176.9</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B155" s="5">
+        <v>0.76874999999999993</v>
+      </c>
+      <c r="D155">
+        <v>5</v>
+      </c>
+      <c r="E155" t="s">
+        <v>16</v>
+      </c>
+      <c r="F155">
+        <v>1723.3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B156" s="5">
+        <v>0.76874999999999993</v>
+      </c>
+      <c r="D156">
+        <v>9</v>
+      </c>
+      <c r="E156" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B157" s="5">
+        <v>0.78541666666666676</v>
+      </c>
+      <c r="D157">
+        <v>10</v>
+      </c>
+      <c r="E157" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B158" s="5">
+        <v>0.81666666666666676</v>
+      </c>
+      <c r="D158">
+        <v>6</v>
+      </c>
+      <c r="E158" t="s">
+        <v>1</v>
+      </c>
+      <c r="F158">
+        <v>1969.6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B159" s="5">
+        <v>0.81666666666666676</v>
+      </c>
+      <c r="D159">
+        <v>16</v>
+      </c>
+      <c r="E159" t="s">
+        <v>2</v>
+      </c>
+      <c r="F159">
+        <v>2179.5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B160" s="5">
+        <v>0.81666666666666676</v>
+      </c>
+      <c r="D160">
+        <v>13</v>
+      </c>
+      <c r="E160" t="s">
+        <v>3</v>
+      </c>
+      <c r="F160">
+        <v>1443.1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B161" s="5">
+        <v>0.81666666666666676</v>
+      </c>
+      <c r="D161">
+        <v>14</v>
+      </c>
+      <c r="E161" t="s">
+        <v>4</v>
+      </c>
+      <c r="F161">
+        <v>1849.4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B162" s="5">
+        <v>0.81666666666666676</v>
+      </c>
+      <c r="D162">
+        <v>11</v>
+      </c>
+      <c r="E162" t="s">
+        <v>6</v>
+      </c>
+      <c r="F162">
+        <v>1857.3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B163" s="5">
+        <v>0.81666666666666676</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+      <c r="E163" t="s">
+        <v>7</v>
+      </c>
+      <c r="F163">
+        <v>2025.1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B164" s="5">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D164">
+        <v>10</v>
+      </c>
+      <c r="E164" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B165" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="D165">
+        <v>4</v>
+      </c>
+      <c r="E165" t="s">
+        <v>25</v>
+      </c>
+      <c r="F165">
+        <v>2111.6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B166" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="D166">
+        <v>2</v>
+      </c>
+      <c r="E166" t="s">
+        <v>26</v>
+      </c>
+      <c r="F166">
+        <v>2006.8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="A167" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B167" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="D167">
+        <v>12</v>
+      </c>
+      <c r="E167" t="s">
+        <v>27</v>
+      </c>
+      <c r="F167">
+        <v>1972.4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B168" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="D168">
+        <v>8</v>
+      </c>
+      <c r="E168" t="s">
+        <v>28</v>
+      </c>
+      <c r="F168">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B169" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="D169">
+        <v>5</v>
+      </c>
+      <c r="E169" t="s">
+        <v>29</v>
+      </c>
+      <c r="F169">
+        <v>2160.6999999999998</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="A170" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B170" s="5">
+        <v>0.875</v>
+      </c>
+      <c r="D170">
+        <v>9</v>
+      </c>
+      <c r="E170" t="s">
+        <v>30</v>
+      </c>
+      <c r="F170">
+        <v>1642.7</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B171" s="5">
+        <v>0.89166666666666661</v>
+      </c>
+      <c r="D171">
+        <v>10</v>
+      </c>
+      <c r="E171" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B172" s="5">
+        <v>0.89861111111111114</v>
+      </c>
+      <c r="D172">
+        <v>6</v>
+      </c>
+      <c r="E172" t="s">
+        <v>5</v>
+      </c>
+      <c r="F172">
+        <v>1620.3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="A173" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B173" s="5">
+        <v>0.89861111111111114</v>
+      </c>
+      <c r="D173">
+        <v>16</v>
+      </c>
+      <c r="E173" t="s">
+        <v>24</v>
+      </c>
+      <c r="F173">
+        <v>1908.1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B174" s="5">
+        <v>0.89861111111111114</v>
+      </c>
+      <c r="D174">
+        <v>13</v>
+      </c>
+      <c r="E174" t="s">
+        <v>8</v>
+      </c>
+      <c r="F174">
+        <v>1294.4000000000001</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B175" s="5">
+        <v>0.89861111111111114</v>
+      </c>
+      <c r="D175">
+        <v>14</v>
+      </c>
+      <c r="E175" t="s">
+        <v>10</v>
+      </c>
+      <c r="F175">
+        <v>2048.1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B176" s="5">
+        <v>0.89861111111111114</v>
+      </c>
+      <c r="D176">
+        <v>11</v>
+      </c>
+      <c r="E176" t="s">
+        <v>12</v>
+      </c>
+      <c r="F176">
+        <v>1738.8</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B177" s="5">
+        <v>0.89861111111111114</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="E177" t="s">
+        <v>14</v>
+      </c>
+      <c r="F177">
+        <v>2025.2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
+      <c r="A178" s="1">
+        <v>42255</v>
+      </c>
+      <c r="B178" s="5">
+        <v>0.91527777777777775</v>
+      </c>
+      <c r="D178">
+        <v>10</v>
+      </c>
+      <c r="E178" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
+      <c r="A179" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B179" s="5">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="D179">
+        <v>10</v>
+      </c>
+      <c r="E179" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
+      <c r="A180" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B180" s="5">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="D180">
+        <v>6</v>
+      </c>
+      <c r="E180" t="s">
+        <v>1</v>
+      </c>
+      <c r="F180">
+        <v>1969.8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
+      <c r="A181" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B181" s="5">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="D181">
+        <v>16</v>
+      </c>
+      <c r="E181" t="s">
+        <v>2</v>
+      </c>
+      <c r="F181">
+        <v>2179.4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
+      <c r="A182" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B182" s="5">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="D182">
+        <v>13</v>
+      </c>
+      <c r="E182" t="s">
+        <v>3</v>
+      </c>
+      <c r="F182">
+        <v>1445.3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
+      <c r="A183" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B183" s="5">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="D183">
+        <v>14</v>
+      </c>
+      <c r="E183" t="s">
+        <v>4</v>
+      </c>
+      <c r="F183">
+        <v>1850.7</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
+      <c r="A184" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B184" s="5">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="D184">
+        <v>11</v>
+      </c>
+      <c r="E184" t="s">
+        <v>6</v>
+      </c>
+      <c r="F184">
+        <v>1860.9</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6">
+      <c r="A185" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B185" s="5">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+      <c r="E185" t="s">
+        <v>7</v>
+      </c>
+      <c r="F185">
+        <v>2026.3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
+      <c r="A186" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B186" s="5">
+        <v>0.71736111111111101</v>
+      </c>
+      <c r="D186">
+        <v>10</v>
+      </c>
+      <c r="E186" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6">
+      <c r="A187" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B187" s="5">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="D187">
+        <v>4</v>
+      </c>
+      <c r="E187" t="s">
+        <v>9</v>
+      </c>
+      <c r="F187">
+        <v>1943.7</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6">
+      <c r="A188" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B188" s="5">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="D188">
+        <v>2</v>
+      </c>
+      <c r="E188" t="s">
+        <v>11</v>
+      </c>
+      <c r="F188">
+        <v>1734.7</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6">
+      <c r="A189" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B189" s="5">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="D189">
+        <v>12</v>
+      </c>
+      <c r="E189" t="s">
+        <v>13</v>
+      </c>
+      <c r="F189">
+        <v>1713.3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6">
+      <c r="A190" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B190" s="5">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="D190">
+        <v>8</v>
+      </c>
+      <c r="E190" t="s">
+        <v>15</v>
+      </c>
+      <c r="F190">
+        <v>2162.4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
+      <c r="A191" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B191" s="5">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="D191">
+        <v>5</v>
+      </c>
+      <c r="E191" t="s">
+        <v>16</v>
+      </c>
+      <c r="F191">
+        <v>1676.9</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6">
+      <c r="A192" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B192" s="5">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="D192">
+        <v>9</v>
+      </c>
+      <c r="E192" t="s">
+        <v>17</v>
+      </c>
+      <c r="F192">
+        <v>1713.6</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7">
+      <c r="A193" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B193" s="5">
+        <v>0.74097222222222225</v>
+      </c>
+      <c r="D193">
+        <v>10</v>
+      </c>
+      <c r="E193" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7">
+      <c r="A194" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B194" s="5">
+        <v>0.78402777777777777</v>
+      </c>
+      <c r="D194">
+        <v>6</v>
+      </c>
+      <c r="E194" t="s">
+        <v>18</v>
+      </c>
+      <c r="F194">
+        <v>1609.6</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7">
+      <c r="A195" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B195" s="5">
+        <v>0.78402777777777777</v>
+      </c>
+      <c r="D195">
+        <v>16</v>
+      </c>
+      <c r="E195" t="s">
+        <v>19</v>
+      </c>
+      <c r="F195">
+        <v>2004.9</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7">
+      <c r="A196" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B196" s="5">
+        <v>0.78402777777777777</v>
+      </c>
+      <c r="D196">
+        <v>13</v>
+      </c>
+      <c r="E196" t="s">
+        <v>20</v>
+      </c>
+      <c r="F196">
+        <v>2198</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7">
+      <c r="A197" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B197" s="5">
+        <v>0.78402777777777777</v>
+      </c>
+      <c r="D197">
+        <v>14</v>
+      </c>
+      <c r="E197" t="s">
+        <v>21</v>
+      </c>
+      <c r="F197">
+        <v>1480.2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7">
+      <c r="A198" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B198" s="5">
+        <v>0.78402777777777777</v>
+      </c>
+      <c r="D198">
+        <v>11</v>
+      </c>
+      <c r="E198" t="s">
+        <v>22</v>
+      </c>
+      <c r="F198">
+        <v>2230.1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7">
+      <c r="A199" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B199" s="5">
+        <v>0.78402777777777777</v>
+      </c>
+      <c r="D199">
+        <v>1</v>
+      </c>
+      <c r="E199" t="s">
+        <v>23</v>
+      </c>
+      <c r="F199">
+        <v>1709.2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7">
+      <c r="A200" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B200" s="5">
+        <v>0.80069444444444438</v>
+      </c>
+      <c r="D200">
+        <v>10</v>
+      </c>
+      <c r="E200" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7">
+      <c r="A201" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B201" s="5">
+        <v>0.8256944444444444</v>
+      </c>
+      <c r="D201">
+        <v>4</v>
+      </c>
+      <c r="E201" t="s">
+        <v>25</v>
+      </c>
+      <c r="F201">
+        <v>2103.5</v>
+      </c>
+      <c r="G201" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7">
+      <c r="A202" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B202" s="5">
+        <v>0.8256944444444444</v>
+      </c>
+      <c r="D202">
+        <v>2</v>
+      </c>
+      <c r="E202" t="s">
+        <v>26</v>
+      </c>
+      <c r="F202">
+        <v>1999.2</v>
+      </c>
+      <c r="G202" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7">
+      <c r="A203" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B203" s="5">
+        <v>0.8256944444444444</v>
+      </c>
+      <c r="D203">
+        <v>12</v>
+      </c>
+      <c r="E203" t="s">
+        <v>27</v>
+      </c>
+      <c r="F203">
+        <v>1967.3</v>
+      </c>
+      <c r="G203" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7">
+      <c r="A204" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B204" s="5">
+        <v>0.8256944444444444</v>
+      </c>
+      <c r="D204">
+        <v>8</v>
+      </c>
+      <c r="E204" t="s">
+        <v>28</v>
+      </c>
+      <c r="F204">
+        <v>2034.7</v>
+      </c>
+      <c r="G204" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7">
+      <c r="A205" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B205" s="5">
+        <v>0.8256944444444444</v>
+      </c>
+      <c r="D205">
+        <v>5</v>
+      </c>
+      <c r="E205" t="s">
+        <v>29</v>
+      </c>
+      <c r="F205">
+        <v>2158.3000000000002</v>
+      </c>
+      <c r="G205" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7">
+      <c r="A206" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B206" s="5">
+        <v>0.8256944444444444</v>
+      </c>
+      <c r="D206">
+        <v>9</v>
+      </c>
+      <c r="E206" t="s">
+        <v>30</v>
+      </c>
+      <c r="F206">
+        <v>1659.2</v>
+      </c>
+      <c r="G206" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7">
+      <c r="A207" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B207" s="5">
+        <v>0.84236111111111101</v>
+      </c>
+      <c r="D207">
+        <v>10</v>
+      </c>
+      <c r="E207" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7">
+      <c r="A208" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B208" s="5">
+        <v>0.84930555555555554</v>
+      </c>
+      <c r="D208">
+        <v>6</v>
+      </c>
+      <c r="E208" t="s">
+        <v>5</v>
+      </c>
+      <c r="F208">
+        <v>1624.6</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6">
+      <c r="A209" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B209" s="5">
+        <v>0.84930555555555554</v>
+      </c>
+      <c r="D209">
+        <v>16</v>
+      </c>
+      <c r="E209" t="s">
+        <v>24</v>
+      </c>
+      <c r="F209">
+        <v>1910.3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6">
+      <c r="A210" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B210" s="5">
+        <v>0.84930555555555554</v>
+      </c>
+      <c r="D210">
+        <v>13</v>
+      </c>
+      <c r="E210" t="s">
+        <v>8</v>
+      </c>
+      <c r="F210">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6">
+      <c r="A211" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B211" s="5">
+        <v>0.84930555555555554</v>
+      </c>
+      <c r="D211">
+        <v>14</v>
+      </c>
+      <c r="E211" t="s">
+        <v>10</v>
+      </c>
+      <c r="F211">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6">
+      <c r="A212" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B212" s="5">
+        <v>0.84930555555555554</v>
+      </c>
+      <c r="D212">
+        <v>11</v>
+      </c>
+      <c r="E212" t="s">
+        <v>12</v>
+      </c>
+      <c r="F212">
+        <v>1745.1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6">
+      <c r="A213" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B213" s="5">
+        <v>0.84930555555555554</v>
+      </c>
+      <c r="D213">
+        <v>1</v>
+      </c>
+      <c r="E213" t="s">
+        <v>14</v>
+      </c>
+      <c r="F213">
+        <v>2034.2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6">
+      <c r="A214" s="1">
+        <v>42258</v>
+      </c>
+      <c r="B214" s="5">
+        <v>0.86597222222222225</v>
+      </c>
+      <c r="D214">
+        <v>10</v>
+      </c>
+      <c r="E214" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
15 September data update
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24520" windowHeight="15360" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24400" windowHeight="15360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="treatments.csv" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="50">
   <si>
     <t>Treatment</t>
   </si>
@@ -240,8 +240,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="157">
+  <cellStyleXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -407,7 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="157">
+  <cellStyles count="161">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -486,6 +490,8 @@
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -564,6 +570,8 @@
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -866,8 +874,8 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1346,11 +1354,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G214"/>
+  <dimension ref="A1:G284"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F143" sqref="F143:F178"/>
+      <pane ySplit="2" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E243" sqref="E243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5333,6 +5341,692 @@
         <v>46</v>
       </c>
     </row>
+    <row r="215" spans="1:6">
+      <c r="A215" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B215" s="5">
+        <v>0.7090277777777777</v>
+      </c>
+      <c r="D215">
+        <v>10</v>
+      </c>
+      <c r="E215" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6">
+      <c r="A216" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B216" s="5">
+        <v>0.70972222222222225</v>
+      </c>
+      <c r="D216">
+        <v>6</v>
+      </c>
+      <c r="E216" t="s">
+        <v>18</v>
+      </c>
+      <c r="F216">
+        <v>1594.2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6">
+      <c r="A217" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B217" s="5">
+        <v>0.70972222222222225</v>
+      </c>
+      <c r="D217">
+        <v>16</v>
+      </c>
+      <c r="E217" t="s">
+        <v>19</v>
+      </c>
+      <c r="F217">
+        <v>1989.3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6">
+      <c r="A218" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B218" s="5">
+        <v>0.70972222222222225</v>
+      </c>
+      <c r="D218">
+        <v>13</v>
+      </c>
+      <c r="E218" t="s">
+        <v>20</v>
+      </c>
+      <c r="F218">
+        <v>2182.8000000000002</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6">
+      <c r="A219" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B219" s="5">
+        <v>0.70972222222222225</v>
+      </c>
+      <c r="D219">
+        <v>14</v>
+      </c>
+      <c r="E219" t="s">
+        <v>21</v>
+      </c>
+      <c r="F219">
+        <v>1448.4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6">
+      <c r="A220" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B220" s="5">
+        <v>0.70972222222222225</v>
+      </c>
+      <c r="D220">
+        <v>11</v>
+      </c>
+      <c r="E220" t="s">
+        <v>22</v>
+      </c>
+      <c r="F220">
+        <v>2210.1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6">
+      <c r="A221" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B221" s="5">
+        <v>0.70972222222222225</v>
+      </c>
+      <c r="D221">
+        <v>1</v>
+      </c>
+      <c r="E221" t="s">
+        <v>23</v>
+      </c>
+      <c r="F221">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6">
+      <c r="A222" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B222" s="5">
+        <v>0.72638888888888886</v>
+      </c>
+      <c r="D222">
+        <v>10</v>
+      </c>
+      <c r="E222" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6">
+      <c r="A223" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B223" s="5">
+        <v>0.75138888888888899</v>
+      </c>
+      <c r="D223">
+        <v>4</v>
+      </c>
+      <c r="E223" t="s">
+        <v>9</v>
+      </c>
+      <c r="F223">
+        <v>1922.3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6">
+      <c r="A224" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B224" s="5">
+        <v>0.75138888888888899</v>
+      </c>
+      <c r="D224">
+        <v>2</v>
+      </c>
+      <c r="E224" t="s">
+        <v>11</v>
+      </c>
+      <c r="F224">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6">
+      <c r="A225" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B225" s="5">
+        <v>0.75138888888888899</v>
+      </c>
+      <c r="D225">
+        <v>12</v>
+      </c>
+      <c r="E225" t="s">
+        <v>13</v>
+      </c>
+      <c r="F225">
+        <v>1697.5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6">
+      <c r="A226" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B226" s="5">
+        <v>0.75138888888888899</v>
+      </c>
+      <c r="D226">
+        <v>8</v>
+      </c>
+      <c r="E226" t="s">
+        <v>15</v>
+      </c>
+      <c r="F226">
+        <v>2148.6</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6">
+      <c r="A227" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B227" s="5">
+        <v>0.75138888888888899</v>
+      </c>
+      <c r="D227">
+        <v>5</v>
+      </c>
+      <c r="E227" t="s">
+        <v>16</v>
+      </c>
+      <c r="F227">
+        <v>1663.8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6">
+      <c r="A228" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B228" s="5">
+        <v>0.75138888888888899</v>
+      </c>
+      <c r="D228">
+        <v>9</v>
+      </c>
+      <c r="E228" t="s">
+        <v>17</v>
+      </c>
+      <c r="F228">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6">
+      <c r="A229" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B229" s="5">
+        <v>0.7680555555555556</v>
+      </c>
+      <c r="D229">
+        <v>10</v>
+      </c>
+      <c r="E229" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6">
+      <c r="A230" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B230" s="5">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D230">
+        <v>6</v>
+      </c>
+      <c r="E230" t="s">
+        <v>1</v>
+      </c>
+      <c r="F230">
+        <v>1965.9</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6">
+      <c r="A231" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B231" s="5">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D231">
+        <v>16</v>
+      </c>
+      <c r="E231" t="s">
+        <v>2</v>
+      </c>
+      <c r="F231">
+        <v>2175.6999999999998</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6">
+      <c r="A232" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B232" s="5">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D232">
+        <v>13</v>
+      </c>
+      <c r="E232" t="s">
+        <v>3</v>
+      </c>
+      <c r="F232">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6">
+      <c r="A233" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B233" s="5">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D233">
+        <v>14</v>
+      </c>
+      <c r="E233" t="s">
+        <v>4</v>
+      </c>
+      <c r="F233">
+        <v>1847.1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6">
+      <c r="A234" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B234" s="5">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D234">
+        <v>11</v>
+      </c>
+      <c r="E234" t="s">
+        <v>6</v>
+      </c>
+      <c r="F234">
+        <v>1856.5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6">
+      <c r="A235" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B235" s="5">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="D235">
+        <v>1</v>
+      </c>
+      <c r="E235" t="s">
+        <v>7</v>
+      </c>
+      <c r="F235">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6">
+      <c r="A236" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B236" s="5">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D236">
+        <v>10</v>
+      </c>
+      <c r="E236" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6">
+      <c r="A237" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B237" s="5">
+        <v>0.93888888888888899</v>
+      </c>
+      <c r="D237">
+        <v>4</v>
+      </c>
+      <c r="E237" t="s">
+        <v>25</v>
+      </c>
+      <c r="F237">
+        <v>2080.6</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6">
+      <c r="A238" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B238" s="5">
+        <v>0.93888888888888899</v>
+      </c>
+      <c r="D238">
+        <v>2</v>
+      </c>
+      <c r="E238" t="s">
+        <v>26</v>
+      </c>
+      <c r="F238">
+        <v>1978.2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6">
+      <c r="A239" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B239" s="5">
+        <v>0.93888888888888899</v>
+      </c>
+      <c r="D239">
+        <v>12</v>
+      </c>
+      <c r="E239" t="s">
+        <v>27</v>
+      </c>
+      <c r="F239">
+        <v>1947.7</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6">
+      <c r="A240" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B240" s="5">
+        <v>0.93888888888888899</v>
+      </c>
+      <c r="D240">
+        <v>8</v>
+      </c>
+      <c r="E240" t="s">
+        <v>28</v>
+      </c>
+      <c r="F240">
+        <v>2010.7</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6">
+      <c r="A241" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B241" s="5">
+        <v>0.93888888888888899</v>
+      </c>
+      <c r="D241">
+        <v>5</v>
+      </c>
+      <c r="E241" t="s">
+        <v>29</v>
+      </c>
+      <c r="F241">
+        <v>2144</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6">
+      <c r="A242" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B242" s="5">
+        <v>0.93888888888888899</v>
+      </c>
+      <c r="D242">
+        <v>9</v>
+      </c>
+      <c r="E242" t="s">
+        <v>30</v>
+      </c>
+      <c r="F242">
+        <v>1637.1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6">
+      <c r="A243" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B243" s="5">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="D243">
+        <v>10</v>
+      </c>
+      <c r="E243" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6">
+      <c r="A244" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B244" s="5">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="D244">
+        <v>6</v>
+      </c>
+      <c r="E244" t="s">
+        <v>5</v>
+      </c>
+      <c r="F244">
+        <v>1612.7</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6">
+      <c r="A245" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B245" s="5">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="D245">
+        <v>16</v>
+      </c>
+      <c r="E245" t="s">
+        <v>24</v>
+      </c>
+      <c r="F245">
+        <v>1906.9</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6">
+      <c r="A246" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B246" s="5">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="D246">
+        <v>13</v>
+      </c>
+      <c r="E246" t="s">
+        <v>8</v>
+      </c>
+      <c r="F246">
+        <v>1288.9000000000001</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6">
+      <c r="A247" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B247" s="5">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="D247">
+        <v>14</v>
+      </c>
+      <c r="E247" t="s">
+        <v>10</v>
+      </c>
+      <c r="F247">
+        <v>2045.6</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6">
+      <c r="A248" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B248" s="5">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="D248">
+        <v>11</v>
+      </c>
+      <c r="E248" t="s">
+        <v>12</v>
+      </c>
+      <c r="F248">
+        <v>1733.5</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6">
+      <c r="A249" s="1">
+        <v>42262</v>
+      </c>
+      <c r="B249" s="5">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="D249">
+        <v>1</v>
+      </c>
+      <c r="E249" t="s">
+        <v>14</v>
+      </c>
+      <c r="F249">
+        <v>2014.4</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6">
+      <c r="A250" s="1"/>
+      <c r="B250" s="5"/>
+    </row>
+    <row r="251" spans="1:6">
+      <c r="B251" s="5"/>
+    </row>
+    <row r="252" spans="1:6">
+      <c r="B252" s="5"/>
+    </row>
+    <row r="253" spans="1:6">
+      <c r="B253" s="5"/>
+    </row>
+    <row r="254" spans="1:6">
+      <c r="B254" s="5"/>
+    </row>
+    <row r="255" spans="1:6">
+      <c r="B255" s="5"/>
+    </row>
+    <row r="256" spans="1:6">
+      <c r="B256" s="5"/>
+    </row>
+    <row r="257" spans="2:4">
+      <c r="B257" s="5"/>
+    </row>
+    <row r="258" spans="2:4">
+      <c r="B258" s="5"/>
+    </row>
+    <row r="259" spans="2:4">
+      <c r="B259" s="5"/>
+    </row>
+    <row r="260" spans="2:4">
+      <c r="B260" s="5"/>
+    </row>
+    <row r="261" spans="2:4">
+      <c r="B261" s="5"/>
+    </row>
+    <row r="262" spans="2:4">
+      <c r="B262" s="5"/>
+    </row>
+    <row r="263" spans="2:4">
+      <c r="B263" s="5"/>
+    </row>
+    <row r="264" spans="2:4">
+      <c r="B264" s="5"/>
+    </row>
+    <row r="265" spans="2:4">
+      <c r="B265" s="5"/>
+    </row>
+    <row r="266" spans="2:4">
+      <c r="D266" s="2"/>
+    </row>
+    <row r="267" spans="2:4">
+      <c r="D267" s="2"/>
+    </row>
+    <row r="268" spans="2:4">
+      <c r="D268" s="2"/>
+    </row>
+    <row r="269" spans="2:4">
+      <c r="D269" s="2"/>
+    </row>
+    <row r="270" spans="2:4">
+      <c r="D270" s="2"/>
+    </row>
+    <row r="271" spans="2:4">
+      <c r="D271" s="2"/>
+    </row>
+    <row r="272" spans="2:4">
+      <c r="D272" s="2"/>
+    </row>
+    <row r="273" spans="4:4">
+      <c r="D273" s="2"/>
+    </row>
+    <row r="274" spans="4:4">
+      <c r="D274" s="2"/>
+    </row>
+    <row r="275" spans="4:4">
+      <c r="D275" s="2"/>
+    </row>
+    <row r="276" spans="4:4">
+      <c r="D276" s="2"/>
+    </row>
+    <row r="277" spans="4:4">
+      <c r="D277" s="2"/>
+    </row>
+    <row r="278" spans="4:4">
+      <c r="D278" s="2"/>
+    </row>
+    <row r="279" spans="4:4">
+      <c r="D279" s="2"/>
+    </row>
+    <row r="280" spans="4:4">
+      <c r="D280" s="2"/>
+    </row>
+    <row r="281" spans="4:4">
+      <c r="D281" s="2"/>
+    </row>
+    <row r="282" spans="4:4">
+      <c r="D282" s="2"/>
+    </row>
+    <row r="283" spans="4:4">
+      <c r="D283" s="2"/>
+    </row>
+    <row r="284" spans="4:4">
+      <c r="D284" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Corrected faulty mass value for AL 8 on 22 September, and added core labels to mass graph.
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="62">
   <si>
     <t>Treatment</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t xml:space="preserve">Placeholder; apparently the Picarro ran from the night of 8 Sep until midday 11 September </t>
+  </si>
+  <si>
+    <t>Mass corrected from 12952.6</t>
   </si>
 </sst>
 </file>
@@ -1440,8 +1443,8 @@
   <dimension ref="A1:G452"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B209" sqref="B209"/>
+      <pane ySplit="2" topLeftCell="A423" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G439" sqref="G439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8821,7 +8824,10 @@
         <v>8</v>
       </c>
       <c r="F438">
-        <v>12952.6</v>
+        <v>1295.5999999999999</v>
+      </c>
+      <c r="G438" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="439" spans="1:7">

</xml_diff>

<commit_message>
Corrected faulty mass values for AL8 and AL29 on 22 September
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11020" yWindow="0" windowWidth="27420" windowHeight="24320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="treatments.csv" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="63">
   <si>
     <t>Treatment</t>
   </si>
@@ -205,7 +205,10 @@
     <t xml:space="preserve">Placeholder; apparently the Picarro ran from the night of 8 Sep until midday 11 September </t>
   </si>
   <si>
-    <t>Mass corrected from 12952.6</t>
+    <t>Changed from 1827 per PS email</t>
+  </si>
+  <si>
+    <t>Changed from 12952.6 per PS email</t>
   </si>
 </sst>
 </file>
@@ -276,8 +279,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="185">
+  <cellStyleXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -473,7 +478,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="185">
+  <cellStyles count="187">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -566,6 +571,7 @@
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -658,6 +664,7 @@
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1443,8 +1450,8 @@
   <dimension ref="A1:G452"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A423" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G439" sqref="G439"/>
+      <pane ySplit="2" topLeftCell="A427" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F439" sqref="F439"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8824,10 +8831,10 @@
         <v>8</v>
       </c>
       <c r="F438">
-        <v>1295.5999999999999</v>
+        <v>1292.5999999999999</v>
       </c>
       <c r="G438" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="439" spans="1:7">
@@ -8861,7 +8868,10 @@
         <v>12</v>
       </c>
       <c r="F440">
-        <v>1827</v>
+        <v>1727</v>
+      </c>
+      <c r="G440" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="441" spans="1:7">

</xml_diff>

<commit_message>
Fixed typo in AL 12 10/27 mass
See issue #17.
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28480" windowHeight="24460" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="24200" windowHeight="15040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="treatments.csv" sheetId="2" r:id="rId1"/>
@@ -1582,8 +1582,8 @@
   <dimension ref="A1:G934"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A839" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E879" sqref="E879"/>
+      <pane ySplit="2" topLeftCell="A855" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F867" sqref="F867"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -15399,7 +15399,7 @@
         <v>25</v>
       </c>
       <c r="F866" s="13">
-        <v>2124.8000000000002</v>
+        <v>2024.8</v>
       </c>
       <c r="G866" s="4" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Removed data per Peyton notes
and generated new diagnostics
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="24200" windowHeight="15040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="15600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="treatments.csv" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="75">
   <si>
     <t>Treatment</t>
   </si>
@@ -234,6 +234,18 @@
   <si>
     <t>***second run of duplicate measurements. First run questionable. Let's disucss.</t>
   </si>
+  <si>
+    <t>and again at:20:44</t>
+  </si>
+  <si>
+    <t>Ignore all data collected past 23:14:04</t>
+  </si>
+  <si>
+    <t>I think we should remove these!</t>
+  </si>
+  <si>
+    <t>Keep these</t>
+  </si>
 </sst>
 </file>
 
@@ -243,7 +255,7 @@
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +298,20 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -313,7 +339,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="231">
+  <cellStyleXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -545,8 +571,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -565,8 +603,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="231">
+  <cellStyles count="243">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -682,6 +723,12 @@
     <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -797,6 +844,12 @@
     <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1099,7 +1152,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -1579,11 +1632,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G934"/>
+  <dimension ref="A1:G1064"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A855" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F867" sqref="F867"/>
+      <pane ySplit="2" topLeftCell="A983" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1011" sqref="E1011"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -15656,169 +15709,2252 @@
       <c r="F879" s="8"/>
     </row>
     <row r="880" spans="1:7">
-      <c r="D880" s="2"/>
-    </row>
-    <row r="881" spans="4:4">
-      <c r="D881" s="2"/>
-    </row>
-    <row r="882" spans="4:4">
-      <c r="D882" s="2"/>
-    </row>
-    <row r="883" spans="4:4">
-      <c r="D883" s="2"/>
-    </row>
-    <row r="884" spans="4:4">
-      <c r="D884" s="2"/>
-    </row>
-    <row r="885" spans="4:4">
-      <c r="D885" s="2"/>
-    </row>
-    <row r="886" spans="4:4">
-      <c r="D886" s="2"/>
-    </row>
-    <row r="887" spans="4:4">
-      <c r="D887" s="2"/>
-    </row>
-    <row r="888" spans="4:4">
-      <c r="D888" s="2"/>
-    </row>
-    <row r="889" spans="4:4">
-      <c r="D889" s="2"/>
-    </row>
-    <row r="890" spans="4:4">
-      <c r="D890" s="2"/>
-    </row>
-    <row r="891" spans="4:4">
-      <c r="D891" s="2"/>
-    </row>
-    <row r="892" spans="4:4">
-      <c r="D892" s="2"/>
-    </row>
-    <row r="893" spans="4:4">
-      <c r="D893" s="2"/>
-    </row>
-    <row r="894" spans="4:4">
-      <c r="D894" s="2"/>
-    </row>
-    <row r="895" spans="4:4">
-      <c r="D895" s="2"/>
-    </row>
-    <row r="896" spans="4:4">
-      <c r="D896" s="2"/>
-    </row>
-    <row r="897" spans="4:4">
-      <c r="D897" s="2"/>
-    </row>
-    <row r="898" spans="4:4">
-      <c r="D898" s="2"/>
-    </row>
-    <row r="899" spans="4:4">
-      <c r="D899" s="2"/>
-    </row>
-    <row r="900" spans="4:4">
-      <c r="D900" s="2"/>
-    </row>
-    <row r="901" spans="4:4">
-      <c r="D901" s="2"/>
-    </row>
-    <row r="902" spans="4:4">
-      <c r="D902" s="2"/>
-    </row>
-    <row r="903" spans="4:4">
-      <c r="D903" s="2"/>
-    </row>
-    <row r="904" spans="4:4">
-      <c r="D904" s="2"/>
-    </row>
-    <row r="905" spans="4:4">
-      <c r="D905" s="2"/>
-    </row>
-    <row r="906" spans="4:4">
-      <c r="D906" s="2"/>
-    </row>
-    <row r="907" spans="4:4">
-      <c r="D907" s="2"/>
-    </row>
-    <row r="908" spans="4:4">
-      <c r="D908" s="2"/>
-    </row>
-    <row r="909" spans="4:4">
-      <c r="D909" s="2"/>
-    </row>
-    <row r="910" spans="4:4">
-      <c r="D910" s="2"/>
-    </row>
-    <row r="911" spans="4:4">
-      <c r="D911" s="2"/>
-    </row>
-    <row r="912" spans="4:4">
-      <c r="D912" s="2"/>
-    </row>
-    <row r="913" spans="4:4">
-      <c r="D913" s="2"/>
-    </row>
-    <row r="914" spans="4:4">
-      <c r="D914" s="2"/>
-    </row>
-    <row r="915" spans="4:4">
-      <c r="D915" s="2"/>
-    </row>
-    <row r="916" spans="4:4">
-      <c r="D916" s="2"/>
-    </row>
-    <row r="917" spans="4:4">
-      <c r="D917" s="2"/>
-    </row>
-    <row r="918" spans="4:4">
-      <c r="D918" s="2"/>
-    </row>
-    <row r="919" spans="4:4">
-      <c r="D919" s="2"/>
-    </row>
-    <row r="920" spans="4:4">
-      <c r="D920" s="2"/>
-    </row>
-    <row r="921" spans="4:4">
-      <c r="D921" s="2"/>
-    </row>
-    <row r="922" spans="4:4">
-      <c r="D922" s="2"/>
-    </row>
-    <row r="923" spans="4:4">
-      <c r="D923" s="2"/>
-    </row>
-    <row r="924" spans="4:4">
-      <c r="D924" s="2"/>
-    </row>
-    <row r="925" spans="4:4">
-      <c r="D925" s="2"/>
-    </row>
-    <row r="926" spans="4:4">
-      <c r="D926" s="2"/>
-    </row>
-    <row r="927" spans="4:4">
-      <c r="D927" s="2"/>
-    </row>
-    <row r="928" spans="4:4">
-      <c r="D928" s="2"/>
-    </row>
-    <row r="929" spans="4:4">
-      <c r="D929" s="2"/>
-    </row>
-    <row r="930" spans="4:4">
-      <c r="D930" s="2"/>
-    </row>
-    <row r="931" spans="4:4">
-      <c r="D931" s="2"/>
-    </row>
-    <row r="932" spans="4:4">
-      <c r="D932" s="2"/>
-    </row>
-    <row r="933" spans="4:4">
-      <c r="D933" s="2"/>
-    </row>
-    <row r="934" spans="4:4">
-      <c r="D934" s="2"/>
+      <c r="A880" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B880" s="5"/>
+      <c r="E880" t="s">
+        <v>1</v>
+      </c>
+      <c r="F880" s="8">
+        <v>1955.4</v>
+      </c>
+    </row>
+    <row r="881" spans="1:6">
+      <c r="A881" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B881" s="5"/>
+      <c r="E881" t="s">
+        <v>2</v>
+      </c>
+      <c r="F881" s="8">
+        <v>2167.5</v>
+      </c>
+    </row>
+    <row r="882" spans="1:6">
+      <c r="A882" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B882" s="5"/>
+      <c r="E882" t="s">
+        <v>3</v>
+      </c>
+      <c r="F882" s="8">
+        <v>1422.5</v>
+      </c>
+    </row>
+    <row r="883" spans="1:6">
+      <c r="A883" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B883" s="5"/>
+      <c r="E883" t="s">
+        <v>4</v>
+      </c>
+      <c r="F883" s="8">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="884" spans="1:6">
+      <c r="A884" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B884" s="5"/>
+      <c r="E884" t="s">
+        <v>6</v>
+      </c>
+      <c r="F884" s="8">
+        <v>1844.7</v>
+      </c>
+    </row>
+    <row r="885" spans="1:6">
+      <c r="A885" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B885" s="5"/>
+      <c r="E885" t="s">
+        <v>7</v>
+      </c>
+      <c r="F885" s="8">
+        <v>2011.4</v>
+      </c>
+    </row>
+    <row r="886" spans="1:6">
+      <c r="A886" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B886" s="5"/>
+      <c r="E886" t="s">
+        <v>9</v>
+      </c>
+      <c r="F886" s="8">
+        <v>1903.4</v>
+      </c>
+    </row>
+    <row r="887" spans="1:6">
+      <c r="A887" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B887" s="5"/>
+      <c r="E887" t="s">
+        <v>11</v>
+      </c>
+      <c r="F887" s="8">
+        <v>1690.9</v>
+      </c>
+    </row>
+    <row r="888" spans="1:6">
+      <c r="A888" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B888" s="5"/>
+      <c r="E888" t="s">
+        <v>13</v>
+      </c>
+      <c r="F888" s="8">
+        <v>1630.9</v>
+      </c>
+    </row>
+    <row r="889" spans="1:6">
+      <c r="A889" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B889" s="5"/>
+      <c r="E889" t="s">
+        <v>15</v>
+      </c>
+      <c r="F889" s="8">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="890" spans="1:6">
+      <c r="A890" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B890" s="5"/>
+      <c r="E890" t="s">
+        <v>16</v>
+      </c>
+      <c r="F890" s="8">
+        <v>1645.5</v>
+      </c>
+    </row>
+    <row r="891" spans="1:6">
+      <c r="A891" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B891" s="5"/>
+      <c r="E891" t="s">
+        <v>17</v>
+      </c>
+      <c r="F891" s="8">
+        <v>1633.5</v>
+      </c>
+    </row>
+    <row r="892" spans="1:6">
+      <c r="A892" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B892" s="5"/>
+      <c r="E892" t="s">
+        <v>18</v>
+      </c>
+      <c r="F892" s="8">
+        <v>1539.1</v>
+      </c>
+    </row>
+    <row r="893" spans="1:6">
+      <c r="A893" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B893" s="5"/>
+      <c r="E893" t="s">
+        <v>19</v>
+      </c>
+      <c r="F893" s="8">
+        <v>1915.9</v>
+      </c>
+    </row>
+    <row r="894" spans="1:6">
+      <c r="A894" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B894" s="5"/>
+      <c r="E894" t="s">
+        <v>20</v>
+      </c>
+      <c r="F894" s="8">
+        <v>2138.6999999999998</v>
+      </c>
+    </row>
+    <row r="895" spans="1:6">
+      <c r="A895" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B895" s="5"/>
+      <c r="E895" t="s">
+        <v>21</v>
+      </c>
+      <c r="F895" s="8">
+        <v>1416.9</v>
+      </c>
+    </row>
+    <row r="896" spans="1:6">
+      <c r="A896" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B896" s="5"/>
+      <c r="E896" t="s">
+        <v>22</v>
+      </c>
+      <c r="F896" s="8">
+        <v>2169.4</v>
+      </c>
+    </row>
+    <row r="897" spans="1:6">
+      <c r="A897" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B897" s="5"/>
+      <c r="E897" t="s">
+        <v>23</v>
+      </c>
+      <c r="F897" s="8">
+        <v>1658</v>
+      </c>
+    </row>
+    <row r="898" spans="1:6">
+      <c r="A898" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B898" s="5"/>
+      <c r="E898" t="s">
+        <v>25</v>
+      </c>
+      <c r="F898" s="8">
+        <v>2017.6</v>
+      </c>
+    </row>
+    <row r="899" spans="1:6">
+      <c r="A899" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B899" s="5"/>
+      <c r="E899" t="s">
+        <v>26</v>
+      </c>
+      <c r="F899" s="8">
+        <v>1907.1</v>
+      </c>
+    </row>
+    <row r="900" spans="1:6">
+      <c r="A900" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B900" s="5"/>
+      <c r="E900" t="s">
+        <v>27</v>
+      </c>
+      <c r="F900" s="8">
+        <v>1876.6</v>
+      </c>
+    </row>
+    <row r="901" spans="1:6">
+      <c r="A901" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B901" s="5"/>
+      <c r="E901" t="s">
+        <v>28</v>
+      </c>
+      <c r="F901" s="8">
+        <v>1953.6</v>
+      </c>
+    </row>
+    <row r="902" spans="1:6">
+      <c r="A902" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B902" s="5"/>
+      <c r="E902" t="s">
+        <v>29</v>
+      </c>
+      <c r="F902" s="8">
+        <v>2091.5</v>
+      </c>
+    </row>
+    <row r="903" spans="1:6">
+      <c r="A903" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B903" s="5"/>
+      <c r="E903" t="s">
+        <v>30</v>
+      </c>
+      <c r="F903" s="8">
+        <v>1548.9</v>
+      </c>
+    </row>
+    <row r="904" spans="1:6">
+      <c r="A904" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B904" s="5"/>
+      <c r="E904" t="s">
+        <v>5</v>
+      </c>
+      <c r="F904" s="8">
+        <v>1576.9</v>
+      </c>
+    </row>
+    <row r="905" spans="1:6">
+      <c r="A905" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B905" s="5"/>
+      <c r="E905" t="s">
+        <v>24</v>
+      </c>
+      <c r="F905" s="8">
+        <v>1893.2</v>
+      </c>
+    </row>
+    <row r="906" spans="1:6">
+      <c r="A906" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B906" s="5"/>
+      <c r="E906" t="s">
+        <v>8</v>
+      </c>
+      <c r="F906" s="8">
+        <v>1273.2</v>
+      </c>
+    </row>
+    <row r="907" spans="1:6">
+      <c r="A907" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B907" s="5"/>
+      <c r="E907" t="s">
+        <v>10</v>
+      </c>
+      <c r="F907" s="8">
+        <v>2027.5</v>
+      </c>
+    </row>
+    <row r="908" spans="1:6">
+      <c r="A908" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B908" s="5"/>
+      <c r="E908" t="s">
+        <v>12</v>
+      </c>
+      <c r="F908" s="8">
+        <v>1714.1</v>
+      </c>
+    </row>
+    <row r="909" spans="1:6">
+      <c r="A909" s="1">
+        <v>42310</v>
+      </c>
+      <c r="B909" s="5"/>
+      <c r="E909" t="s">
+        <v>14</v>
+      </c>
+      <c r="F909" s="8">
+        <v>1988.3</v>
+      </c>
+    </row>
+    <row r="910" spans="1:6">
+      <c r="A910" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B910" s="5">
+        <v>0.76111111111111107</v>
+      </c>
+      <c r="D910">
+        <v>10</v>
+      </c>
+      <c r="E910" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F910" s="8"/>
+    </row>
+    <row r="911" spans="1:6">
+      <c r="A911" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B911" s="5">
+        <v>0.76527777777777783</v>
+      </c>
+      <c r="D911">
+        <v>6</v>
+      </c>
+      <c r="E911" t="s">
+        <v>1</v>
+      </c>
+      <c r="F911" s="8">
+        <v>1964.1</v>
+      </c>
+    </row>
+    <row r="912" spans="1:6">
+      <c r="A912" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B912" s="5">
+        <v>0.76527777777777783</v>
+      </c>
+      <c r="D912">
+        <v>16</v>
+      </c>
+      <c r="E912" t="s">
+        <v>2</v>
+      </c>
+      <c r="F912" s="8">
+        <v>2171.1</v>
+      </c>
+    </row>
+    <row r="913" spans="1:7">
+      <c r="A913" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B913" s="5">
+        <v>0.76527777777777783</v>
+      </c>
+      <c r="D913">
+        <v>13</v>
+      </c>
+      <c r="E913" t="s">
+        <v>3</v>
+      </c>
+      <c r="F913" s="8">
+        <v>1421.4</v>
+      </c>
+    </row>
+    <row r="914" spans="1:7">
+      <c r="A914" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B914" s="5">
+        <v>0.76527777777777783</v>
+      </c>
+      <c r="D914">
+        <v>14</v>
+      </c>
+      <c r="E914" t="s">
+        <v>4</v>
+      </c>
+      <c r="F914" s="8">
+        <v>1837.7</v>
+      </c>
+    </row>
+    <row r="915" spans="1:7">
+      <c r="A915" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B915" s="5">
+        <v>0.76527777777777783</v>
+      </c>
+      <c r="D915">
+        <v>11</v>
+      </c>
+      <c r="E915" t="s">
+        <v>6</v>
+      </c>
+      <c r="F915" s="8">
+        <v>1850.4</v>
+      </c>
+    </row>
+    <row r="916" spans="1:7">
+      <c r="A916" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B916" s="5">
+        <v>0.76527777777777783</v>
+      </c>
+      <c r="D916">
+        <v>1</v>
+      </c>
+      <c r="E916" t="s">
+        <v>7</v>
+      </c>
+      <c r="F916" s="8">
+        <v>2013.9</v>
+      </c>
+    </row>
+    <row r="917" spans="1:7">
+      <c r="A917" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B917" s="5">
+        <v>0.78194444444444444</v>
+      </c>
+      <c r="D917">
+        <v>10</v>
+      </c>
+      <c r="E917" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="918" spans="1:7">
+      <c r="A918" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B918" s="5">
+        <v>0.78888888888888886</v>
+      </c>
+      <c r="D918">
+        <v>4</v>
+      </c>
+      <c r="E918" t="s">
+        <v>9</v>
+      </c>
+      <c r="F918" s="8">
+        <v>1934.9</v>
+      </c>
+    </row>
+    <row r="919" spans="1:7">
+      <c r="A919" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B919" s="5">
+        <v>0.78888888888888886</v>
+      </c>
+      <c r="D919">
+        <v>2</v>
+      </c>
+      <c r="E919" t="s">
+        <v>11</v>
+      </c>
+      <c r="F919" s="8">
+        <v>1704.3</v>
+      </c>
+    </row>
+    <row r="920" spans="1:7">
+      <c r="A920" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B920" s="5">
+        <v>0.78888888888888886</v>
+      </c>
+      <c r="D920">
+        <v>12</v>
+      </c>
+      <c r="E920" t="s">
+        <v>13</v>
+      </c>
+      <c r="F920" s="8">
+        <v>1634.8</v>
+      </c>
+    </row>
+    <row r="921" spans="1:7">
+      <c r="A921" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B921" s="5">
+        <v>0.78888888888888886</v>
+      </c>
+      <c r="D921">
+        <v>8</v>
+      </c>
+      <c r="E921" t="s">
+        <v>15</v>
+      </c>
+      <c r="F921" s="8">
+        <v>2115.4</v>
+      </c>
+    </row>
+    <row r="922" spans="1:7">
+      <c r="A922" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B922" s="5">
+        <v>0.78888888888888886</v>
+      </c>
+      <c r="D922">
+        <v>5</v>
+      </c>
+      <c r="E922" t="s">
+        <v>16</v>
+      </c>
+      <c r="F922" s="8">
+        <v>1666.4</v>
+      </c>
+    </row>
+    <row r="923" spans="1:7">
+      <c r="A923" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B923" s="5">
+        <v>0.78888888888888886</v>
+      </c>
+      <c r="D923">
+        <v>9</v>
+      </c>
+      <c r="E923" t="s">
+        <v>17</v>
+      </c>
+      <c r="F923" s="8">
+        <v>1632.2</v>
+      </c>
+    </row>
+    <row r="924" spans="1:7">
+      <c r="A924" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B924" s="5">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="D924">
+        <v>10</v>
+      </c>
+      <c r="E924" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="925" spans="1:7">
+      <c r="A925" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B925" s="5">
+        <v>0.8340277777777777</v>
+      </c>
+      <c r="D925">
+        <v>6</v>
+      </c>
+      <c r="E925" t="s">
+        <v>18</v>
+      </c>
+      <c r="F925" s="8">
+        <v>1543.9</v>
+      </c>
+      <c r="G925" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="926" spans="1:7">
+      <c r="A926" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B926" s="5">
+        <v>0.8340277777777777</v>
+      </c>
+      <c r="D926">
+        <v>16</v>
+      </c>
+      <c r="E926" t="s">
+        <v>19</v>
+      </c>
+      <c r="F926" s="8">
+        <v>1919.9</v>
+      </c>
+      <c r="G926" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="927" spans="1:7">
+      <c r="A927" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B927" s="5">
+        <v>0.8340277777777777</v>
+      </c>
+      <c r="D927">
+        <v>13</v>
+      </c>
+      <c r="E927" t="s">
+        <v>20</v>
+      </c>
+      <c r="F927" s="8">
+        <v>2143.1</v>
+      </c>
+      <c r="G927" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="928" spans="1:7">
+      <c r="A928" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B928" s="5">
+        <v>0.8340277777777777</v>
+      </c>
+      <c r="D928">
+        <v>14</v>
+      </c>
+      <c r="E928" t="s">
+        <v>21</v>
+      </c>
+      <c r="F928" s="8">
+        <v>1435.1</v>
+      </c>
+      <c r="G928" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="929" spans="1:7">
+      <c r="A929" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B929" s="5">
+        <v>0.8340277777777777</v>
+      </c>
+      <c r="D929">
+        <v>11</v>
+      </c>
+      <c r="E929" t="s">
+        <v>22</v>
+      </c>
+      <c r="F929" s="8">
+        <v>2173.5</v>
+      </c>
+      <c r="G929" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="930" spans="1:7">
+      <c r="A930" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B930" s="5">
+        <v>0.8340277777777777</v>
+      </c>
+      <c r="D930">
+        <v>1</v>
+      </c>
+      <c r="E930" t="s">
+        <v>23</v>
+      </c>
+      <c r="F930" s="8">
+        <v>1662.9</v>
+      </c>
+      <c r="G930" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="931" spans="1:7">
+      <c r="A931" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B931" s="5">
+        <v>0.8881944444444444</v>
+      </c>
+      <c r="D931">
+        <v>10</v>
+      </c>
+      <c r="E931" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="932" spans="1:7">
+      <c r="A932" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B932" s="5">
+        <v>0.92291666666666661</v>
+      </c>
+      <c r="D932">
+        <v>4</v>
+      </c>
+      <c r="E932" t="s">
+        <v>25</v>
+      </c>
+      <c r="F932" s="8">
+        <v>2027</v>
+      </c>
+      <c r="G932" s="4"/>
+    </row>
+    <row r="933" spans="1:7">
+      <c r="A933" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B933" s="5">
+        <v>0.92291666666666661</v>
+      </c>
+      <c r="D933">
+        <v>2</v>
+      </c>
+      <c r="E933" t="s">
+        <v>26</v>
+      </c>
+      <c r="F933" s="8">
+        <v>1906</v>
+      </c>
+      <c r="G933" s="4"/>
+    </row>
+    <row r="934" spans="1:7">
+      <c r="A934" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B934" s="5">
+        <v>0.92291666666666661</v>
+      </c>
+      <c r="D934">
+        <v>12</v>
+      </c>
+      <c r="E934" t="s">
+        <v>27</v>
+      </c>
+      <c r="F934" s="8">
+        <v>1875.2</v>
+      </c>
+      <c r="G934" s="4"/>
+    </row>
+    <row r="935" spans="1:7">
+      <c r="A935" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B935" s="5">
+        <v>0.92291666666666661</v>
+      </c>
+      <c r="D935">
+        <v>8</v>
+      </c>
+      <c r="E935" t="s">
+        <v>28</v>
+      </c>
+      <c r="F935" s="8">
+        <v>1956.8</v>
+      </c>
+      <c r="G935" s="4"/>
+    </row>
+    <row r="936" spans="1:7">
+      <c r="A936" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B936" s="5">
+        <v>0.92291666666666661</v>
+      </c>
+      <c r="D936">
+        <v>5</v>
+      </c>
+      <c r="E936" t="s">
+        <v>29</v>
+      </c>
+      <c r="F936" s="8">
+        <v>2090.1</v>
+      </c>
+      <c r="G936" s="4"/>
+    </row>
+    <row r="937" spans="1:7">
+      <c r="A937" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B937" s="5">
+        <v>0.92291666666666661</v>
+      </c>
+      <c r="D937">
+        <v>9</v>
+      </c>
+      <c r="E937" t="s">
+        <v>30</v>
+      </c>
+      <c r="F937" s="8">
+        <v>1555.2</v>
+      </c>
+      <c r="G937" s="4"/>
+    </row>
+    <row r="938" spans="1:7">
+      <c r="A938" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B938" s="5">
+        <v>0.93958333333333333</v>
+      </c>
+      <c r="D938">
+        <v>10</v>
+      </c>
+      <c r="E938" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="939" spans="1:7">
+      <c r="A939" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B939" s="5">
+        <v>0.94652777777777775</v>
+      </c>
+      <c r="D939">
+        <v>6</v>
+      </c>
+      <c r="E939" t="s">
+        <v>5</v>
+      </c>
+      <c r="F939" s="8">
+        <v>1587.5</v>
+      </c>
+    </row>
+    <row r="940" spans="1:7">
+      <c r="A940" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B940" s="5">
+        <v>0.94652777777777775</v>
+      </c>
+      <c r="D940">
+        <v>16</v>
+      </c>
+      <c r="E940" t="s">
+        <v>24</v>
+      </c>
+      <c r="F940" s="8">
+        <v>1892.1</v>
+      </c>
+    </row>
+    <row r="941" spans="1:7">
+      <c r="A941" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B941" s="5">
+        <v>0.94652777777777775</v>
+      </c>
+      <c r="D941">
+        <v>13</v>
+      </c>
+      <c r="E941" t="s">
+        <v>8</v>
+      </c>
+      <c r="F941" s="8">
+        <v>1272.2</v>
+      </c>
+    </row>
+    <row r="942" spans="1:7">
+      <c r="A942" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B942" s="5">
+        <v>0.94652777777777775</v>
+      </c>
+      <c r="D942">
+        <v>14</v>
+      </c>
+      <c r="E942" t="s">
+        <v>10</v>
+      </c>
+      <c r="F942" s="8">
+        <v>2023.7</v>
+      </c>
+    </row>
+    <row r="943" spans="1:7">
+      <c r="A943" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B943" s="5">
+        <v>0.94652777777777775</v>
+      </c>
+      <c r="D943">
+        <v>11</v>
+      </c>
+      <c r="E943" t="s">
+        <v>12</v>
+      </c>
+      <c r="F943" s="8">
+        <v>1716.5</v>
+      </c>
+    </row>
+    <row r="944" spans="1:7">
+      <c r="A944" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B944" s="5">
+        <v>0.94652777777777775</v>
+      </c>
+      <c r="D944">
+        <v>1</v>
+      </c>
+      <c r="E944" t="s">
+        <v>14</v>
+      </c>
+      <c r="F944" s="8">
+        <v>1986.3</v>
+      </c>
+    </row>
+    <row r="945" spans="1:7">
+      <c r="A945" s="1">
+        <v>42311</v>
+      </c>
+      <c r="B945" s="5">
+        <v>0.96319444444444446</v>
+      </c>
+      <c r="D945">
+        <v>10</v>
+      </c>
+      <c r="E945" t="s">
+        <v>46</v>
+      </c>
+      <c r="F945" s="8"/>
+      <c r="G945" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="946" spans="1:7">
+      <c r="A946" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B946" s="5"/>
+      <c r="D946" s="5"/>
+      <c r="E946" t="s">
+        <v>1</v>
+      </c>
+      <c r="F946" s="8">
+        <v>1954.6</v>
+      </c>
+    </row>
+    <row r="947" spans="1:7">
+      <c r="A947" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B947" s="5"/>
+      <c r="D947" s="5"/>
+      <c r="E947" t="s">
+        <v>2</v>
+      </c>
+      <c r="F947" s="8">
+        <v>2167.6</v>
+      </c>
+    </row>
+    <row r="948" spans="1:7">
+      <c r="A948" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B948" s="5"/>
+      <c r="D948" s="5"/>
+      <c r="E948" t="s">
+        <v>3</v>
+      </c>
+      <c r="F948" s="8">
+        <v>1421.1</v>
+      </c>
+    </row>
+    <row r="949" spans="1:7">
+      <c r="A949" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B949" s="5"/>
+      <c r="D949" s="5"/>
+      <c r="E949" t="s">
+        <v>4</v>
+      </c>
+      <c r="F949" s="8">
+        <v>1836.3</v>
+      </c>
+    </row>
+    <row r="950" spans="1:7">
+      <c r="A950" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B950" s="5"/>
+      <c r="D950" s="5"/>
+      <c r="E950" t="s">
+        <v>6</v>
+      </c>
+      <c r="F950" s="8">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="951" spans="1:7">
+      <c r="A951" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B951" s="5"/>
+      <c r="D951" s="5"/>
+      <c r="E951" t="s">
+        <v>7</v>
+      </c>
+      <c r="F951" s="8">
+        <v>2008.2</v>
+      </c>
+    </row>
+    <row r="952" spans="1:7">
+      <c r="A952" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B952" s="5"/>
+      <c r="D952" s="5"/>
+      <c r="E952" t="s">
+        <v>9</v>
+      </c>
+      <c r="F952" s="8">
+        <v>1903.4</v>
+      </c>
+    </row>
+    <row r="953" spans="1:7">
+      <c r="A953" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B953" s="5"/>
+      <c r="D953" s="5"/>
+      <c r="E953" t="s">
+        <v>11</v>
+      </c>
+      <c r="F953" s="8">
+        <v>1692.4</v>
+      </c>
+    </row>
+    <row r="954" spans="1:7">
+      <c r="A954" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B954" s="5"/>
+      <c r="D954" s="5"/>
+      <c r="E954" t="s">
+        <v>13</v>
+      </c>
+      <c r="F954" s="8">
+        <v>1627.3</v>
+      </c>
+    </row>
+    <row r="955" spans="1:7">
+      <c r="A955" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B955" s="5"/>
+      <c r="D955" s="5"/>
+      <c r="E955" t="s">
+        <v>15</v>
+      </c>
+      <c r="F955" s="8">
+        <v>2102.4</v>
+      </c>
+    </row>
+    <row r="956" spans="1:7">
+      <c r="A956" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B956" s="5"/>
+      <c r="D956" s="5"/>
+      <c r="E956" t="s">
+        <v>16</v>
+      </c>
+      <c r="F956" s="8">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="957" spans="1:7">
+      <c r="A957" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B957" s="5"/>
+      <c r="D957" s="5"/>
+      <c r="E957" t="s">
+        <v>17</v>
+      </c>
+      <c r="F957" s="8">
+        <v>1630.4</v>
+      </c>
+    </row>
+    <row r="958" spans="1:7">
+      <c r="A958" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B958" s="5"/>
+      <c r="D958" s="5"/>
+      <c r="E958" t="s">
+        <v>18</v>
+      </c>
+      <c r="F958" s="8">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="959" spans="1:7">
+      <c r="A959" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B959" s="5"/>
+      <c r="D959" s="5"/>
+      <c r="E959" t="s">
+        <v>19</v>
+      </c>
+      <c r="F959" s="8">
+        <v>1914.6</v>
+      </c>
+    </row>
+    <row r="960" spans="1:7">
+      <c r="A960" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B960" s="5"/>
+      <c r="D960" s="5"/>
+      <c r="E960" t="s">
+        <v>20</v>
+      </c>
+      <c r="F960" s="8">
+        <v>2133.9</v>
+      </c>
+    </row>
+    <row r="961" spans="1:6">
+      <c r="A961" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B961" s="5"/>
+      <c r="D961" s="5"/>
+      <c r="E961" t="s">
+        <v>21</v>
+      </c>
+      <c r="F961" s="8">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="962" spans="1:6">
+      <c r="A962" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B962" s="5"/>
+      <c r="D962" s="5"/>
+      <c r="E962" t="s">
+        <v>22</v>
+      </c>
+      <c r="F962" s="8">
+        <v>2168.1</v>
+      </c>
+    </row>
+    <row r="963" spans="1:6">
+      <c r="A963" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B963" s="5"/>
+      <c r="D963" s="5"/>
+      <c r="E963" t="s">
+        <v>23</v>
+      </c>
+      <c r="F963" s="8">
+        <v>1655.4</v>
+      </c>
+    </row>
+    <row r="964" spans="1:6">
+      <c r="A964" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B964" s="5"/>
+      <c r="D964" s="5"/>
+      <c r="E964" t="s">
+        <v>25</v>
+      </c>
+      <c r="F964" s="8">
+        <v>2015.2</v>
+      </c>
+    </row>
+    <row r="965" spans="1:6">
+      <c r="A965" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B965" s="5"/>
+      <c r="D965" s="5"/>
+      <c r="E965" t="s">
+        <v>26</v>
+      </c>
+      <c r="F965" s="8">
+        <v>1899.7</v>
+      </c>
+    </row>
+    <row r="966" spans="1:6">
+      <c r="A966" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B966" s="5"/>
+      <c r="D966" s="5"/>
+      <c r="E966" t="s">
+        <v>27</v>
+      </c>
+      <c r="F966" s="8">
+        <v>1867.7</v>
+      </c>
+    </row>
+    <row r="967" spans="1:6">
+      <c r="A967" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B967" s="5"/>
+      <c r="D967" s="5"/>
+      <c r="E967" t="s">
+        <v>28</v>
+      </c>
+      <c r="F967" s="8">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="968" spans="1:6">
+      <c r="A968" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B968" s="5"/>
+      <c r="D968" s="5"/>
+      <c r="E968" t="s">
+        <v>29</v>
+      </c>
+      <c r="F968" s="8">
+        <v>2082.8000000000002</v>
+      </c>
+    </row>
+    <row r="969" spans="1:6">
+      <c r="A969" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B969" s="5"/>
+      <c r="D969" s="5"/>
+      <c r="E969" t="s">
+        <v>30</v>
+      </c>
+      <c r="F969" s="8">
+        <v>1543.9</v>
+      </c>
+    </row>
+    <row r="970" spans="1:6">
+      <c r="A970" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B970" s="5"/>
+      <c r="D970" s="5"/>
+      <c r="E970" t="s">
+        <v>5</v>
+      </c>
+      <c r="F970" s="8">
+        <v>1578.5</v>
+      </c>
+    </row>
+    <row r="971" spans="1:6">
+      <c r="A971" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B971" s="5"/>
+      <c r="D971" s="5"/>
+      <c r="E971" t="s">
+        <v>24</v>
+      </c>
+      <c r="F971" s="8">
+        <v>1892.8</v>
+      </c>
+    </row>
+    <row r="972" spans="1:6">
+      <c r="A972" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B972" s="5"/>
+      <c r="D972" s="5"/>
+      <c r="E972" t="s">
+        <v>8</v>
+      </c>
+      <c r="F972" s="8">
+        <v>1270.9000000000001</v>
+      </c>
+    </row>
+    <row r="973" spans="1:6">
+      <c r="A973" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B973" s="5"/>
+      <c r="D973" s="5"/>
+      <c r="E973" t="s">
+        <v>10</v>
+      </c>
+      <c r="F973" s="8">
+        <v>2022.6</v>
+      </c>
+    </row>
+    <row r="974" spans="1:6">
+      <c r="A974" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B974" s="5"/>
+      <c r="D974" s="5"/>
+      <c r="E974" t="s">
+        <v>12</v>
+      </c>
+      <c r="F974" s="8">
+        <v>1716.1</v>
+      </c>
+    </row>
+    <row r="975" spans="1:6">
+      <c r="A975" s="1">
+        <v>42317</v>
+      </c>
+      <c r="B975" s="5"/>
+      <c r="D975" s="5"/>
+      <c r="E975" t="s">
+        <v>14</v>
+      </c>
+      <c r="F975" s="8">
+        <v>1982.9</v>
+      </c>
+    </row>
+    <row r="976" spans="1:6">
+      <c r="A976" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B976" s="5">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="D976">
+        <v>10</v>
+      </c>
+      <c r="E976" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="977" spans="1:7">
+      <c r="A977" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B977" s="5">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="D977">
+        <v>6</v>
+      </c>
+      <c r="E977" t="s">
+        <v>5</v>
+      </c>
+      <c r="F977" s="8">
+        <v>1584.6</v>
+      </c>
+    </row>
+    <row r="978" spans="1:7">
+      <c r="A978" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B978" s="5">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="D978">
+        <v>16</v>
+      </c>
+      <c r="E978" t="s">
+        <v>24</v>
+      </c>
+      <c r="F978" s="8">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="979" spans="1:7">
+      <c r="A979" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B979" s="5">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="D979">
+        <v>13</v>
+      </c>
+      <c r="E979" t="s">
+        <v>8</v>
+      </c>
+      <c r="F979" s="8">
+        <v>1270.8</v>
+      </c>
+    </row>
+    <row r="980" spans="1:7">
+      <c r="A980" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B980" s="5">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="D980">
+        <v>14</v>
+      </c>
+      <c r="E980" t="s">
+        <v>10</v>
+      </c>
+      <c r="F980" s="8">
+        <v>2024.5</v>
+      </c>
+    </row>
+    <row r="981" spans="1:7">
+      <c r="A981" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B981" s="5">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="D981">
+        <v>11</v>
+      </c>
+      <c r="E981" t="s">
+        <v>12</v>
+      </c>
+      <c r="F981" s="8">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="982" spans="1:7">
+      <c r="A982" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B982" s="5">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="D982">
+        <v>1</v>
+      </c>
+      <c r="E982" t="s">
+        <v>14</v>
+      </c>
+      <c r="F982" s="8">
+        <v>1981.3</v>
+      </c>
+    </row>
+    <row r="983" spans="1:7">
+      <c r="A983" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B983" s="5">
+        <v>0.80486111111111114</v>
+      </c>
+      <c r="D983">
+        <v>10</v>
+      </c>
+      <c r="E983" t="s">
+        <v>46</v>
+      </c>
+      <c r="F983" s="8"/>
+    </row>
+    <row r="984" spans="1:7">
+      <c r="A984" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B984" s="5">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="D984" s="14">
+        <v>4</v>
+      </c>
+      <c r="E984" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F984" s="15">
+        <v>2025.2</v>
+      </c>
+      <c r="G984" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="985" spans="1:7">
+      <c r="A985" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B985" s="5">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="D985" s="14">
+        <v>2</v>
+      </c>
+      <c r="E985" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F985" s="15">
+        <v>1906.4</v>
+      </c>
+      <c r="G985" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="986" spans="1:7">
+      <c r="A986" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B986" s="5">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="D986" s="14">
+        <v>12</v>
+      </c>
+      <c r="E986" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F986" s="15">
+        <v>1867.7</v>
+      </c>
+      <c r="G986" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="987" spans="1:7">
+      <c r="A987" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B987" s="5">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="D987" s="14">
+        <v>8</v>
+      </c>
+      <c r="E987" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F987" s="15">
+        <v>1960.5</v>
+      </c>
+      <c r="G987" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="988" spans="1:7">
+      <c r="A988" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B988" s="5">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="D988" s="14">
+        <v>5</v>
+      </c>
+      <c r="E988" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F988" s="15">
+        <v>2083.6999999999998</v>
+      </c>
+      <c r="G988" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="989" spans="1:7">
+      <c r="A989" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B989" s="5">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="D989" s="14">
+        <v>9</v>
+      </c>
+      <c r="E989" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F989" s="15">
+        <v>1548.9</v>
+      </c>
+      <c r="G989" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="990" spans="1:7">
+      <c r="A990" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B990" s="5">
+        <v>0.85972222222222217</v>
+      </c>
+      <c r="D990">
+        <v>10</v>
+      </c>
+      <c r="E990" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="991" spans="1:7">
+      <c r="A991" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B991" s="5">
+        <v>0.86388888888888893</v>
+      </c>
+      <c r="D991">
+        <v>6</v>
+      </c>
+      <c r="E991" t="s">
+        <v>25</v>
+      </c>
+      <c r="F991" s="8">
+        <v>2025.2</v>
+      </c>
+      <c r="G991" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="992" spans="1:7">
+      <c r="A992" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B992" s="5">
+        <v>0.86388888888888893</v>
+      </c>
+      <c r="D992">
+        <v>16</v>
+      </c>
+      <c r="E992" t="s">
+        <v>26</v>
+      </c>
+      <c r="F992" s="8">
+        <v>1906.4</v>
+      </c>
+      <c r="G992" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="993" spans="1:7">
+      <c r="A993" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B993" s="5">
+        <v>0.86388888888888893</v>
+      </c>
+      <c r="D993">
+        <v>13</v>
+      </c>
+      <c r="E993" t="s">
+        <v>27</v>
+      </c>
+      <c r="F993" s="8">
+        <v>1867.7</v>
+      </c>
+      <c r="G993" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="994" spans="1:7">
+      <c r="A994" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B994" s="5">
+        <v>0.86388888888888893</v>
+      </c>
+      <c r="D994">
+        <v>14</v>
+      </c>
+      <c r="E994" t="s">
+        <v>28</v>
+      </c>
+      <c r="F994" s="8">
+        <v>1960.5</v>
+      </c>
+      <c r="G994" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="995" spans="1:7">
+      <c r="A995" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B995" s="5">
+        <v>0.86388888888888893</v>
+      </c>
+      <c r="D995">
+        <v>11</v>
+      </c>
+      <c r="E995" t="s">
+        <v>29</v>
+      </c>
+      <c r="F995" s="8">
+        <v>2083.6999999999998</v>
+      </c>
+      <c r="G995" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="996" spans="1:7">
+      <c r="A996" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B996" s="5">
+        <v>0.86388888888888893</v>
+      </c>
+      <c r="D996">
+        <v>1</v>
+      </c>
+      <c r="E996" t="s">
+        <v>30</v>
+      </c>
+      <c r="F996" s="8">
+        <v>1548.9</v>
+      </c>
+      <c r="G996" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="997" spans="1:7">
+      <c r="A997" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B997" s="5">
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="D997">
+        <v>10</v>
+      </c>
+      <c r="E997" t="s">
+        <v>47</v>
+      </c>
+      <c r="F997" s="16"/>
+    </row>
+    <row r="998" spans="1:7">
+      <c r="A998" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B998" s="5">
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="D998">
+        <v>6</v>
+      </c>
+      <c r="E998" t="s">
+        <v>1</v>
+      </c>
+      <c r="F998" s="8">
+        <v>1954.2</v>
+      </c>
+    </row>
+    <row r="999" spans="1:7">
+      <c r="A999" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B999" s="5">
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="D999">
+        <v>16</v>
+      </c>
+      <c r="E999" t="s">
+        <v>2</v>
+      </c>
+      <c r="F999" s="8">
+        <v>2166.6999999999998</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:7">
+      <c r="A1000" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B1000" s="5">
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="D1000">
+        <v>13</v>
+      </c>
+      <c r="E1000" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1000" s="8">
+        <v>1415.2</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:7">
+      <c r="A1001" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B1001" s="5">
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="D1001">
+        <v>14</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1001" s="8">
+        <v>1836.2</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:7">
+      <c r="A1002" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B1002" s="5">
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="D1002">
+        <v>11</v>
+      </c>
+      <c r="E1002" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1002" s="8">
+        <v>1846.4</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:7">
+      <c r="A1003" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B1003" s="5">
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="D1003">
+        <v>1</v>
+      </c>
+      <c r="E1003" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1003" s="8">
+        <v>2005.4</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:7">
+      <c r="A1004" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B1004" s="5">
+        <v>0.98333333333333339</v>
+      </c>
+      <c r="D1004">
+        <v>10</v>
+      </c>
+      <c r="E1004" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:7">
+      <c r="A1005" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B1005" s="5">
+        <v>0.9902777777777777</v>
+      </c>
+      <c r="D1005">
+        <v>4</v>
+      </c>
+      <c r="E1005" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1005" s="8">
+        <v>1914.5</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:7">
+      <c r="A1006" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B1006" s="5">
+        <v>0.9902777777777777</v>
+      </c>
+      <c r="D1006">
+        <v>2</v>
+      </c>
+      <c r="E1006" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1006" s="8">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:7">
+      <c r="A1007" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B1007" s="5">
+        <v>0.9902777777777777</v>
+      </c>
+      <c r="D1007">
+        <v>12</v>
+      </c>
+      <c r="E1007" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1007" s="8">
+        <v>1638.7</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:7">
+      <c r="A1008" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B1008" s="5">
+        <v>0.9902777777777777</v>
+      </c>
+      <c r="D1008">
+        <v>8</v>
+      </c>
+      <c r="E1008" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1008" s="8">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:6">
+      <c r="A1009" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B1009" s="5">
+        <v>0.9902777777777777</v>
+      </c>
+      <c r="D1009">
+        <v>5</v>
+      </c>
+      <c r="E1009" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1009" s="8">
+        <v>1653.9</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:6">
+      <c r="A1010" s="1">
+        <v>42319</v>
+      </c>
+      <c r="B1010" s="5">
+        <v>0.9902777777777777</v>
+      </c>
+      <c r="D1010">
+        <v>9</v>
+      </c>
+      <c r="E1010" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1010" s="8">
+        <v>1632.8</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:6">
+      <c r="A1011" s="1">
+        <v>42320</v>
+      </c>
+      <c r="B1011" s="5">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="D1011">
+        <v>10</v>
+      </c>
+      <c r="E1011" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:6">
+      <c r="A1012" s="1">
+        <v>42320</v>
+      </c>
+      <c r="B1012" s="5">
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="D1012">
+        <v>6</v>
+      </c>
+      <c r="E1012" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1012" s="8">
+        <v>1534.6</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:6">
+      <c r="A1013" s="1">
+        <v>42320</v>
+      </c>
+      <c r="B1013" s="5">
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="D1013">
+        <v>16</v>
+      </c>
+      <c r="E1013" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1013" s="8">
+        <v>1911.8</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:6">
+      <c r="A1014" s="1">
+        <v>42320</v>
+      </c>
+      <c r="B1014" s="5">
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="D1014">
+        <v>13</v>
+      </c>
+      <c r="E1014" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1014" s="8">
+        <v>2133</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:6">
+      <c r="A1015" s="1">
+        <v>42320</v>
+      </c>
+      <c r="B1015" s="5">
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="D1015">
+        <v>14</v>
+      </c>
+      <c r="E1015" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1015" s="8">
+        <v>1421.2</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:6">
+      <c r="A1016" s="1">
+        <v>42320</v>
+      </c>
+      <c r="B1016" s="5">
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="D1016">
+        <v>11</v>
+      </c>
+      <c r="E1016" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1016" s="8">
+        <v>2165.6999999999998</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:6">
+      <c r="A1017" s="1">
+        <v>42320</v>
+      </c>
+      <c r="B1017" s="5">
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="D1017">
+        <v>1</v>
+      </c>
+      <c r="E1017" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1017" s="8">
+        <v>1666.6</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:6">
+      <c r="D1018" s="2"/>
+    </row>
+    <row r="1019" spans="1:6">
+      <c r="D1019" s="2"/>
+    </row>
+    <row r="1020" spans="1:6">
+      <c r="D1020" s="2"/>
+    </row>
+    <row r="1021" spans="1:6">
+      <c r="D1021" s="2"/>
+    </row>
+    <row r="1022" spans="1:6">
+      <c r="D1022" s="2"/>
+    </row>
+    <row r="1023" spans="1:6">
+      <c r="D1023" s="2"/>
+    </row>
+    <row r="1024" spans="1:6">
+      <c r="D1024" s="2"/>
+    </row>
+    <row r="1025" spans="4:4">
+      <c r="D1025" s="2"/>
+    </row>
+    <row r="1026" spans="4:4">
+      <c r="D1026" s="2"/>
+    </row>
+    <row r="1027" spans="4:4">
+      <c r="D1027" s="2"/>
+    </row>
+    <row r="1028" spans="4:4">
+      <c r="D1028" s="2"/>
+    </row>
+    <row r="1029" spans="4:4">
+      <c r="D1029" s="2"/>
+    </row>
+    <row r="1030" spans="4:4">
+      <c r="D1030" s="2"/>
+    </row>
+    <row r="1031" spans="4:4">
+      <c r="D1031" s="2"/>
+    </row>
+    <row r="1032" spans="4:4">
+      <c r="D1032" s="2"/>
+    </row>
+    <row r="1033" spans="4:4">
+      <c r="D1033" s="2"/>
+    </row>
+    <row r="1034" spans="4:4">
+      <c r="D1034" s="2"/>
+    </row>
+    <row r="1035" spans="4:4">
+      <c r="D1035" s="2"/>
+    </row>
+    <row r="1036" spans="4:4">
+      <c r="D1036" s="2"/>
+    </row>
+    <row r="1037" spans="4:4">
+      <c r="D1037" s="2"/>
+    </row>
+    <row r="1038" spans="4:4">
+      <c r="D1038" s="2"/>
+    </row>
+    <row r="1039" spans="4:4">
+      <c r="D1039" s="2"/>
+    </row>
+    <row r="1040" spans="4:4">
+      <c r="D1040" s="2"/>
+    </row>
+    <row r="1041" spans="4:4">
+      <c r="D1041" s="2"/>
+    </row>
+    <row r="1042" spans="4:4">
+      <c r="D1042" s="2"/>
+    </row>
+    <row r="1043" spans="4:4">
+      <c r="D1043" s="2"/>
+    </row>
+    <row r="1044" spans="4:4">
+      <c r="D1044" s="2"/>
+    </row>
+    <row r="1045" spans="4:4">
+      <c r="D1045" s="2"/>
+    </row>
+    <row r="1046" spans="4:4">
+      <c r="D1046" s="2"/>
+    </row>
+    <row r="1047" spans="4:4">
+      <c r="D1047" s="2"/>
+    </row>
+    <row r="1048" spans="4:4">
+      <c r="D1048" s="2"/>
+    </row>
+    <row r="1049" spans="4:4">
+      <c r="D1049" s="2"/>
+    </row>
+    <row r="1050" spans="4:4">
+      <c r="D1050" s="2"/>
+    </row>
+    <row r="1051" spans="4:4">
+      <c r="D1051" s="2"/>
+    </row>
+    <row r="1052" spans="4:4">
+      <c r="D1052" s="2"/>
+    </row>
+    <row r="1053" spans="4:4">
+      <c r="D1053" s="2"/>
+    </row>
+    <row r="1054" spans="4:4">
+      <c r="D1054" s="2"/>
+    </row>
+    <row r="1055" spans="4:4">
+      <c r="D1055" s="2"/>
+    </row>
+    <row r="1056" spans="4:4">
+      <c r="D1056" s="2"/>
+    </row>
+    <row r="1057" spans="4:4">
+      <c r="D1057" s="2"/>
+    </row>
+    <row r="1058" spans="4:4">
+      <c r="D1058" s="2"/>
+    </row>
+    <row r="1059" spans="4:4">
+      <c r="D1059" s="2"/>
+    </row>
+    <row r="1060" spans="4:4">
+      <c r="D1060" s="2"/>
+    </row>
+    <row r="1061" spans="4:4">
+      <c r="D1061" s="2"/>
+    </row>
+    <row r="1062" spans="4:4">
+      <c r="D1062" s="2"/>
+    </row>
+    <row r="1063" spans="4:4">
+      <c r="D1063" s="2"/>
+    </row>
+    <row r="1064" spans="4:4">
+      <c r="D1064" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A3:G448">

</xml_diff>

<commit_message>
Calculate headspace correct using soil volume
Per @apeyton comment in issue #27 - we now calculate headspace in each
core based on soil volume (which has been renamed for clarity).
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="24400" windowHeight="15360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="treatments.csv" sheetId="2" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>NOTE: this sheet gets updated each time</t>
   </si>
   <si>
-    <t>Volume</t>
-  </si>
-  <si>
     <t>Time_set_start_UTC</t>
   </si>
   <si>
@@ -257,6 +254,9 @@
   </si>
   <si>
     <t>new port valves</t>
+  </si>
+  <si>
+    <t>SoilVolume_cm3</t>
   </si>
 </sst>
 </file>
@@ -1211,9 +1211,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1234,12 +1234,12 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>40</v>
@@ -1694,7 +1694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1215"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A1195" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A1216" sqref="A1216"/>
     </sheetView>
@@ -1715,7 +1715,7 @@
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>37</v>
@@ -1747,7 +1747,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1884,7 +1884,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2021,7 +2021,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2158,7 +2158,7 @@
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2295,7 +2295,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2432,7 +2432,7 @@
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2569,7 +2569,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -2706,7 +2706,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2843,7 +2843,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2980,7 +2980,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3117,7 +3117,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -3254,7 +3254,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -3391,7 +3391,7 @@
         <v>10</v>
       </c>
       <c r="E87" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -3528,7 +3528,7 @@
         <v>10</v>
       </c>
       <c r="E94" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3665,7 +3665,7 @@
         <v>10</v>
       </c>
       <c r="E101" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -3802,7 +3802,7 @@
         <v>10</v>
       </c>
       <c r="E108" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -3939,7 +3939,7 @@
         <v>10</v>
       </c>
       <c r="E115" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -4076,7 +4076,7 @@
         <v>10</v>
       </c>
       <c r="E122" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -4213,7 +4213,7 @@
         <v>10</v>
       </c>
       <c r="E129" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -4350,7 +4350,7 @@
         <v>10</v>
       </c>
       <c r="E136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -4874,7 +4874,7 @@
         <v>10</v>
       </c>
       <c r="E173" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -4990,7 +4990,7 @@
         <v>10</v>
       </c>
       <c r="E180" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="181" spans="1:6">
@@ -5106,7 +5106,7 @@
         <v>10</v>
       </c>
       <c r="E187" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -5222,7 +5222,7 @@
         <v>10</v>
       </c>
       <c r="E194" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="195" spans="1:6">
@@ -5338,7 +5338,7 @@
         <v>10</v>
       </c>
       <c r="E201" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="202" spans="1:6">
@@ -5454,7 +5454,7 @@
         <v>10</v>
       </c>
       <c r="E208" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="209" spans="1:7">
@@ -5468,10 +5468,10 @@
         <v>10</v>
       </c>
       <c r="E209" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G209" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="210" spans="1:7">
@@ -5875,7 +5875,7 @@
         <v>10</v>
       </c>
       <c r="E240" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="241" spans="1:6">
@@ -5991,7 +5991,7 @@
         <v>10</v>
       </c>
       <c r="E247" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="248" spans="1:6">
@@ -6107,7 +6107,7 @@
         <v>10</v>
       </c>
       <c r="E254" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="255" spans="1:6">
@@ -6223,7 +6223,7 @@
         <v>10</v>
       </c>
       <c r="E261" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="262" spans="1:7">
@@ -6243,7 +6243,7 @@
         <v>2103.5</v>
       </c>
       <c r="G262" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -6263,7 +6263,7 @@
         <v>1999.2</v>
       </c>
       <c r="G263" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -6283,7 +6283,7 @@
         <v>1967.3</v>
       </c>
       <c r="G264" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -6303,7 +6303,7 @@
         <v>2034.7</v>
       </c>
       <c r="G265" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -6323,7 +6323,7 @@
         <v>2158.3000000000002</v>
       </c>
       <c r="G266" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -6343,7 +6343,7 @@
         <v>1659.2</v>
       </c>
       <c r="G267" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="268" spans="1:7">
@@ -6357,7 +6357,7 @@
         <v>10</v>
       </c>
       <c r="E268" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="269" spans="1:7">
@@ -6473,7 +6473,7 @@
         <v>10</v>
       </c>
       <c r="E275" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="276" spans="1:6">
@@ -6877,7 +6877,7 @@
         <v>10</v>
       </c>
       <c r="E306" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="307" spans="1:6">
@@ -6993,7 +6993,7 @@
         <v>10</v>
       </c>
       <c r="E313" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="314" spans="1:6">
@@ -7109,7 +7109,7 @@
         <v>10</v>
       </c>
       <c r="E320" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="321" spans="1:6">
@@ -7225,7 +7225,7 @@
         <v>10</v>
       </c>
       <c r="E327" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="328" spans="1:6">
@@ -7341,7 +7341,7 @@
         <v>10</v>
       </c>
       <c r="E334" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="335" spans="1:6">
@@ -7457,7 +7457,7 @@
         <v>10</v>
       </c>
       <c r="E341" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="342" spans="1:7">
@@ -7573,7 +7573,7 @@
         <v>10</v>
       </c>
       <c r="E348" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="349" spans="1:7">
@@ -7593,7 +7593,7 @@
         <v>1921.4</v>
       </c>
       <c r="G349" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="350" spans="1:7">
@@ -7613,7 +7613,7 @@
         <v>1711.5</v>
       </c>
       <c r="G350" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="351" spans="1:7">
@@ -7633,7 +7633,7 @@
         <v>1699</v>
       </c>
       <c r="G351" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="352" spans="1:7">
@@ -7653,7 +7653,7 @@
         <v>2146.8000000000002</v>
       </c>
       <c r="G352" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="353" spans="1:7">
@@ -7673,7 +7673,7 @@
         <v>1661.6</v>
       </c>
       <c r="G353" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="354" spans="1:7">
@@ -7693,7 +7693,7 @@
         <v>1703.8</v>
       </c>
       <c r="G354" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="355" spans="1:7">
@@ -7707,7 +7707,7 @@
         <v>10</v>
       </c>
       <c r="E355" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="356" spans="1:7">
@@ -7823,7 +7823,7 @@
         <v>10</v>
       </c>
       <c r="E362" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="363" spans="1:7">
@@ -7939,7 +7939,7 @@
         <v>10</v>
       </c>
       <c r="E369" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="370" spans="1:7">
@@ -8055,7 +8055,7 @@
         <v>10</v>
       </c>
       <c r="E376" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="377" spans="1:7">
@@ -8071,7 +8071,7 @@
         <v>1962.9</v>
       </c>
       <c r="G377" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="378" spans="1:7">
@@ -8087,7 +8087,7 @@
         <v>2173.1</v>
       </c>
       <c r="G378" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="379" spans="1:7">
@@ -8103,7 +8103,7 @@
         <v>1441.9</v>
       </c>
       <c r="G379" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="380" spans="1:7">
@@ -8119,7 +8119,7 @@
         <v>1843.5</v>
       </c>
       <c r="G380" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="381" spans="1:7">
@@ -8135,7 +8135,7 @@
         <v>1853.6</v>
       </c>
       <c r="G381" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="382" spans="1:7">
@@ -8151,7 +8151,7 @@
         <v>2016.2</v>
       </c>
       <c r="G382" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="383" spans="1:7">
@@ -8167,7 +8167,7 @@
         <v>1908.3</v>
       </c>
       <c r="G383" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="384" spans="1:7">
@@ -8183,7 +8183,7 @@
         <v>1698.8</v>
       </c>
       <c r="G384" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="385" spans="1:7">
@@ -8225,7 +8225,7 @@
         <v>1648</v>
       </c>
       <c r="G387" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="388" spans="1:7">
@@ -8254,7 +8254,7 @@
         <v>1580.9</v>
       </c>
       <c r="G389" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="390" spans="1:7">
@@ -8270,7 +8270,7 @@
         <v>1974.9</v>
       </c>
       <c r="G390" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="391" spans="1:7">
@@ -8286,7 +8286,7 @@
         <v>2171.3000000000002</v>
       </c>
       <c r="G391" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="392" spans="1:7">
@@ -8302,7 +8302,7 @@
         <v>1421</v>
       </c>
       <c r="G392" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="393" spans="1:7">
@@ -8318,7 +8318,7 @@
         <v>2196.4</v>
       </c>
       <c r="G393" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="394" spans="1:7">
@@ -8334,7 +8334,7 @@
         <v>1678.7</v>
       </c>
       <c r="G394" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="395" spans="1:7">
@@ -8428,7 +8428,7 @@
         <v>1611.8</v>
       </c>
       <c r="G401" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="402" spans="1:7">
@@ -8444,7 +8444,7 @@
         <v>1903.3</v>
       </c>
       <c r="G402" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="403" spans="1:7">
@@ -8460,7 +8460,7 @@
         <v>1286.8</v>
       </c>
       <c r="G403" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="404" spans="1:7">
@@ -8476,7 +8476,7 @@
         <v>2041.3</v>
       </c>
       <c r="G404" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="405" spans="1:7">
@@ -8505,7 +8505,7 @@
         <v>2012.2</v>
       </c>
       <c r="G406" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="407" spans="1:7">
@@ -8519,7 +8519,7 @@
         <v>10</v>
       </c>
       <c r="E407" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="408" spans="1:7">
@@ -8556,7 +8556,7 @@
         <v>2180.4</v>
       </c>
       <c r="G409" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="410" spans="1:7">
@@ -8576,7 +8576,7 @@
         <v>1443.3</v>
       </c>
       <c r="G410" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="411" spans="1:7">
@@ -8641,7 +8641,7 @@
         <v>10</v>
       </c>
       <c r="E414" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="415" spans="1:7">
@@ -8757,7 +8757,7 @@
         <v>10</v>
       </c>
       <c r="E421" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="422" spans="1:7">
@@ -8777,7 +8777,7 @@
         <v>1973.3</v>
       </c>
       <c r="G422" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="423" spans="1:7">
@@ -8797,7 +8797,7 @@
         <v>2180.4</v>
       </c>
       <c r="G423" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="424" spans="1:7">
@@ -8817,7 +8817,7 @@
         <v>1443.3</v>
       </c>
       <c r="G424" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="425" spans="1:7">
@@ -8837,7 +8837,7 @@
         <v>1851</v>
       </c>
       <c r="G425" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="426" spans="1:7">
@@ -8857,7 +8857,7 @@
         <v>1862.9</v>
       </c>
       <c r="G426" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="427" spans="1:7">
@@ -8877,7 +8877,7 @@
         <v>2026.8</v>
       </c>
       <c r="G427" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="428" spans="1:7">
@@ -8891,7 +8891,7 @@
         <v>10</v>
       </c>
       <c r="E428" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="429" spans="1:7">
@@ -8911,7 +8911,7 @@
         <v>1585.9</v>
       </c>
       <c r="G429" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="430" spans="1:7">
@@ -8931,7 +8931,7 @@
         <v>1986.5</v>
       </c>
       <c r="G430" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="431" spans="1:7">
@@ -8951,7 +8951,7 @@
         <v>2209.4</v>
       </c>
       <c r="G431" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="432" spans="1:7">
@@ -8971,7 +8971,7 @@
         <v>1453.3</v>
       </c>
       <c r="G432" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="433" spans="1:7">
@@ -8991,7 +8991,7 @@
         <v>2216.5</v>
       </c>
       <c r="G433" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="434" spans="1:7">
@@ -9011,7 +9011,7 @@
         <v>1703.3</v>
       </c>
       <c r="G434" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="435" spans="1:7">
@@ -9025,7 +9025,7 @@
         <v>10</v>
       </c>
       <c r="E435" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="436" spans="1:7">
@@ -9079,7 +9079,7 @@
         <v>1292.5999999999999</v>
       </c>
       <c r="G438" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="439" spans="1:7">
@@ -9116,7 +9116,7 @@
         <v>1727</v>
       </c>
       <c r="G440" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="441" spans="1:7">
@@ -9136,7 +9136,7 @@
         <v>2042.8</v>
       </c>
       <c r="G441" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="442" spans="1:7">
@@ -9150,7 +9150,7 @@
         <v>10</v>
       </c>
       <c r="E442" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="443" spans="1:7">
@@ -9266,7 +9266,7 @@
         <v>10</v>
       </c>
       <c r="E449" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="450" spans="1:6">
@@ -9772,7 +9772,7 @@
         <v>10</v>
       </c>
       <c r="E486" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F486" s="8"/>
     </row>
@@ -9889,7 +9889,7 @@
         <v>10</v>
       </c>
       <c r="E493" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F493" s="8"/>
     </row>
@@ -10006,7 +10006,7 @@
         <v>10</v>
       </c>
       <c r="E500" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F500" s="8"/>
     </row>
@@ -10123,7 +10123,7 @@
         <v>10</v>
       </c>
       <c r="E507" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F507" s="8"/>
     </row>
@@ -10240,7 +10240,7 @@
         <v>10</v>
       </c>
       <c r="E514" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F514" s="8"/>
     </row>
@@ -10645,11 +10645,11 @@
         <v>10</v>
       </c>
       <c r="E545" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F545" s="8"/>
       <c r="G545" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="546" spans="1:7">
@@ -10765,7 +10765,7 @@
         <v>10</v>
       </c>
       <c r="E552" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F552" s="8"/>
     </row>
@@ -10882,7 +10882,7 @@
         <v>10</v>
       </c>
       <c r="E559" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F559" s="8"/>
     </row>
@@ -10999,7 +10999,7 @@
         <v>10</v>
       </c>
       <c r="E566" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F566" s="8"/>
     </row>
@@ -11116,7 +11116,7 @@
         <v>10</v>
       </c>
       <c r="E573" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F573" s="8"/>
     </row>
@@ -11233,7 +11233,7 @@
         <v>10</v>
       </c>
       <c r="E580" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F580" s="8"/>
     </row>
@@ -11350,7 +11350,7 @@
         <v>10</v>
       </c>
       <c r="E587" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="588" spans="1:6">
@@ -11466,7 +11466,7 @@
         <v>10</v>
       </c>
       <c r="E594" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F594" s="8"/>
     </row>
@@ -11583,7 +11583,7 @@
         <v>10</v>
       </c>
       <c r="E601" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="602" spans="1:6">
@@ -11699,7 +11699,7 @@
         <v>10</v>
       </c>
       <c r="E608" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F608" s="8"/>
     </row>
@@ -11816,7 +11816,7 @@
         <v>10</v>
       </c>
       <c r="E615" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F615" s="8"/>
     </row>
@@ -12221,7 +12221,7 @@
         <v>10</v>
       </c>
       <c r="E646" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F646" s="8"/>
     </row>
@@ -12338,7 +12338,7 @@
         <v>10</v>
       </c>
       <c r="E653" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F653" s="8"/>
     </row>
@@ -12455,7 +12455,7 @@
         <v>10</v>
       </c>
       <c r="E660" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="661" spans="1:6">
@@ -12571,7 +12571,7 @@
         <v>10</v>
       </c>
       <c r="E667" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F667" s="8"/>
     </row>
@@ -12688,7 +12688,7 @@
         <v>10</v>
       </c>
       <c r="E674" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F674" s="8"/>
     </row>
@@ -12805,7 +12805,7 @@
         <v>10</v>
       </c>
       <c r="E681" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F681" s="8"/>
     </row>
@@ -13312,7 +13312,7 @@
         <v>10</v>
       </c>
       <c r="E718" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F718" s="8"/>
     </row>
@@ -13429,7 +13429,7 @@
         <v>10</v>
       </c>
       <c r="E725" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F725" s="8"/>
     </row>
@@ -13546,7 +13546,7 @@
         <v>10</v>
       </c>
       <c r="E732" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F732" s="8"/>
     </row>
@@ -13561,11 +13561,11 @@
         <v>10</v>
       </c>
       <c r="E733" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F733" s="8"/>
       <c r="G733" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="734" spans="1:7">
@@ -13681,7 +13681,7 @@
         <v>10</v>
       </c>
       <c r="E740" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F740" s="8"/>
     </row>
@@ -14158,7 +14158,7 @@
         <v>10</v>
       </c>
       <c r="E777" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F777" s="8"/>
     </row>
@@ -14275,7 +14275,7 @@
         <v>10</v>
       </c>
       <c r="E784" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="785" spans="1:7">
@@ -14295,7 +14295,7 @@
         <v>1921.6</v>
       </c>
       <c r="G785" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="786" spans="1:7">
@@ -14315,7 +14315,7 @@
         <v>1703.7</v>
       </c>
       <c r="G786" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="787" spans="1:7">
@@ -14397,7 +14397,7 @@
         <v>10</v>
       </c>
       <c r="E791" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="792" spans="1:7">
@@ -14513,11 +14513,11 @@
         <v>10</v>
       </c>
       <c r="E798" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F798" s="8"/>
       <c r="G798" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="799" spans="1:7">
@@ -14531,11 +14531,11 @@
         <v>10</v>
       </c>
       <c r="E799" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F799" s="8"/>
       <c r="G799" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="800" spans="1:7">
@@ -14651,7 +14651,7 @@
         <v>10</v>
       </c>
       <c r="E806" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F806" s="8"/>
     </row>
@@ -14768,7 +14768,7 @@
         <v>10</v>
       </c>
       <c r="E813" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F813" s="8"/>
     </row>
@@ -15143,7 +15143,7 @@
         <v>10</v>
       </c>
       <c r="E844" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F844" s="8"/>
     </row>
@@ -15260,7 +15260,7 @@
         <v>10</v>
       </c>
       <c r="E851" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F851" s="8"/>
     </row>
@@ -15377,7 +15377,7 @@
         <v>10</v>
       </c>
       <c r="E858" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F858" s="8"/>
     </row>
@@ -15494,7 +15494,7 @@
         <v>10</v>
       </c>
       <c r="E865" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F865" s="8"/>
     </row>
@@ -15515,7 +15515,7 @@
         <v>2024.8</v>
       </c>
       <c r="G866" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="867" spans="1:7">
@@ -15535,7 +15535,7 @@
         <v>1911.54</v>
       </c>
       <c r="G867" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="868" spans="1:7">
@@ -15555,7 +15555,7 @@
         <v>1882</v>
       </c>
       <c r="G868" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="869" spans="1:7">
@@ -15575,7 +15575,7 @@
         <v>1958.9</v>
       </c>
       <c r="G869" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="870" spans="1:7">
@@ -15595,7 +15595,7 @@
         <v>2096.3000000000002</v>
       </c>
       <c r="G870" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="871" spans="1:7">
@@ -15615,7 +15615,7 @@
         <v>1558.8</v>
       </c>
       <c r="G871" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="872" spans="1:7">
@@ -15629,7 +15629,7 @@
         <v>10</v>
       </c>
       <c r="E872" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F872" s="8"/>
     </row>
@@ -15650,7 +15650,7 @@
         <v>1584.5</v>
       </c>
       <c r="G873" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="874" spans="1:7">
@@ -15670,7 +15670,7 @@
         <v>1895.2</v>
       </c>
       <c r="G874" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="875" spans="1:7">
@@ -15690,7 +15690,7 @@
         <v>1275.0999999999999</v>
       </c>
       <c r="G875" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="876" spans="1:7">
@@ -15710,7 +15710,7 @@
         <v>2027.1</v>
       </c>
       <c r="G876" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="877" spans="1:7">
@@ -15730,7 +15730,7 @@
         <v>1715.4</v>
       </c>
       <c r="G877" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="878" spans="1:7">
@@ -15750,7 +15750,7 @@
         <v>1992.4</v>
       </c>
       <c r="G878" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="879" spans="1:7">
@@ -15764,7 +15764,7 @@
         <v>10</v>
       </c>
       <c r="E879" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F879" s="8"/>
     </row>
@@ -16139,7 +16139,7 @@
         <v>10</v>
       </c>
       <c r="E910" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F910" s="8"/>
     </row>
@@ -16256,7 +16256,7 @@
         <v>10</v>
       </c>
       <c r="E917" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="918" spans="1:7">
@@ -16372,7 +16372,7 @@
         <v>10</v>
       </c>
       <c r="E924" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="925" spans="1:7">
@@ -16392,7 +16392,7 @@
         <v>1543.9</v>
       </c>
       <c r="G925" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="926" spans="1:7">
@@ -16412,7 +16412,7 @@
         <v>1919.9</v>
       </c>
       <c r="G926" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="927" spans="1:7">
@@ -16432,7 +16432,7 @@
         <v>2143.1</v>
       </c>
       <c r="G927" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="928" spans="1:7">
@@ -16452,7 +16452,7 @@
         <v>1435.1</v>
       </c>
       <c r="G928" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="929" spans="1:7">
@@ -16472,7 +16472,7 @@
         <v>2173.5</v>
       </c>
       <c r="G929" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="930" spans="1:7">
@@ -16492,7 +16492,7 @@
         <v>1662.9</v>
       </c>
       <c r="G930" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="931" spans="1:7">
@@ -16506,7 +16506,7 @@
         <v>10</v>
       </c>
       <c r="E931" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="932" spans="1:7">
@@ -16628,7 +16628,7 @@
         <v>10</v>
       </c>
       <c r="E938" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="939" spans="1:7">
@@ -16744,11 +16744,11 @@
         <v>10</v>
       </c>
       <c r="E945" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F945" s="8"/>
       <c r="G945" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="946" spans="1:7">
@@ -17152,7 +17152,7 @@
         <v>10</v>
       </c>
       <c r="E976" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="977" spans="1:7">
@@ -17268,7 +17268,7 @@
         <v>10</v>
       </c>
       <c r="E983" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F983" s="8"/>
     </row>
@@ -17289,7 +17289,7 @@
         <v>2025.2</v>
       </c>
       <c r="G984" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="985" spans="1:7">
@@ -17309,7 +17309,7 @@
         <v>1906.4</v>
       </c>
       <c r="G985" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="986" spans="1:7">
@@ -17329,7 +17329,7 @@
         <v>1867.7</v>
       </c>
       <c r="G986" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="987" spans="1:7">
@@ -17349,7 +17349,7 @@
         <v>1960.5</v>
       </c>
       <c r="G987" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="988" spans="1:7">
@@ -17369,7 +17369,7 @@
         <v>2083.6999999999998</v>
       </c>
       <c r="G988" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="989" spans="1:7">
@@ -17389,7 +17389,7 @@
         <v>1548.9</v>
       </c>
       <c r="G989" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="990" spans="1:7">
@@ -17403,7 +17403,7 @@
         <v>10</v>
       </c>
       <c r="E990" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="991" spans="1:7">
@@ -17423,7 +17423,7 @@
         <v>2025.2</v>
       </c>
       <c r="G991" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="992" spans="1:7">
@@ -17443,7 +17443,7 @@
         <v>1906.4</v>
       </c>
       <c r="G992" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="993" spans="1:7">
@@ -17463,7 +17463,7 @@
         <v>1867.7</v>
       </c>
       <c r="G993" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="994" spans="1:7">
@@ -17483,7 +17483,7 @@
         <v>1960.5</v>
       </c>
       <c r="G994" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="995" spans="1:7">
@@ -17503,7 +17503,7 @@
         <v>2083.6999999999998</v>
       </c>
       <c r="G995" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="996" spans="1:7">
@@ -17523,7 +17523,7 @@
         <v>1548.9</v>
       </c>
       <c r="G996" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="997" spans="1:7">
@@ -17537,7 +17537,7 @@
         <v>10</v>
       </c>
       <c r="E997" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F997" s="16"/>
     </row>
@@ -17654,7 +17654,7 @@
         <v>10</v>
       </c>
       <c r="E1004" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1005" spans="1:7">
@@ -17770,7 +17770,7 @@
         <v>10</v>
       </c>
       <c r="E1011" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1012" spans="1:6">
@@ -18246,7 +18246,7 @@
         <v>10</v>
       </c>
       <c r="E1048" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1048" s="8"/>
     </row>
@@ -18363,7 +18363,7 @@
         <v>10</v>
       </c>
       <c r="E1055" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1056" spans="1:6">
@@ -18479,7 +18479,7 @@
         <v>10</v>
       </c>
       <c r="E1062" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1063" spans="1:7">
@@ -18595,7 +18595,7 @@
         <v>10</v>
       </c>
       <c r="E1069" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="1070" spans="1:7">
@@ -18615,7 +18615,7 @@
         <v>2023.8</v>
       </c>
       <c r="G1070" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1071" spans="1:7">
@@ -18635,7 +18635,7 @@
         <v>1905.5</v>
       </c>
       <c r="G1071" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1072" spans="1:7">
@@ -18655,7 +18655,7 @@
         <v>1864.1</v>
       </c>
       <c r="G1072" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1073" spans="1:7">
@@ -18675,7 +18675,7 @@
         <v>1957.2</v>
       </c>
       <c r="G1073" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1074" spans="1:7">
@@ -18695,7 +18695,7 @@
         <v>2079.6</v>
       </c>
       <c r="G1074" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1075" spans="1:7">
@@ -18715,7 +18715,7 @@
         <v>1550.3</v>
       </c>
       <c r="G1075" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1076" spans="1:7">
@@ -18729,7 +18729,7 @@
         <v>10</v>
       </c>
       <c r="E1076" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="1077" spans="1:7">
@@ -18845,7 +18845,7 @@
         <v>10</v>
       </c>
       <c r="E1083" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1083" s="8"/>
     </row>
@@ -19220,7 +19220,7 @@
         <v>10</v>
       </c>
       <c r="E1114" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1114" s="8"/>
     </row>
@@ -19337,7 +19337,7 @@
         <v>10</v>
       </c>
       <c r="E1121" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1121" s="8"/>
     </row>
@@ -19454,7 +19454,7 @@
         <v>10</v>
       </c>
       <c r="E1128" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1128" s="8"/>
     </row>
@@ -19571,10 +19571,10 @@
         <v>10</v>
       </c>
       <c r="E1135" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G1135" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="1136" spans="1:7">
@@ -19588,10 +19588,10 @@
         <v>10</v>
       </c>
       <c r="E1136" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1136" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="1137" spans="1:7">
@@ -19611,7 +19611,7 @@
         <v>2012.7</v>
       </c>
       <c r="G1137" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1138" spans="1:7">
@@ -19631,7 +19631,7 @@
         <v>1896.4</v>
       </c>
       <c r="G1138" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1139" spans="1:7">
@@ -19651,7 +19651,7 @@
         <v>1856.2</v>
       </c>
       <c r="G1139" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1140" spans="1:7">
@@ -19671,7 +19671,7 @@
         <v>1948.5</v>
       </c>
       <c r="G1140" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1141" spans="1:7">
@@ -19691,7 +19691,7 @@
         <v>2069.1</v>
       </c>
       <c r="G1141" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1142" spans="1:7">
@@ -19711,7 +19711,7 @@
         <v>1529.5</v>
       </c>
       <c r="G1142" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1143" spans="1:7">
@@ -19725,7 +19725,7 @@
         <v>10</v>
       </c>
       <c r="E1143" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1143" s="8"/>
     </row>
@@ -20202,7 +20202,7 @@
         <v>10</v>
       </c>
       <c r="E1180" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1181" spans="1:6">
@@ -20318,7 +20318,7 @@
         <v>10</v>
       </c>
       <c r="E1187" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1188" spans="1:6">
@@ -20434,7 +20434,7 @@
         <v>10</v>
       </c>
       <c r="E1194" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1195" spans="1:6">
@@ -20550,7 +20550,7 @@
         <v>10</v>
       </c>
       <c r="E1201" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="1202" spans="1:7">
@@ -20570,7 +20570,7 @@
         <v>2021.8</v>
       </c>
       <c r="G1202" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1203" spans="1:7">
@@ -20590,7 +20590,7 @@
         <v>1903.6</v>
       </c>
       <c r="G1203" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1204" spans="1:7">
@@ -20610,7 +20610,7 @@
         <v>1856.8</v>
       </c>
       <c r="G1204" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1205" spans="1:7">
@@ -20630,7 +20630,7 @@
         <v>1952.9</v>
       </c>
       <c r="G1205" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1206" spans="1:7">
@@ -20650,7 +20650,7 @@
         <v>2066.8000000000002</v>
       </c>
       <c r="G1206" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1207" spans="1:7">
@@ -20670,7 +20670,7 @@
         <v>1542.3</v>
       </c>
       <c r="G1207" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1208" spans="1:7">
@@ -20684,7 +20684,7 @@
         <v>10</v>
       </c>
       <c r="E1208" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="1209" spans="1:7">
@@ -20800,7 +20800,7 @@
         <v>10</v>
       </c>
       <c r="E1215" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F1215" s="8"/>
     </row>

</xml_diff>

<commit_message>
Added core dry mass data
Per @apeyton Slack upload on 31 December 2015.
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="81">
   <si>
     <t>Treatment</t>
   </si>
@@ -258,6 +258,12 @@
   <si>
     <t>SoilVolume_cm3</t>
   </si>
+  <si>
+    <t>CoreSleeveMass_g</t>
+  </si>
+  <si>
+    <t>SoilDryMass_g</t>
+  </si>
 </sst>
 </file>
 
@@ -351,8 +357,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="267">
+  <cellStyleXfs count="271">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -643,7 +653,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="267">
+  <cellStyles count="271">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -777,6 +787,8 @@
     <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -910,6 +922,8 @@
     <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1209,21 +1223,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="18">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="18">
       <c r="A1" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1236,156 +1250,234 @@
       <c r="D2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3">
+        <v>1139.9000000000001</v>
+      </c>
+      <c r="E3">
+        <v>148.9</v>
+      </c>
+      <c r="F3">
+        <v>1759.3119999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4">
+        <v>1139.9000000000001</v>
+      </c>
+      <c r="E4">
+        <v>151.9</v>
+      </c>
+      <c r="F4">
+        <v>832.48400000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D5">
+        <v>1242.4000000000001</v>
+      </c>
+      <c r="E5">
+        <v>151.6</v>
+      </c>
+      <c r="F5">
+        <v>1799.9380000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
         <v>1162.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>1253.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>150.9</v>
+      </c>
+      <c r="F6">
+        <v>1229.8240000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>1139.9000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>1162.7</v>
+      </c>
+      <c r="E7">
+        <v>151.1</v>
+      </c>
+      <c r="F7">
+        <v>1666.933</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>22</v>
       </c>
       <c r="D8">
-        <v>1185.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>1048.7</v>
+      </c>
+      <c r="E8">
+        <v>149.30000000000001</v>
+      </c>
+      <c r="F8">
+        <v>1421.643</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D9">
         <v>1231</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>149</v>
+      </c>
+      <c r="F9">
+        <v>1845.2750000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>22</v>
       </c>
       <c r="D10">
-        <v>1185.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>1071.5</v>
+      </c>
+      <c r="E10">
+        <v>147.69999999999999</v>
+      </c>
+      <c r="F10">
+        <v>1495.182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>22</v>
       </c>
       <c r="D11">
-        <v>1162.7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>1025.9000000000001</v>
+      </c>
+      <c r="E11">
+        <v>134.69999999999999</v>
+      </c>
+      <c r="F11">
+        <v>1335.673</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <v>22</v>
       </c>
       <c r="D12">
-        <v>1071.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>1253.8</v>
+      </c>
+      <c r="E12">
+        <v>154.80000000000001</v>
+      </c>
+      <c r="F12">
+        <v>1964.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>1048.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>1185.5</v>
+      </c>
+      <c r="E13">
+        <v>128.80000000000001</v>
+      </c>
+      <c r="F13">
+        <v>1600.3969999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1398,24 +1490,36 @@
       <c r="D14">
         <v>1299.4000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>148.4</v>
+      </c>
+      <c r="F14">
+        <v>1907.1690000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>22</v>
       </c>
       <c r="D15">
-        <v>1139.9000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>1231</v>
+      </c>
+      <c r="E15">
+        <v>146.80000000000001</v>
+      </c>
+      <c r="F15">
+        <v>1461.6859999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
@@ -1424,12 +1528,18 @@
         <v>22</v>
       </c>
       <c r="D16">
-        <v>1094.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>1162.7</v>
+      </c>
+      <c r="E16">
+        <v>129.9</v>
+      </c>
+      <c r="F16">
+        <v>1708.298</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
@@ -1438,38 +1548,56 @@
         <v>22</v>
       </c>
       <c r="D17">
-        <v>1025.9000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>1162.7</v>
+      </c>
+      <c r="E17">
+        <v>132.30000000000001</v>
+      </c>
+      <c r="F17">
+        <v>1727.0160000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C18">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>1162.7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>957.5</v>
+      </c>
+      <c r="E18">
+        <v>149.6</v>
+      </c>
+      <c r="F18">
+        <v>1162.577</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <v>1299.4000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>1048.7</v>
+      </c>
+      <c r="E19">
+        <v>129.4</v>
+      </c>
+      <c r="F19">
+        <v>1726.425</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1482,10 +1610,16 @@
       <c r="D20">
         <v>957.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>148.19999999999999</v>
+      </c>
+      <c r="F20">
+        <v>1140.2629999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>35</v>
@@ -1494,38 +1628,56 @@
         <v>22</v>
       </c>
       <c r="D21">
-        <v>1253.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>1299.4000000000001</v>
+      </c>
+      <c r="E21">
+        <v>147.19999999999999</v>
+      </c>
+      <c r="F21">
+        <v>1950.2550000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C22">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D22">
         <v>1094.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>154.9</v>
+      </c>
+      <c r="F22">
+        <v>1351.7080000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D23">
-        <v>957.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>1185.5</v>
+      </c>
+      <c r="E23">
+        <v>147.69999999999999</v>
+      </c>
+      <c r="F23">
+        <v>1651.3109999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1538,148 +1690,199 @@
       <c r="D24">
         <v>1185.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>155.4</v>
+      </c>
+      <c r="F24">
+        <v>1486.2750000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D25">
         <v>1094.3</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>148.9</v>
+      </c>
+      <c r="F25">
+        <v>1448.2239999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D26">
-        <v>1139.9000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>1162.7</v>
+      </c>
+      <c r="E26">
+        <v>149.4</v>
+      </c>
+      <c r="F26">
+        <v>1567.252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
       </c>
       <c r="C27">
+        <v>22</v>
+      </c>
+      <c r="D27">
+        <v>1253.8</v>
+      </c>
+      <c r="E27">
+        <v>150.9</v>
+      </c>
+      <c r="F27">
+        <v>1815.444</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
         <v>4</v>
-      </c>
-      <c r="D27">
-        <v>1094.3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>14</v>
       </c>
       <c r="B28" t="s">
         <v>32</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D28">
         <v>1185.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28">
+        <v>152.1</v>
+      </c>
+      <c r="F28">
+        <v>1414.568</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D29">
-        <v>1242.4000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>1094.3</v>
+      </c>
+      <c r="E29">
+        <v>148.30000000000001</v>
+      </c>
+      <c r="F29">
+        <v>1470.0139999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>4</v>
       </c>
       <c r="D30">
-        <v>1048.7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>1139.9000000000001</v>
+      </c>
+      <c r="E30">
+        <v>133.5</v>
+      </c>
+      <c r="F30">
+        <v>1640.9259999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31">
         <v>4</v>
       </c>
       <c r="D31">
-        <v>1162.7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>1094.3</v>
+      </c>
+      <c r="E31">
+        <v>149.1</v>
+      </c>
+      <c r="F31">
+        <v>735.10699999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D32">
         <v>1139.9000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <v>148.6</v>
+      </c>
+      <c r="F32">
+        <v>1385.0909999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C33">
-        <v>4</v>
-      </c>
-      <c r="D33">
-        <v>1231</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
-      <c r="D34">
-        <v>1162.7</v>
-      </c>
     </row>
   </sheetData>
+  <sortState ref="A3:D34">
+    <sortCondition ref="A3:A34"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Added Peyton's new data file
Also shifted reading of mass data from script 2 to script 4
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="15600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24680" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="treatments.csv" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="78">
   <si>
     <t>Treatment</t>
   </si>
@@ -254,15 +254,6 @@
   </si>
   <si>
     <t>new port valves</t>
-  </si>
-  <si>
-    <t>SoilVolume_cm3</t>
-  </si>
-  <si>
-    <t>CoreSleeveMass_g</t>
-  </si>
-  <si>
-    <t>SoilDryMass_g</t>
   </si>
 </sst>
 </file>
@@ -1223,21 +1214,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="18">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="18">
       <c r="A1" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1247,17 +1238,8 @@
       <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1267,17 +1249,8 @@
       <c r="C3">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>1139.9000000000001</v>
-      </c>
-      <c r="E3">
-        <v>148.9</v>
-      </c>
-      <c r="F3">
-        <v>1759.3119999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1287,17 +1260,8 @@
       <c r="C4">
         <v>22</v>
       </c>
-      <c r="D4">
-        <v>1139.9000000000001</v>
-      </c>
-      <c r="E4">
-        <v>151.9</v>
-      </c>
-      <c r="F4">
-        <v>832.48400000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1307,17 +1271,8 @@
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>1242.4000000000001</v>
-      </c>
-      <c r="E5">
-        <v>151.6</v>
-      </c>
-      <c r="F5">
-        <v>1799.9380000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1327,17 +1282,8 @@
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>1162.7</v>
-      </c>
-      <c r="E6">
-        <v>150.9</v>
-      </c>
-      <c r="F6">
-        <v>1229.8240000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1347,17 +1293,8 @@
       <c r="C7">
         <v>4</v>
       </c>
-      <c r="D7">
-        <v>1162.7</v>
-      </c>
-      <c r="E7">
-        <v>151.1</v>
-      </c>
-      <c r="F7">
-        <v>1666.933</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1367,17 +1304,8 @@
       <c r="C8">
         <v>22</v>
       </c>
-      <c r="D8">
-        <v>1048.7</v>
-      </c>
-      <c r="E8">
-        <v>149.30000000000001</v>
-      </c>
-      <c r="F8">
-        <v>1421.643</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1387,17 +1315,8 @@
       <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9">
-        <v>1231</v>
-      </c>
-      <c r="E9">
-        <v>149</v>
-      </c>
-      <c r="F9">
-        <v>1845.2750000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1407,17 +1326,8 @@
       <c r="C10">
         <v>22</v>
       </c>
-      <c r="D10">
-        <v>1071.5</v>
-      </c>
-      <c r="E10">
-        <v>147.69999999999999</v>
-      </c>
-      <c r="F10">
-        <v>1495.182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1427,17 +1337,8 @@
       <c r="C11">
         <v>22</v>
       </c>
-      <c r="D11">
-        <v>1025.9000000000001</v>
-      </c>
-      <c r="E11">
-        <v>134.69999999999999</v>
-      </c>
-      <c r="F11">
-        <v>1335.673</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1447,17 +1348,8 @@
       <c r="C12">
         <v>22</v>
       </c>
-      <c r="D12">
-        <v>1253.8</v>
-      </c>
-      <c r="E12">
-        <v>154.80000000000001</v>
-      </c>
-      <c r="F12">
-        <v>1964.05</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1467,17 +1359,8 @@
       <c r="C13">
         <v>4</v>
       </c>
-      <c r="D13">
-        <v>1185.5</v>
-      </c>
-      <c r="E13">
-        <v>128.80000000000001</v>
-      </c>
-      <c r="F13">
-        <v>1600.3969999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1487,17 +1370,8 @@
       <c r="C14">
         <v>22</v>
       </c>
-      <c r="D14">
-        <v>1299.4000000000001</v>
-      </c>
-      <c r="E14">
-        <v>148.4</v>
-      </c>
-      <c r="F14">
-        <v>1907.1690000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1507,17 +1381,8 @@
       <c r="C15">
         <v>22</v>
       </c>
-      <c r="D15">
-        <v>1231</v>
-      </c>
-      <c r="E15">
-        <v>146.80000000000001</v>
-      </c>
-      <c r="F15">
-        <v>1461.6859999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1527,17 +1392,8 @@
       <c r="C16">
         <v>22</v>
       </c>
-      <c r="D16">
-        <v>1162.7</v>
-      </c>
-      <c r="E16">
-        <v>129.9</v>
-      </c>
-      <c r="F16">
-        <v>1708.298</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1547,17 +1403,8 @@
       <c r="C17">
         <v>22</v>
       </c>
-      <c r="D17">
-        <v>1162.7</v>
-      </c>
-      <c r="E17">
-        <v>132.30000000000001</v>
-      </c>
-      <c r="F17">
-        <v>1727.0160000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -1567,17 +1414,8 @@
       <c r="C18">
         <v>4</v>
       </c>
-      <c r="D18">
-        <v>957.5</v>
-      </c>
-      <c r="E18">
-        <v>149.6</v>
-      </c>
-      <c r="F18">
-        <v>1162.577</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1587,17 +1425,8 @@
       <c r="C19">
         <v>4</v>
       </c>
-      <c r="D19">
-        <v>1048.7</v>
-      </c>
-      <c r="E19">
-        <v>129.4</v>
-      </c>
-      <c r="F19">
-        <v>1726.425</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1607,17 +1436,8 @@
       <c r="C20">
         <v>22</v>
       </c>
-      <c r="D20">
-        <v>957.5</v>
-      </c>
-      <c r="E20">
-        <v>148.19999999999999</v>
-      </c>
-      <c r="F20">
-        <v>1140.2629999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1627,17 +1447,8 @@
       <c r="C21">
         <v>22</v>
       </c>
-      <c r="D21">
-        <v>1299.4000000000001</v>
-      </c>
-      <c r="E21">
-        <v>147.19999999999999</v>
-      </c>
-      <c r="F21">
-        <v>1950.2550000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1647,17 +1458,8 @@
       <c r="C22">
         <v>4</v>
       </c>
-      <c r="D22">
-        <v>1094.3</v>
-      </c>
-      <c r="E22">
-        <v>154.9</v>
-      </c>
-      <c r="F22">
-        <v>1351.7080000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1667,17 +1469,8 @@
       <c r="C23">
         <v>22</v>
       </c>
-      <c r="D23">
-        <v>1185.5</v>
-      </c>
-      <c r="E23">
-        <v>147.69999999999999</v>
-      </c>
-      <c r="F23">
-        <v>1651.3109999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1687,17 +1480,8 @@
       <c r="C24">
         <v>4</v>
       </c>
-      <c r="D24">
-        <v>1185.5</v>
-      </c>
-      <c r="E24">
-        <v>155.4</v>
-      </c>
-      <c r="F24">
-        <v>1486.2750000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1707,17 +1491,8 @@
       <c r="C25">
         <v>22</v>
       </c>
-      <c r="D25">
-        <v>1094.3</v>
-      </c>
-      <c r="E25">
-        <v>148.9</v>
-      </c>
-      <c r="F25">
-        <v>1448.2239999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1727,17 +1502,8 @@
       <c r="C26">
         <v>22</v>
       </c>
-      <c r="D26">
-        <v>1162.7</v>
-      </c>
-      <c r="E26">
-        <v>149.4</v>
-      </c>
-      <c r="F26">
-        <v>1567.252</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1747,17 +1513,8 @@
       <c r="C27">
         <v>22</v>
       </c>
-      <c r="D27">
-        <v>1253.8</v>
-      </c>
-      <c r="E27">
-        <v>150.9</v>
-      </c>
-      <c r="F27">
-        <v>1815.444</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1767,17 +1524,8 @@
       <c r="C28">
         <v>22</v>
       </c>
-      <c r="D28">
-        <v>1185.5</v>
-      </c>
-      <c r="E28">
-        <v>152.1</v>
-      </c>
-      <c r="F28">
-        <v>1414.568</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -1787,17 +1535,8 @@
       <c r="C29">
         <v>22</v>
       </c>
-      <c r="D29">
-        <v>1094.3</v>
-      </c>
-      <c r="E29">
-        <v>148.30000000000001</v>
-      </c>
-      <c r="F29">
-        <v>1470.0139999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1807,17 +1546,8 @@
       <c r="C30">
         <v>4</v>
       </c>
-      <c r="D30">
-        <v>1139.9000000000001</v>
-      </c>
-      <c r="E30">
-        <v>133.5</v>
-      </c>
-      <c r="F30">
-        <v>1640.9259999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1827,17 +1557,8 @@
       <c r="C31">
         <v>4</v>
       </c>
-      <c r="D31">
-        <v>1094.3</v>
-      </c>
-      <c r="E31">
-        <v>149.1</v>
-      </c>
-      <c r="F31">
-        <v>735.10699999999997</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1846,15 +1567,6 @@
       </c>
       <c r="C32">
         <v>22</v>
-      </c>
-      <c r="D32">
-        <v>1139.9000000000001</v>
-      </c>
-      <c r="E32">
-        <v>148.6</v>
-      </c>
-      <c r="F32">
-        <v>1385.0909999999999</v>
       </c>
     </row>
     <row r="33" spans="1:3">

</xml_diff>

<commit_message>
Updated to 20 C throughout, reran diagnostics
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24680" windowHeight="15600"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24400" windowHeight="15360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="treatments.csv" sheetId="2" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>Ambient4</t>
   </si>
   <si>
-    <t>Ambient22</t>
-  </si>
-  <si>
     <t xml:space="preserve">10ml water added 9/10/2015 accidental </t>
   </si>
   <si>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>new port valves</t>
+  </si>
+  <si>
+    <t>Ambient20</t>
   </si>
 </sst>
 </file>
@@ -1216,9 +1216,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
         <v>40</v>
@@ -1609,9 +1609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1215"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A1195" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1216" sqref="A1216"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1662,7 +1662,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1799,7 +1799,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1936,7 +1936,7 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2621,7 +2621,7 @@
         <v>10</v>
       </c>
       <c r="E52" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2758,7 +2758,7 @@
         <v>10</v>
       </c>
       <c r="E59" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -2895,7 +2895,7 @@
         <v>10</v>
       </c>
       <c r="E66" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3032,7 +3032,7 @@
         <v>10</v>
       </c>
       <c r="E73" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -3169,7 +3169,7 @@
         <v>10</v>
       </c>
       <c r="E80" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -3306,7 +3306,7 @@
         <v>10</v>
       </c>
       <c r="E87" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -3991,7 +3991,7 @@
         <v>10</v>
       </c>
       <c r="E122" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -4128,7 +4128,7 @@
         <v>10</v>
       </c>
       <c r="E129" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -4265,7 +4265,7 @@
         <v>10</v>
       </c>
       <c r="E136" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -4789,7 +4789,7 @@
         <v>10</v>
       </c>
       <c r="E173" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -4905,7 +4905,7 @@
         <v>10</v>
       </c>
       <c r="E180" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="181" spans="1:6">
@@ -5021,7 +5021,7 @@
         <v>10</v>
       </c>
       <c r="E187" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -5386,7 +5386,7 @@
         <v>45</v>
       </c>
       <c r="G209" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="210" spans="1:7">
@@ -5790,7 +5790,7 @@
         <v>10</v>
       </c>
       <c r="E240" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="241" spans="1:6">
@@ -5906,7 +5906,7 @@
         <v>10</v>
       </c>
       <c r="E247" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="248" spans="1:6">
@@ -6022,7 +6022,7 @@
         <v>10</v>
       </c>
       <c r="E254" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="255" spans="1:6">
@@ -6158,7 +6158,7 @@
         <v>2103.5</v>
       </c>
       <c r="G262" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -6178,7 +6178,7 @@
         <v>1999.2</v>
       </c>
       <c r="G263" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -6198,7 +6198,7 @@
         <v>1967.3</v>
       </c>
       <c r="G264" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -6218,7 +6218,7 @@
         <v>2034.7</v>
       </c>
       <c r="G265" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -6238,7 +6238,7 @@
         <v>2158.3000000000002</v>
       </c>
       <c r="G266" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -6258,7 +6258,7 @@
         <v>1659.2</v>
       </c>
       <c r="G267" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="268" spans="1:7">
@@ -6792,7 +6792,7 @@
         <v>10</v>
       </c>
       <c r="E306" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="307" spans="1:6">
@@ -6908,7 +6908,7 @@
         <v>10</v>
       </c>
       <c r="E313" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="314" spans="1:6">
@@ -7024,7 +7024,7 @@
         <v>10</v>
       </c>
       <c r="E320" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="321" spans="1:6">
@@ -7372,7 +7372,7 @@
         <v>10</v>
       </c>
       <c r="E341" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="342" spans="1:7">
@@ -7488,7 +7488,7 @@
         <v>10</v>
       </c>
       <c r="E348" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="349" spans="1:7">
@@ -7508,7 +7508,7 @@
         <v>1921.4</v>
       </c>
       <c r="G349" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="350" spans="1:7">
@@ -7528,7 +7528,7 @@
         <v>1711.5</v>
       </c>
       <c r="G350" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="351" spans="1:7">
@@ -7548,7 +7548,7 @@
         <v>1699</v>
       </c>
       <c r="G351" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="352" spans="1:7">
@@ -7568,7 +7568,7 @@
         <v>2146.8000000000002</v>
       </c>
       <c r="G352" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="353" spans="1:7">
@@ -7588,7 +7588,7 @@
         <v>1661.6</v>
       </c>
       <c r="G353" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="354" spans="1:7">
@@ -7608,7 +7608,7 @@
         <v>1703.8</v>
       </c>
       <c r="G354" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="355" spans="1:7">
@@ -7622,7 +7622,7 @@
         <v>10</v>
       </c>
       <c r="E355" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="356" spans="1:7">
@@ -7986,7 +7986,7 @@
         <v>1962.9</v>
       </c>
       <c r="G377" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="378" spans="1:7">
@@ -8002,7 +8002,7 @@
         <v>2173.1</v>
       </c>
       <c r="G378" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="379" spans="1:7">
@@ -8018,7 +8018,7 @@
         <v>1441.9</v>
       </c>
       <c r="G379" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="380" spans="1:7">
@@ -8034,7 +8034,7 @@
         <v>1843.5</v>
       </c>
       <c r="G380" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="381" spans="1:7">
@@ -8050,7 +8050,7 @@
         <v>1853.6</v>
       </c>
       <c r="G381" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="382" spans="1:7">
@@ -8066,7 +8066,7 @@
         <v>2016.2</v>
       </c>
       <c r="G382" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="383" spans="1:7">
@@ -8082,7 +8082,7 @@
         <v>1908.3</v>
       </c>
       <c r="G383" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="384" spans="1:7">
@@ -8098,7 +8098,7 @@
         <v>1698.8</v>
       </c>
       <c r="G384" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="385" spans="1:7">
@@ -8140,7 +8140,7 @@
         <v>1648</v>
       </c>
       <c r="G387" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="388" spans="1:7">
@@ -8169,7 +8169,7 @@
         <v>1580.9</v>
       </c>
       <c r="G389" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="390" spans="1:7">
@@ -8185,7 +8185,7 @@
         <v>1974.9</v>
       </c>
       <c r="G390" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="391" spans="1:7">
@@ -8201,7 +8201,7 @@
         <v>2171.3000000000002</v>
       </c>
       <c r="G391" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="392" spans="1:7">
@@ -8217,7 +8217,7 @@
         <v>1421</v>
       </c>
       <c r="G392" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="393" spans="1:7">
@@ -8233,7 +8233,7 @@
         <v>2196.4</v>
       </c>
       <c r="G393" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="394" spans="1:7">
@@ -8249,7 +8249,7 @@
         <v>1678.7</v>
       </c>
       <c r="G394" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="395" spans="1:7">
@@ -8343,7 +8343,7 @@
         <v>1611.8</v>
       </c>
       <c r="G401" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="402" spans="1:7">
@@ -8359,7 +8359,7 @@
         <v>1903.3</v>
       </c>
       <c r="G402" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="403" spans="1:7">
@@ -8375,7 +8375,7 @@
         <v>1286.8</v>
       </c>
       <c r="G403" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="404" spans="1:7">
@@ -8391,7 +8391,7 @@
         <v>2041.3</v>
       </c>
       <c r="G404" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="405" spans="1:7">
@@ -8420,7 +8420,7 @@
         <v>2012.2</v>
       </c>
       <c r="G406" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="407" spans="1:7">
@@ -8434,7 +8434,7 @@
         <v>10</v>
       </c>
       <c r="E407" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="408" spans="1:7">
@@ -8471,7 +8471,7 @@
         <v>2180.4</v>
       </c>
       <c r="G409" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="410" spans="1:7">
@@ -8491,7 +8491,7 @@
         <v>1443.3</v>
       </c>
       <c r="G410" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="411" spans="1:7">
@@ -8556,7 +8556,7 @@
         <v>10</v>
       </c>
       <c r="E414" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="415" spans="1:7">
@@ -8672,7 +8672,7 @@
         <v>10</v>
       </c>
       <c r="E421" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="422" spans="1:7">
@@ -8692,7 +8692,7 @@
         <v>1973.3</v>
       </c>
       <c r="G422" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="423" spans="1:7">
@@ -8712,7 +8712,7 @@
         <v>2180.4</v>
       </c>
       <c r="G423" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="424" spans="1:7">
@@ -8732,7 +8732,7 @@
         <v>1443.3</v>
       </c>
       <c r="G424" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="425" spans="1:7">
@@ -8752,7 +8752,7 @@
         <v>1851</v>
       </c>
       <c r="G425" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="426" spans="1:7">
@@ -8772,7 +8772,7 @@
         <v>1862.9</v>
       </c>
       <c r="G426" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="427" spans="1:7">
@@ -8792,7 +8792,7 @@
         <v>2026.8</v>
       </c>
       <c r="G427" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="428" spans="1:7">
@@ -8806,7 +8806,7 @@
         <v>10</v>
       </c>
       <c r="E428" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="429" spans="1:7">
@@ -8826,7 +8826,7 @@
         <v>1585.9</v>
       </c>
       <c r="G429" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="430" spans="1:7">
@@ -8846,7 +8846,7 @@
         <v>1986.5</v>
       </c>
       <c r="G430" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="431" spans="1:7">
@@ -8866,7 +8866,7 @@
         <v>2209.4</v>
       </c>
       <c r="G431" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="432" spans="1:7">
@@ -8886,7 +8886,7 @@
         <v>1453.3</v>
       </c>
       <c r="G432" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="433" spans="1:7">
@@ -8906,7 +8906,7 @@
         <v>2216.5</v>
       </c>
       <c r="G433" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="434" spans="1:7">
@@ -8926,7 +8926,7 @@
         <v>1703.3</v>
       </c>
       <c r="G434" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="435" spans="1:7">
@@ -8994,7 +8994,7 @@
         <v>1292.5999999999999</v>
       </c>
       <c r="G438" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="439" spans="1:7">
@@ -9031,7 +9031,7 @@
         <v>1727</v>
       </c>
       <c r="G440" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="441" spans="1:7">
@@ -9051,7 +9051,7 @@
         <v>2042.8</v>
       </c>
       <c r="G441" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="442" spans="1:7">
@@ -9687,7 +9687,7 @@
         <v>10</v>
       </c>
       <c r="E486" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F486" s="8"/>
     </row>
@@ -9804,7 +9804,7 @@
         <v>10</v>
       </c>
       <c r="E493" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F493" s="8"/>
     </row>
@@ -9921,7 +9921,7 @@
         <v>10</v>
       </c>
       <c r="E500" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F500" s="8"/>
     </row>
@@ -10560,11 +10560,11 @@
         <v>10</v>
       </c>
       <c r="E545" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F545" s="8"/>
       <c r="G545" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="546" spans="1:7">
@@ -10680,7 +10680,7 @@
         <v>10</v>
       </c>
       <c r="E552" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F552" s="8"/>
     </row>
@@ -10797,7 +10797,7 @@
         <v>10</v>
       </c>
       <c r="E559" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F559" s="8"/>
     </row>
@@ -11265,7 +11265,7 @@
         <v>10</v>
       </c>
       <c r="E587" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="588" spans="1:6">
@@ -11381,7 +11381,7 @@
         <v>10</v>
       </c>
       <c r="E594" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F594" s="8"/>
     </row>
@@ -11498,7 +11498,7 @@
         <v>10</v>
       </c>
       <c r="E601" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="602" spans="1:6">
@@ -12136,7 +12136,7 @@
         <v>10</v>
       </c>
       <c r="E646" s="11" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F646" s="8"/>
     </row>
@@ -12253,7 +12253,7 @@
         <v>10</v>
       </c>
       <c r="E653" s="11" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F653" s="8"/>
     </row>
@@ -12370,7 +12370,7 @@
         <v>10</v>
       </c>
       <c r="E660" s="11" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="661" spans="1:6">
@@ -13227,7 +13227,7 @@
         <v>10</v>
       </c>
       <c r="E718" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F718" s="8"/>
     </row>
@@ -13344,7 +13344,7 @@
         <v>10</v>
       </c>
       <c r="E725" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F725" s="8"/>
     </row>
@@ -13461,7 +13461,7 @@
         <v>10</v>
       </c>
       <c r="E732" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F732" s="8"/>
     </row>
@@ -13480,7 +13480,7 @@
       </c>
       <c r="F733" s="8"/>
       <c r="G733" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="734" spans="1:7">
@@ -14073,7 +14073,7 @@
         <v>10</v>
       </c>
       <c r="E777" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F777" s="8"/>
     </row>
@@ -14190,7 +14190,7 @@
         <v>10</v>
       </c>
       <c r="E784" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="785" spans="1:7">
@@ -14210,7 +14210,7 @@
         <v>1921.6</v>
       </c>
       <c r="G785" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="786" spans="1:7">
@@ -14230,7 +14230,7 @@
         <v>1703.7</v>
       </c>
       <c r="G786" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="787" spans="1:7">
@@ -14312,7 +14312,7 @@
         <v>10</v>
       </c>
       <c r="E791" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="792" spans="1:7">
@@ -14428,11 +14428,11 @@
         <v>10</v>
       </c>
       <c r="E798" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F798" s="8"/>
       <c r="G798" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="799" spans="1:7">
@@ -14450,7 +14450,7 @@
       </c>
       <c r="F799" s="8"/>
       <c r="G799" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="800" spans="1:7">
@@ -15058,7 +15058,7 @@
         <v>10</v>
       </c>
       <c r="E844" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F844" s="8"/>
     </row>
@@ -15175,7 +15175,7 @@
         <v>10</v>
       </c>
       <c r="E851" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F851" s="8"/>
     </row>
@@ -15292,7 +15292,7 @@
         <v>10</v>
       </c>
       <c r="E858" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F858" s="8"/>
     </row>
@@ -15409,7 +15409,7 @@
         <v>10</v>
       </c>
       <c r="E865" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F865" s="8"/>
     </row>
@@ -15430,7 +15430,7 @@
         <v>2024.8</v>
       </c>
       <c r="G866" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="867" spans="1:7">
@@ -15450,7 +15450,7 @@
         <v>1911.54</v>
       </c>
       <c r="G867" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="868" spans="1:7">
@@ -15470,7 +15470,7 @@
         <v>1882</v>
       </c>
       <c r="G868" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="869" spans="1:7">
@@ -15490,7 +15490,7 @@
         <v>1958.9</v>
       </c>
       <c r="G869" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="870" spans="1:7">
@@ -15510,7 +15510,7 @@
         <v>2096.3000000000002</v>
       </c>
       <c r="G870" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="871" spans="1:7">
@@ -15530,7 +15530,7 @@
         <v>1558.8</v>
       </c>
       <c r="G871" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="872" spans="1:7">
@@ -15565,7 +15565,7 @@
         <v>1584.5</v>
       </c>
       <c r="G873" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="874" spans="1:7">
@@ -15585,7 +15585,7 @@
         <v>1895.2</v>
       </c>
       <c r="G874" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="875" spans="1:7">
@@ -15605,7 +15605,7 @@
         <v>1275.0999999999999</v>
       </c>
       <c r="G875" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="876" spans="1:7">
@@ -15625,7 +15625,7 @@
         <v>2027.1</v>
       </c>
       <c r="G876" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="877" spans="1:7">
@@ -15645,7 +15645,7 @@
         <v>1715.4</v>
       </c>
       <c r="G877" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="878" spans="1:7">
@@ -15665,7 +15665,7 @@
         <v>1992.4</v>
       </c>
       <c r="G878" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="879" spans="1:7">
@@ -16054,7 +16054,7 @@
         <v>10</v>
       </c>
       <c r="E910" s="11" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F910" s="8"/>
     </row>
@@ -16171,7 +16171,7 @@
         <v>10</v>
       </c>
       <c r="E917" s="11" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="918" spans="1:7">
@@ -16287,7 +16287,7 @@
         <v>10</v>
       </c>
       <c r="E924" s="11" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="925" spans="1:7">
@@ -16307,7 +16307,7 @@
         <v>1543.9</v>
       </c>
       <c r="G925" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="926" spans="1:7">
@@ -16327,7 +16327,7 @@
         <v>1919.9</v>
       </c>
       <c r="G926" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="927" spans="1:7">
@@ -16347,7 +16347,7 @@
         <v>2143.1</v>
       </c>
       <c r="G927" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="928" spans="1:7">
@@ -16367,7 +16367,7 @@
         <v>1435.1</v>
       </c>
       <c r="G928" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="929" spans="1:7">
@@ -16387,7 +16387,7 @@
         <v>2173.5</v>
       </c>
       <c r="G929" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="930" spans="1:7">
@@ -16407,7 +16407,7 @@
         <v>1662.9</v>
       </c>
       <c r="G930" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="931" spans="1:7">
@@ -16663,7 +16663,7 @@
       </c>
       <c r="F945" s="8"/>
       <c r="G945" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="946" spans="1:7">
@@ -17204,7 +17204,7 @@
         <v>2025.2</v>
       </c>
       <c r="G984" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="985" spans="1:7">
@@ -17224,7 +17224,7 @@
         <v>1906.4</v>
       </c>
       <c r="G985" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="986" spans="1:7">
@@ -17244,7 +17244,7 @@
         <v>1867.7</v>
       </c>
       <c r="G986" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="987" spans="1:7">
@@ -17264,7 +17264,7 @@
         <v>1960.5</v>
       </c>
       <c r="G987" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="988" spans="1:7">
@@ -17284,7 +17284,7 @@
         <v>2083.6999999999998</v>
       </c>
       <c r="G988" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="989" spans="1:7">
@@ -17304,7 +17304,7 @@
         <v>1548.9</v>
       </c>
       <c r="G989" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="990" spans="1:7">
@@ -17338,7 +17338,7 @@
         <v>2025.2</v>
       </c>
       <c r="G991" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="992" spans="1:7">
@@ -17358,7 +17358,7 @@
         <v>1906.4</v>
       </c>
       <c r="G992" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="993" spans="1:7">
@@ -17378,7 +17378,7 @@
         <v>1867.7</v>
       </c>
       <c r="G993" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="994" spans="1:7">
@@ -17398,7 +17398,7 @@
         <v>1960.5</v>
       </c>
       <c r="G994" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="995" spans="1:7">
@@ -17418,7 +17418,7 @@
         <v>2083.6999999999998</v>
       </c>
       <c r="G995" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="996" spans="1:7">
@@ -17438,7 +17438,7 @@
         <v>1548.9</v>
       </c>
       <c r="G996" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="997" spans="1:7">
@@ -17452,7 +17452,7 @@
         <v>10</v>
       </c>
       <c r="E997" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F997" s="16"/>
     </row>
@@ -17569,7 +17569,7 @@
         <v>10</v>
       </c>
       <c r="E1004" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1005" spans="1:7">
@@ -17685,7 +17685,7 @@
         <v>10</v>
       </c>
       <c r="E1011" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1012" spans="1:6">
@@ -18161,7 +18161,7 @@
         <v>10</v>
       </c>
       <c r="E1048" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F1048" s="8"/>
     </row>
@@ -18278,7 +18278,7 @@
         <v>10</v>
       </c>
       <c r="E1055" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1056" spans="1:6">
@@ -18394,7 +18394,7 @@
         <v>10</v>
       </c>
       <c r="E1062" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1063" spans="1:7">
@@ -18530,7 +18530,7 @@
         <v>2023.8</v>
       </c>
       <c r="G1070" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1071" spans="1:7">
@@ -18550,7 +18550,7 @@
         <v>1905.5</v>
       </c>
       <c r="G1071" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1072" spans="1:7">
@@ -18570,7 +18570,7 @@
         <v>1864.1</v>
       </c>
       <c r="G1072" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1073" spans="1:7">
@@ -18590,7 +18590,7 @@
         <v>1957.2</v>
       </c>
       <c r="G1073" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1074" spans="1:7">
@@ -18610,7 +18610,7 @@
         <v>2079.6</v>
       </c>
       <c r="G1074" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1075" spans="1:7">
@@ -18630,7 +18630,7 @@
         <v>1550.3</v>
       </c>
       <c r="G1075" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1076" spans="1:7">
@@ -19135,7 +19135,7 @@
         <v>10</v>
       </c>
       <c r="E1114" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F1114" s="8"/>
     </row>
@@ -19252,7 +19252,7 @@
         <v>10</v>
       </c>
       <c r="E1121" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F1121" s="8"/>
     </row>
@@ -19369,7 +19369,7 @@
         <v>10</v>
       </c>
       <c r="E1128" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F1128" s="8"/>
     </row>
@@ -19486,10 +19486,10 @@
         <v>10</v>
       </c>
       <c r="E1135" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="G1135" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="1136" spans="1:7">
@@ -19506,7 +19506,7 @@
         <v>45</v>
       </c>
       <c r="G1136" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="1137" spans="1:7">
@@ -19526,7 +19526,7 @@
         <v>2012.7</v>
       </c>
       <c r="G1137" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1138" spans="1:7">
@@ -19546,7 +19546,7 @@
         <v>1896.4</v>
       </c>
       <c r="G1138" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1139" spans="1:7">
@@ -19566,7 +19566,7 @@
         <v>1856.2</v>
       </c>
       <c r="G1139" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1140" spans="1:7">
@@ -19586,7 +19586,7 @@
         <v>1948.5</v>
       </c>
       <c r="G1140" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1141" spans="1:7">
@@ -19606,7 +19606,7 @@
         <v>2069.1</v>
       </c>
       <c r="G1141" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1142" spans="1:7">
@@ -19626,7 +19626,7 @@
         <v>1529.5</v>
       </c>
       <c r="G1142" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="1143" spans="1:7">
@@ -20117,7 +20117,7 @@
         <v>10</v>
       </c>
       <c r="E1180" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1181" spans="1:6">
@@ -20233,7 +20233,7 @@
         <v>10</v>
       </c>
       <c r="E1187" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1188" spans="1:6">
@@ -20349,7 +20349,7 @@
         <v>10</v>
       </c>
       <c r="E1194" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="1195" spans="1:6">
@@ -20485,7 +20485,7 @@
         <v>2021.8</v>
       </c>
       <c r="G1202" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="1203" spans="1:7">
@@ -20505,7 +20505,7 @@
         <v>1903.6</v>
       </c>
       <c r="G1203" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="1204" spans="1:7">
@@ -20525,7 +20525,7 @@
         <v>1856.8</v>
       </c>
       <c r="G1204" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="1205" spans="1:7">
@@ -20545,7 +20545,7 @@
         <v>1952.9</v>
       </c>
       <c r="G1205" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="1206" spans="1:7">
@@ -20565,7 +20565,7 @@
         <v>2066.8000000000002</v>
       </c>
       <c r="G1206" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="1207" spans="1:7">
@@ -20585,7 +20585,7 @@
         <v>1542.3</v>
       </c>
       <c r="G1207" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="1208" spans="1:7">

</xml_diff>

<commit_message>
Added time data to mass msmts to eliminate warning
(Placeholder data that is.) Addresses issue #33
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24680" windowHeight="15600" activeTab="1"/>
@@ -351,8 +351,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="271">
+  <cellStyleXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -647,7 +649,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="271">
+  <cellStyles count="273">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -783,6 +785,7 @@
     <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -918,6 +921,7 @@
     <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1613,8 +1617,8 @@
   <dimension ref="A1:G1215"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A1193" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1196" sqref="C1196"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4395,7 +4399,9 @@
       <c r="A143" s="1">
         <v>42254</v>
       </c>
-      <c r="B143" s="5"/>
+      <c r="B143" s="6">
+        <v>0</v>
+      </c>
       <c r="D143" s="5"/>
       <c r="E143" t="s">
         <v>1</v>
@@ -4408,7 +4414,9 @@
       <c r="A144" s="1">
         <v>42254</v>
       </c>
-      <c r="B144" s="5"/>
+      <c r="B144" s="6">
+        <v>0</v>
+      </c>
       <c r="D144" s="5"/>
       <c r="E144" t="s">
         <v>2</v>
@@ -4421,7 +4429,9 @@
       <c r="A145" s="1">
         <v>42254</v>
       </c>
-      <c r="B145" s="5"/>
+      <c r="B145" s="6">
+        <v>0</v>
+      </c>
       <c r="D145" s="5"/>
       <c r="E145" t="s">
         <v>3</v>
@@ -4434,7 +4444,9 @@
       <c r="A146" s="1">
         <v>42254</v>
       </c>
-      <c r="B146" s="5"/>
+      <c r="B146" s="6">
+        <v>0</v>
+      </c>
       <c r="D146" s="5"/>
       <c r="E146" t="s">
         <v>4</v>
@@ -4447,7 +4459,9 @@
       <c r="A147" s="1">
         <v>42254</v>
       </c>
-      <c r="B147" s="5"/>
+      <c r="B147" s="6">
+        <v>0</v>
+      </c>
       <c r="D147" s="5"/>
       <c r="E147" t="s">
         <v>6</v>
@@ -4460,7 +4474,9 @@
       <c r="A148" s="1">
         <v>42254</v>
       </c>
-      <c r="B148" s="5"/>
+      <c r="B148" s="6">
+        <v>0</v>
+      </c>
       <c r="D148" s="5"/>
       <c r="E148" t="s">
         <v>7</v>
@@ -4473,7 +4489,9 @@
       <c r="A149" s="1">
         <v>42254</v>
       </c>
-      <c r="B149" s="5"/>
+      <c r="B149" s="6">
+        <v>0</v>
+      </c>
       <c r="D149" s="5"/>
       <c r="E149" t="s">
         <v>9</v>
@@ -4486,7 +4504,9 @@
       <c r="A150" s="1">
         <v>42254</v>
       </c>
-      <c r="B150" s="5"/>
+      <c r="B150" s="6">
+        <v>0</v>
+      </c>
       <c r="D150" s="5"/>
       <c r="E150" t="s">
         <v>11</v>
@@ -4499,7 +4519,9 @@
       <c r="A151" s="1">
         <v>42254</v>
       </c>
-      <c r="B151" s="5"/>
+      <c r="B151" s="6">
+        <v>0</v>
+      </c>
       <c r="D151" s="5"/>
       <c r="E151" t="s">
         <v>13</v>
@@ -4512,7 +4534,9 @@
       <c r="A152" s="1">
         <v>42254</v>
       </c>
-      <c r="B152" s="5"/>
+      <c r="B152" s="6">
+        <v>0</v>
+      </c>
       <c r="D152" s="5"/>
       <c r="E152" t="s">
         <v>15</v>
@@ -4525,7 +4549,9 @@
       <c r="A153" s="1">
         <v>42254</v>
       </c>
-      <c r="B153" s="5"/>
+      <c r="B153" s="6">
+        <v>0</v>
+      </c>
       <c r="D153" s="5"/>
       <c r="E153" t="s">
         <v>16</v>
@@ -4538,7 +4564,9 @@
       <c r="A154" s="1">
         <v>42254</v>
       </c>
-      <c r="B154" s="5"/>
+      <c r="B154" s="6">
+        <v>0</v>
+      </c>
       <c r="D154" s="5"/>
       <c r="E154" t="s">
         <v>17</v>
@@ -4551,7 +4579,9 @@
       <c r="A155" s="1">
         <v>42254</v>
       </c>
-      <c r="B155" s="5"/>
+      <c r="B155" s="6">
+        <v>0</v>
+      </c>
       <c r="D155" s="5"/>
       <c r="E155" t="s">
         <v>18</v>
@@ -4564,7 +4594,9 @@
       <c r="A156" s="1">
         <v>42254</v>
       </c>
-      <c r="B156" s="5"/>
+      <c r="B156" s="6">
+        <v>0</v>
+      </c>
       <c r="D156" s="5"/>
       <c r="E156" t="s">
         <v>19</v>
@@ -4577,7 +4609,9 @@
       <c r="A157" s="1">
         <v>42254</v>
       </c>
-      <c r="B157" s="5"/>
+      <c r="B157" s="6">
+        <v>0</v>
+      </c>
       <c r="D157" s="5"/>
       <c r="E157" t="s">
         <v>20</v>
@@ -4590,7 +4624,9 @@
       <c r="A158" s="1">
         <v>42254</v>
       </c>
-      <c r="B158" s="5"/>
+      <c r="B158" s="6">
+        <v>0</v>
+      </c>
       <c r="D158" s="5"/>
       <c r="E158" t="s">
         <v>21</v>
@@ -4603,7 +4639,9 @@
       <c r="A159" s="1">
         <v>42254</v>
       </c>
-      <c r="B159" s="5"/>
+      <c r="B159" s="6">
+        <v>0</v>
+      </c>
       <c r="D159" s="5"/>
       <c r="E159" t="s">
         <v>22</v>
@@ -4616,7 +4654,9 @@
       <c r="A160" s="1">
         <v>42254</v>
       </c>
-      <c r="B160" s="5"/>
+      <c r="B160" s="6">
+        <v>0</v>
+      </c>
       <c r="D160" s="5"/>
       <c r="E160" t="s">
         <v>23</v>
@@ -4629,7 +4669,9 @@
       <c r="A161" s="1">
         <v>42254</v>
       </c>
-      <c r="B161" s="5"/>
+      <c r="B161" s="6">
+        <v>0</v>
+      </c>
       <c r="D161" s="5"/>
       <c r="E161" t="s">
         <v>5</v>
@@ -4642,7 +4684,9 @@
       <c r="A162" s="1">
         <v>42254</v>
       </c>
-      <c r="B162" s="5"/>
+      <c r="B162" s="6">
+        <v>0</v>
+      </c>
       <c r="D162" s="5"/>
       <c r="E162" t="s">
         <v>24</v>
@@ -4655,7 +4699,9 @@
       <c r="A163" s="1">
         <v>42254</v>
       </c>
-      <c r="B163" s="5"/>
+      <c r="B163" s="6">
+        <v>0</v>
+      </c>
       <c r="D163" s="5"/>
       <c r="E163" t="s">
         <v>8</v>
@@ -4668,7 +4714,9 @@
       <c r="A164" s="1">
         <v>42254</v>
       </c>
-      <c r="B164" s="5"/>
+      <c r="B164" s="6">
+        <v>0</v>
+      </c>
       <c r="D164" s="5"/>
       <c r="E164" t="s">
         <v>10</v>
@@ -4681,7 +4729,9 @@
       <c r="A165" s="1">
         <v>42254</v>
       </c>
-      <c r="B165" s="5"/>
+      <c r="B165" s="6">
+        <v>0</v>
+      </c>
       <c r="D165" s="5"/>
       <c r="E165" t="s">
         <v>12</v>
@@ -4694,7 +4744,9 @@
       <c r="A166" s="1">
         <v>42254</v>
       </c>
-      <c r="B166" s="5"/>
+      <c r="B166" s="6">
+        <v>0</v>
+      </c>
       <c r="D166" s="5"/>
       <c r="E166" t="s">
         <v>14</v>
@@ -4707,7 +4759,9 @@
       <c r="A167" s="1">
         <v>42254</v>
       </c>
-      <c r="B167" s="5"/>
+      <c r="B167" s="6">
+        <v>0</v>
+      </c>
       <c r="D167" s="5"/>
       <c r="E167" t="s">
         <v>25</v>
@@ -4720,7 +4774,9 @@
       <c r="A168" s="1">
         <v>42254</v>
       </c>
-      <c r="B168" s="5"/>
+      <c r="B168" s="6">
+        <v>0</v>
+      </c>
       <c r="D168" s="5"/>
       <c r="E168" t="s">
         <v>26</v>
@@ -4733,7 +4789,9 @@
       <c r="A169" s="1">
         <v>42254</v>
       </c>
-      <c r="B169" s="5"/>
+      <c r="B169" s="6">
+        <v>0</v>
+      </c>
       <c r="D169" s="5"/>
       <c r="E169" t="s">
         <v>27</v>
@@ -4746,7 +4804,9 @@
       <c r="A170" s="1">
         <v>42254</v>
       </c>
-      <c r="B170" s="5"/>
+      <c r="B170" s="6">
+        <v>0</v>
+      </c>
       <c r="D170" s="5"/>
       <c r="E170" t="s">
         <v>28</v>
@@ -4759,7 +4819,9 @@
       <c r="A171" s="1">
         <v>42254</v>
       </c>
-      <c r="B171" s="5"/>
+      <c r="B171" s="6">
+        <v>0</v>
+      </c>
       <c r="D171" s="5"/>
       <c r="E171" t="s">
         <v>29</v>
@@ -4772,7 +4834,9 @@
       <c r="A172" s="1">
         <v>42254</v>
       </c>
-      <c r="B172" s="5"/>
+      <c r="B172" s="6">
+        <v>0</v>
+      </c>
       <c r="D172" s="5"/>
       <c r="E172" t="s">
         <v>30</v>
@@ -5396,7 +5460,9 @@
       <c r="A210" s="1">
         <v>42257</v>
       </c>
-      <c r="B210" s="5"/>
+      <c r="B210" s="6">
+        <v>0</v>
+      </c>
       <c r="D210" s="5"/>
       <c r="E210" t="s">
         <v>1</v>
@@ -5409,7 +5475,9 @@
       <c r="A211" s="1">
         <v>42257</v>
       </c>
-      <c r="B211" s="5"/>
+      <c r="B211" s="6">
+        <v>0</v>
+      </c>
       <c r="D211" s="5"/>
       <c r="E211" t="s">
         <v>2</v>
@@ -5422,7 +5490,9 @@
       <c r="A212" s="1">
         <v>42257</v>
       </c>
-      <c r="B212" s="5"/>
+      <c r="B212" s="6">
+        <v>0</v>
+      </c>
       <c r="D212" s="5"/>
       <c r="E212" t="s">
         <v>3</v>
@@ -5435,7 +5505,9 @@
       <c r="A213" s="1">
         <v>42257</v>
       </c>
-      <c r="B213" s="5"/>
+      <c r="B213" s="6">
+        <v>0</v>
+      </c>
       <c r="D213" s="5"/>
       <c r="E213" t="s">
         <v>4</v>
@@ -5448,7 +5520,9 @@
       <c r="A214" s="1">
         <v>42257</v>
       </c>
-      <c r="B214" s="5"/>
+      <c r="B214" s="6">
+        <v>0</v>
+      </c>
       <c r="D214" s="5"/>
       <c r="E214" t="s">
         <v>6</v>
@@ -5461,7 +5535,9 @@
       <c r="A215" s="1">
         <v>42257</v>
       </c>
-      <c r="B215" s="5"/>
+      <c r="B215" s="6">
+        <v>0</v>
+      </c>
       <c r="D215" s="5"/>
       <c r="E215" t="s">
         <v>7</v>
@@ -5474,7 +5550,9 @@
       <c r="A216" s="1">
         <v>42257</v>
       </c>
-      <c r="B216" s="5"/>
+      <c r="B216" s="6">
+        <v>0</v>
+      </c>
       <c r="D216" s="5"/>
       <c r="E216" t="s">
         <v>9</v>
@@ -5487,7 +5565,9 @@
       <c r="A217" s="1">
         <v>42257</v>
       </c>
-      <c r="B217" s="5"/>
+      <c r="B217" s="6">
+        <v>0</v>
+      </c>
       <c r="D217" s="5"/>
       <c r="E217" t="s">
         <v>11</v>
@@ -5500,7 +5580,9 @@
       <c r="A218" s="1">
         <v>42257</v>
       </c>
-      <c r="B218" s="5"/>
+      <c r="B218" s="6">
+        <v>0</v>
+      </c>
       <c r="D218" s="5"/>
       <c r="E218" t="s">
         <v>13</v>
@@ -5513,7 +5595,9 @@
       <c r="A219" s="1">
         <v>42257</v>
       </c>
-      <c r="B219" s="5"/>
+      <c r="B219" s="6">
+        <v>0</v>
+      </c>
       <c r="D219" s="5"/>
       <c r="E219" t="s">
         <v>15</v>
@@ -5526,7 +5610,9 @@
       <c r="A220" s="1">
         <v>42257</v>
       </c>
-      <c r="B220" s="5"/>
+      <c r="B220" s="6">
+        <v>0</v>
+      </c>
       <c r="D220" s="5"/>
       <c r="E220" t="s">
         <v>16</v>
@@ -5539,7 +5625,9 @@
       <c r="A221" s="1">
         <v>42257</v>
       </c>
-      <c r="B221" s="5"/>
+      <c r="B221" s="6">
+        <v>0</v>
+      </c>
       <c r="D221" s="5"/>
       <c r="E221" t="s">
         <v>17</v>
@@ -5552,7 +5640,9 @@
       <c r="A222" s="1">
         <v>42257</v>
       </c>
-      <c r="B222" s="5"/>
+      <c r="B222" s="6">
+        <v>0</v>
+      </c>
       <c r="D222" s="5"/>
       <c r="E222" t="s">
         <v>18</v>
@@ -5565,7 +5655,9 @@
       <c r="A223" s="1">
         <v>42257</v>
       </c>
-      <c r="B223" s="5"/>
+      <c r="B223" s="6">
+        <v>0</v>
+      </c>
       <c r="D223" s="5"/>
       <c r="E223" t="s">
         <v>19</v>
@@ -5578,7 +5670,9 @@
       <c r="A224" s="1">
         <v>42257</v>
       </c>
-      <c r="B224" s="5"/>
+      <c r="B224" s="6">
+        <v>0</v>
+      </c>
       <c r="D224" s="5"/>
       <c r="E224" t="s">
         <v>20</v>
@@ -5591,7 +5685,9 @@
       <c r="A225" s="1">
         <v>42257</v>
       </c>
-      <c r="B225" s="5"/>
+      <c r="B225" s="6">
+        <v>0</v>
+      </c>
       <c r="D225" s="5"/>
       <c r="E225" t="s">
         <v>21</v>
@@ -5604,7 +5700,9 @@
       <c r="A226" s="1">
         <v>42257</v>
       </c>
-      <c r="B226" s="5"/>
+      <c r="B226" s="6">
+        <v>0</v>
+      </c>
       <c r="D226" s="5"/>
       <c r="E226" t="s">
         <v>22</v>
@@ -5617,7 +5715,9 @@
       <c r="A227" s="1">
         <v>42257</v>
       </c>
-      <c r="B227" s="5"/>
+      <c r="B227" s="6">
+        <v>0</v>
+      </c>
       <c r="D227" s="5"/>
       <c r="E227" t="s">
         <v>23</v>
@@ -5630,7 +5730,9 @@
       <c r="A228" s="1">
         <v>42257</v>
       </c>
-      <c r="B228" s="5"/>
+      <c r="B228" s="6">
+        <v>0</v>
+      </c>
       <c r="D228" s="5"/>
       <c r="E228" t="s">
         <v>5</v>
@@ -5643,7 +5745,9 @@
       <c r="A229" s="1">
         <v>42257</v>
       </c>
-      <c r="B229" s="5"/>
+      <c r="B229" s="6">
+        <v>0</v>
+      </c>
       <c r="D229" s="5"/>
       <c r="E229" t="s">
         <v>24</v>
@@ -5656,7 +5760,9 @@
       <c r="A230" s="1">
         <v>42257</v>
       </c>
-      <c r="B230" s="5"/>
+      <c r="B230" s="6">
+        <v>0</v>
+      </c>
       <c r="D230" s="5"/>
       <c r="E230" t="s">
         <v>8</v>
@@ -5669,7 +5775,9 @@
       <c r="A231" s="1">
         <v>42257</v>
       </c>
-      <c r="B231" s="5"/>
+      <c r="B231" s="6">
+        <v>0</v>
+      </c>
       <c r="D231" s="5"/>
       <c r="E231" t="s">
         <v>10</v>
@@ -5682,7 +5790,9 @@
       <c r="A232" s="1">
         <v>42257</v>
       </c>
-      <c r="B232" s="5"/>
+      <c r="B232" s="6">
+        <v>0</v>
+      </c>
       <c r="D232" s="5"/>
       <c r="E232" t="s">
         <v>12</v>
@@ -5695,7 +5805,9 @@
       <c r="A233" s="1">
         <v>42257</v>
       </c>
-      <c r="B233" s="5"/>
+      <c r="B233" s="6">
+        <v>0</v>
+      </c>
       <c r="D233" s="5"/>
       <c r="E233" t="s">
         <v>14</v>
@@ -5708,7 +5820,9 @@
       <c r="A234" s="1">
         <v>42257</v>
       </c>
-      <c r="B234" s="5"/>
+      <c r="B234" s="6">
+        <v>0</v>
+      </c>
       <c r="D234" s="5"/>
       <c r="E234" t="s">
         <v>25</v>
@@ -5721,7 +5835,9 @@
       <c r="A235" s="1">
         <v>42257</v>
       </c>
-      <c r="B235" s="5"/>
+      <c r="B235" s="6">
+        <v>0</v>
+      </c>
       <c r="D235" s="5"/>
       <c r="E235" t="s">
         <v>26</v>
@@ -5734,7 +5850,9 @@
       <c r="A236" s="1">
         <v>42257</v>
       </c>
-      <c r="B236" s="5"/>
+      <c r="B236" s="6">
+        <v>0</v>
+      </c>
       <c r="D236" s="5"/>
       <c r="E236" t="s">
         <v>27</v>
@@ -5747,7 +5865,9 @@
       <c r="A237" s="1">
         <v>42257</v>
       </c>
-      <c r="B237" s="5"/>
+      <c r="B237" s="6">
+        <v>0</v>
+      </c>
       <c r="D237" s="5"/>
       <c r="E237" t="s">
         <v>28</v>
@@ -5760,7 +5880,9 @@
       <c r="A238" s="1">
         <v>42257</v>
       </c>
-      <c r="B238" s="5"/>
+      <c r="B238" s="6">
+        <v>0</v>
+      </c>
       <c r="D238" s="5"/>
       <c r="E238" t="s">
         <v>29</v>
@@ -5773,7 +5895,9 @@
       <c r="A239" s="1">
         <v>42257</v>
       </c>
-      <c r="B239" s="5"/>
+      <c r="B239" s="6">
+        <v>0</v>
+      </c>
       <c r="D239" s="5"/>
       <c r="E239" t="s">
         <v>30</v>
@@ -6398,7 +6522,9 @@
       <c r="A276" s="1">
         <v>42261</v>
       </c>
-      <c r="B276" s="5"/>
+      <c r="B276" s="6">
+        <v>0</v>
+      </c>
       <c r="D276" s="5"/>
       <c r="E276" t="s">
         <v>1</v>
@@ -6411,7 +6537,9 @@
       <c r="A277" s="1">
         <v>42261</v>
       </c>
-      <c r="B277" s="5"/>
+      <c r="B277" s="6">
+        <v>0</v>
+      </c>
       <c r="D277" s="5"/>
       <c r="E277" t="s">
         <v>2</v>
@@ -6424,7 +6552,9 @@
       <c r="A278" s="1">
         <v>42261</v>
       </c>
-      <c r="B278" s="5"/>
+      <c r="B278" s="6">
+        <v>0</v>
+      </c>
       <c r="D278" s="5"/>
       <c r="E278" t="s">
         <v>3</v>
@@ -6437,7 +6567,9 @@
       <c r="A279" s="1">
         <v>42261</v>
       </c>
-      <c r="B279" s="5"/>
+      <c r="B279" s="6">
+        <v>0</v>
+      </c>
       <c r="D279" s="5"/>
       <c r="E279" t="s">
         <v>4</v>
@@ -6450,7 +6582,9 @@
       <c r="A280" s="1">
         <v>42261</v>
       </c>
-      <c r="B280" s="5"/>
+      <c r="B280" s="6">
+        <v>0</v>
+      </c>
       <c r="D280" s="5"/>
       <c r="E280" t="s">
         <v>6</v>
@@ -6463,7 +6597,9 @@
       <c r="A281" s="1">
         <v>42261</v>
       </c>
-      <c r="B281" s="5"/>
+      <c r="B281" s="6">
+        <v>0</v>
+      </c>
       <c r="D281" s="5"/>
       <c r="E281" t="s">
         <v>7</v>
@@ -6476,7 +6612,9 @@
       <c r="A282" s="1">
         <v>42261</v>
       </c>
-      <c r="B282" s="5"/>
+      <c r="B282" s="6">
+        <v>0</v>
+      </c>
       <c r="D282" s="5"/>
       <c r="E282" t="s">
         <v>9</v>
@@ -6489,7 +6627,9 @@
       <c r="A283" s="1">
         <v>42261</v>
       </c>
-      <c r="B283" s="5"/>
+      <c r="B283" s="6">
+        <v>0</v>
+      </c>
       <c r="D283" s="5"/>
       <c r="E283" t="s">
         <v>11</v>
@@ -6502,7 +6642,9 @@
       <c r="A284" s="1">
         <v>42261</v>
       </c>
-      <c r="B284" s="5"/>
+      <c r="B284" s="6">
+        <v>0</v>
+      </c>
       <c r="D284" s="5"/>
       <c r="E284" t="s">
         <v>13</v>
@@ -6515,7 +6657,9 @@
       <c r="A285" s="1">
         <v>42261</v>
       </c>
-      <c r="B285" s="5"/>
+      <c r="B285" s="6">
+        <v>0</v>
+      </c>
       <c r="D285" s="5"/>
       <c r="E285" t="s">
         <v>15</v>
@@ -6528,7 +6672,9 @@
       <c r="A286" s="1">
         <v>42261</v>
       </c>
-      <c r="B286" s="5"/>
+      <c r="B286" s="6">
+        <v>0</v>
+      </c>
       <c r="D286" s="5"/>
       <c r="E286" t="s">
         <v>16</v>
@@ -6541,7 +6687,9 @@
       <c r="A287" s="1">
         <v>42261</v>
       </c>
-      <c r="B287" s="5"/>
+      <c r="B287" s="6">
+        <v>0</v>
+      </c>
       <c r="D287" s="5"/>
       <c r="E287" t="s">
         <v>17</v>
@@ -6554,7 +6702,9 @@
       <c r="A288" s="1">
         <v>42261</v>
       </c>
-      <c r="B288" s="5"/>
+      <c r="B288" s="6">
+        <v>0</v>
+      </c>
       <c r="D288" s="5"/>
       <c r="E288" t="s">
         <v>18</v>
@@ -6567,7 +6717,9 @@
       <c r="A289" s="1">
         <v>42261</v>
       </c>
-      <c r="B289" s="5"/>
+      <c r="B289" s="6">
+        <v>0</v>
+      </c>
       <c r="D289" s="5"/>
       <c r="E289" t="s">
         <v>19</v>
@@ -6580,7 +6732,9 @@
       <c r="A290" s="1">
         <v>42261</v>
       </c>
-      <c r="B290" s="5"/>
+      <c r="B290" s="6">
+        <v>0</v>
+      </c>
       <c r="D290" s="5"/>
       <c r="E290" t="s">
         <v>20</v>
@@ -6593,7 +6747,9 @@
       <c r="A291" s="1">
         <v>42261</v>
       </c>
-      <c r="B291" s="5"/>
+      <c r="B291" s="6">
+        <v>0</v>
+      </c>
       <c r="D291" s="5"/>
       <c r="E291" t="s">
         <v>21</v>
@@ -6606,7 +6762,9 @@
       <c r="A292" s="1">
         <v>42261</v>
       </c>
-      <c r="B292" s="5"/>
+      <c r="B292" s="6">
+        <v>0</v>
+      </c>
       <c r="D292" s="5"/>
       <c r="E292" t="s">
         <v>22</v>
@@ -6619,7 +6777,9 @@
       <c r="A293" s="1">
         <v>42261</v>
       </c>
-      <c r="B293" s="5"/>
+      <c r="B293" s="6">
+        <v>0</v>
+      </c>
       <c r="D293" s="5"/>
       <c r="E293" t="s">
         <v>23</v>
@@ -6632,7 +6792,9 @@
       <c r="A294" s="1">
         <v>42261</v>
       </c>
-      <c r="B294" s="5"/>
+      <c r="B294" s="6">
+        <v>0</v>
+      </c>
       <c r="D294" s="5"/>
       <c r="E294" t="s">
         <v>5</v>
@@ -6645,7 +6807,9 @@
       <c r="A295" s="1">
         <v>42261</v>
       </c>
-      <c r="B295" s="5"/>
+      <c r="B295" s="6">
+        <v>0</v>
+      </c>
       <c r="D295" s="5"/>
       <c r="E295" t="s">
         <v>24</v>
@@ -6658,7 +6822,9 @@
       <c r="A296" s="1">
         <v>42261</v>
       </c>
-      <c r="B296" s="5"/>
+      <c r="B296" s="6">
+        <v>0</v>
+      </c>
       <c r="D296" s="5"/>
       <c r="E296" t="s">
         <v>8</v>
@@ -6671,7 +6837,9 @@
       <c r="A297" s="1">
         <v>42261</v>
       </c>
-      <c r="B297" s="5"/>
+      <c r="B297" s="6">
+        <v>0</v>
+      </c>
       <c r="D297" s="5"/>
       <c r="E297" t="s">
         <v>10</v>
@@ -6684,7 +6852,9 @@
       <c r="A298" s="1">
         <v>42261</v>
       </c>
-      <c r="B298" s="5"/>
+      <c r="B298" s="6">
+        <v>0</v>
+      </c>
       <c r="D298" s="5"/>
       <c r="E298" t="s">
         <v>12</v>
@@ -6697,7 +6867,9 @@
       <c r="A299" s="1">
         <v>42261</v>
       </c>
-      <c r="B299" s="5"/>
+      <c r="B299" s="6">
+        <v>0</v>
+      </c>
       <c r="D299" s="5"/>
       <c r="E299" t="s">
         <v>14</v>
@@ -6710,7 +6882,9 @@
       <c r="A300" s="1">
         <v>42261</v>
       </c>
-      <c r="B300" s="5"/>
+      <c r="B300" s="6">
+        <v>0</v>
+      </c>
       <c r="D300" s="5"/>
       <c r="E300" t="s">
         <v>25</v>
@@ -6723,7 +6897,9 @@
       <c r="A301" s="1">
         <v>42261</v>
       </c>
-      <c r="B301" s="5"/>
+      <c r="B301" s="6">
+        <v>0</v>
+      </c>
       <c r="D301" s="5"/>
       <c r="E301" t="s">
         <v>26</v>
@@ -6736,7 +6912,9 @@
       <c r="A302" s="1">
         <v>42261</v>
       </c>
-      <c r="B302" s="5"/>
+      <c r="B302" s="6">
+        <v>0</v>
+      </c>
       <c r="D302" s="5"/>
       <c r="E302" t="s">
         <v>27</v>
@@ -6749,7 +6927,9 @@
       <c r="A303" s="1">
         <v>42261</v>
       </c>
-      <c r="B303" s="5"/>
+      <c r="B303" s="6">
+        <v>0</v>
+      </c>
       <c r="D303" s="5"/>
       <c r="E303" t="s">
         <v>28</v>
@@ -6762,7 +6942,9 @@
       <c r="A304" s="1">
         <v>42261</v>
       </c>
-      <c r="B304" s="5"/>
+      <c r="B304" s="6">
+        <v>0</v>
+      </c>
       <c r="D304" s="5"/>
       <c r="E304" t="s">
         <v>29</v>
@@ -6775,7 +6957,9 @@
       <c r="A305" s="1">
         <v>42261</v>
       </c>
-      <c r="B305" s="5"/>
+      <c r="B305" s="6">
+        <v>0</v>
+      </c>
       <c r="D305" s="5"/>
       <c r="E305" t="s">
         <v>30</v>
@@ -7980,7 +8164,9 @@
       <c r="A377" s="1">
         <v>42268</v>
       </c>
-      <c r="B377" s="5"/>
+      <c r="B377" s="6">
+        <v>0</v>
+      </c>
       <c r="C377" s="5"/>
       <c r="E377" t="s">
         <v>1</v>
@@ -7996,7 +8182,9 @@
       <c r="A378" s="1">
         <v>42268</v>
       </c>
-      <c r="B378" s="5"/>
+      <c r="B378" s="6">
+        <v>0</v>
+      </c>
       <c r="C378" s="5"/>
       <c r="E378" t="s">
         <v>2</v>
@@ -8012,7 +8200,9 @@
       <c r="A379" s="1">
         <v>42268</v>
       </c>
-      <c r="B379" s="5"/>
+      <c r="B379" s="6">
+        <v>0</v>
+      </c>
       <c r="C379" s="5"/>
       <c r="E379" t="s">
         <v>3</v>
@@ -8028,7 +8218,9 @@
       <c r="A380" s="1">
         <v>42268</v>
       </c>
-      <c r="B380" s="5"/>
+      <c r="B380" s="6">
+        <v>0</v>
+      </c>
       <c r="C380" s="5"/>
       <c r="E380" t="s">
         <v>4</v>
@@ -8044,7 +8236,9 @@
       <c r="A381" s="1">
         <v>42268</v>
       </c>
-      <c r="B381" s="5"/>
+      <c r="B381" s="6">
+        <v>0</v>
+      </c>
       <c r="C381" s="5"/>
       <c r="E381" t="s">
         <v>6</v>
@@ -8060,7 +8254,9 @@
       <c r="A382" s="1">
         <v>42268</v>
       </c>
-      <c r="B382" s="5"/>
+      <c r="B382" s="6">
+        <v>0</v>
+      </c>
       <c r="C382" s="5"/>
       <c r="E382" t="s">
         <v>7</v>
@@ -8076,7 +8272,9 @@
       <c r="A383" s="1">
         <v>42268</v>
       </c>
-      <c r="B383" s="5"/>
+      <c r="B383" s="6">
+        <v>0</v>
+      </c>
       <c r="C383" s="5"/>
       <c r="E383" t="s">
         <v>9</v>
@@ -8092,7 +8290,9 @@
       <c r="A384" s="1">
         <v>42268</v>
       </c>
-      <c r="B384" s="5"/>
+      <c r="B384" s="6">
+        <v>0</v>
+      </c>
       <c r="C384" s="5"/>
       <c r="E384" t="s">
         <v>11</v>
@@ -8108,7 +8308,9 @@
       <c r="A385" s="1">
         <v>42268</v>
       </c>
-      <c r="B385" s="5"/>
+      <c r="B385" s="6">
+        <v>0</v>
+      </c>
       <c r="C385" s="5"/>
       <c r="E385" t="s">
         <v>13</v>
@@ -8121,7 +8323,9 @@
       <c r="A386" s="1">
         <v>42268</v>
       </c>
-      <c r="B386" s="5"/>
+      <c r="B386" s="6">
+        <v>0</v>
+      </c>
       <c r="C386" s="5"/>
       <c r="E386" t="s">
         <v>15</v>
@@ -8134,7 +8338,9 @@
       <c r="A387" s="1">
         <v>42268</v>
       </c>
-      <c r="B387" s="5"/>
+      <c r="B387" s="6">
+        <v>0</v>
+      </c>
       <c r="C387" s="5"/>
       <c r="E387" t="s">
         <v>16</v>
@@ -8150,7 +8356,9 @@
       <c r="A388" s="1">
         <v>42268</v>
       </c>
-      <c r="B388" s="5"/>
+      <c r="B388" s="6">
+        <v>0</v>
+      </c>
       <c r="C388" s="5"/>
       <c r="E388" t="s">
         <v>17</v>
@@ -8163,7 +8371,9 @@
       <c r="A389" s="1">
         <v>42268</v>
       </c>
-      <c r="B389" s="5"/>
+      <c r="B389" s="6">
+        <v>0</v>
+      </c>
       <c r="C389" s="5"/>
       <c r="E389" t="s">
         <v>18</v>
@@ -8179,7 +8389,9 @@
       <c r="A390" s="1">
         <v>42268</v>
       </c>
-      <c r="B390" s="5"/>
+      <c r="B390" s="6">
+        <v>0</v>
+      </c>
       <c r="C390" s="5"/>
       <c r="E390" t="s">
         <v>19</v>
@@ -8195,7 +8407,9 @@
       <c r="A391" s="1">
         <v>42268</v>
       </c>
-      <c r="B391" s="5"/>
+      <c r="B391" s="6">
+        <v>0</v>
+      </c>
       <c r="C391" s="5"/>
       <c r="E391" t="s">
         <v>20</v>
@@ -8211,7 +8425,9 @@
       <c r="A392" s="1">
         <v>42268</v>
       </c>
-      <c r="B392" s="5"/>
+      <c r="B392" s="6">
+        <v>0</v>
+      </c>
       <c r="C392" s="5"/>
       <c r="E392" t="s">
         <v>21</v>
@@ -8227,7 +8443,9 @@
       <c r="A393" s="1">
         <v>42268</v>
       </c>
-      <c r="B393" s="5"/>
+      <c r="B393" s="6">
+        <v>0</v>
+      </c>
       <c r="C393" s="5"/>
       <c r="E393" t="s">
         <v>22</v>
@@ -8243,7 +8461,9 @@
       <c r="A394" s="1">
         <v>42268</v>
       </c>
-      <c r="B394" s="5"/>
+      <c r="B394" s="6">
+        <v>0</v>
+      </c>
       <c r="C394" s="5"/>
       <c r="E394" t="s">
         <v>23</v>
@@ -8259,7 +8479,9 @@
       <c r="A395" s="1">
         <v>42268</v>
       </c>
-      <c r="B395" s="5"/>
+      <c r="B395" s="6">
+        <v>0</v>
+      </c>
       <c r="C395" s="5"/>
       <c r="E395" t="s">
         <v>25</v>
@@ -8272,7 +8494,9 @@
       <c r="A396" s="1">
         <v>42268</v>
       </c>
-      <c r="B396" s="5"/>
+      <c r="B396" s="6">
+        <v>0</v>
+      </c>
       <c r="C396" s="5"/>
       <c r="E396" t="s">
         <v>26</v>
@@ -8285,7 +8509,9 @@
       <c r="A397" s="1">
         <v>42268</v>
       </c>
-      <c r="B397" s="5"/>
+      <c r="B397" s="6">
+        <v>0</v>
+      </c>
       <c r="C397" s="5"/>
       <c r="E397" t="s">
         <v>27</v>
@@ -8298,7 +8524,9 @@
       <c r="A398" s="1">
         <v>42268</v>
       </c>
-      <c r="B398" s="5"/>
+      <c r="B398" s="6">
+        <v>0</v>
+      </c>
       <c r="C398" s="5"/>
       <c r="E398" t="s">
         <v>28</v>
@@ -8311,7 +8539,9 @@
       <c r="A399" s="1">
         <v>42268</v>
       </c>
-      <c r="B399" s="5"/>
+      <c r="B399" s="6">
+        <v>0</v>
+      </c>
       <c r="C399" s="5"/>
       <c r="E399" t="s">
         <v>29</v>
@@ -8324,7 +8554,9 @@
       <c r="A400" s="1">
         <v>42268</v>
       </c>
-      <c r="B400" s="5"/>
+      <c r="B400" s="6">
+        <v>0</v>
+      </c>
       <c r="C400" s="5"/>
       <c r="E400" t="s">
         <v>30</v>
@@ -8337,7 +8569,9 @@
       <c r="A401" s="1">
         <v>42268</v>
       </c>
-      <c r="B401" s="5"/>
+      <c r="B401" s="6">
+        <v>0</v>
+      </c>
       <c r="C401" s="5"/>
       <c r="E401" t="s">
         <v>5</v>
@@ -8353,7 +8587,9 @@
       <c r="A402" s="1">
         <v>42268</v>
       </c>
-      <c r="B402" s="5"/>
+      <c r="B402" s="6">
+        <v>0</v>
+      </c>
       <c r="C402" s="5"/>
       <c r="E402" t="s">
         <v>24</v>
@@ -8369,7 +8605,9 @@
       <c r="A403" s="1">
         <v>42268</v>
       </c>
-      <c r="B403" s="5"/>
+      <c r="B403" s="6">
+        <v>0</v>
+      </c>
       <c r="C403" s="5"/>
       <c r="E403" t="s">
         <v>8</v>
@@ -8385,7 +8623,9 @@
       <c r="A404" s="1">
         <v>42268</v>
       </c>
-      <c r="B404" s="5"/>
+      <c r="B404" s="6">
+        <v>0</v>
+      </c>
       <c r="C404" s="5"/>
       <c r="E404" t="s">
         <v>10</v>
@@ -8401,7 +8641,9 @@
       <c r="A405" s="1">
         <v>42268</v>
       </c>
-      <c r="B405" s="5"/>
+      <c r="B405" s="6">
+        <v>0</v>
+      </c>
       <c r="C405" s="5"/>
       <c r="E405" t="s">
         <v>12</v>
@@ -8414,7 +8656,9 @@
       <c r="A406" s="1">
         <v>42268</v>
       </c>
-      <c r="B406" s="5"/>
+      <c r="B406" s="6">
+        <v>0</v>
+      </c>
       <c r="C406" s="5"/>
       <c r="E406" t="s">
         <v>14</v>
@@ -9191,7 +9435,9 @@
       <c r="A450" s="1">
         <v>42271</v>
       </c>
-      <c r="B450" s="5"/>
+      <c r="B450" s="6">
+        <v>0</v>
+      </c>
       <c r="D450" s="5"/>
       <c r="E450" t="s">
         <v>1</v>
@@ -9204,7 +9450,9 @@
       <c r="A451" s="1">
         <v>42271</v>
       </c>
-      <c r="B451" s="5"/>
+      <c r="B451" s="6">
+        <v>0</v>
+      </c>
       <c r="D451" s="5"/>
       <c r="E451" t="s">
         <v>2</v>
@@ -9217,7 +9465,9 @@
       <c r="A452" s="1">
         <v>42271</v>
       </c>
-      <c r="B452" s="5"/>
+      <c r="B452" s="6">
+        <v>0</v>
+      </c>
       <c r="D452" s="5"/>
       <c r="E452" t="s">
         <v>3</v>
@@ -9230,7 +9480,9 @@
       <c r="A453" s="1">
         <v>42271</v>
       </c>
-      <c r="B453" s="5"/>
+      <c r="B453" s="6">
+        <v>0</v>
+      </c>
       <c r="D453" s="5"/>
       <c r="E453" t="s">
         <v>4</v>
@@ -9243,7 +9495,9 @@
       <c r="A454" s="1">
         <v>42271</v>
       </c>
-      <c r="B454" s="5"/>
+      <c r="B454" s="6">
+        <v>0</v>
+      </c>
       <c r="D454" s="5"/>
       <c r="E454" t="s">
         <v>6</v>
@@ -9256,7 +9510,9 @@
       <c r="A455" s="1">
         <v>42271</v>
       </c>
-      <c r="B455" s="5"/>
+      <c r="B455" s="6">
+        <v>0</v>
+      </c>
       <c r="D455" s="5"/>
       <c r="E455" t="s">
         <v>7</v>
@@ -9269,7 +9525,9 @@
       <c r="A456" s="1">
         <v>42271</v>
       </c>
-      <c r="B456" s="5"/>
+      <c r="B456" s="6">
+        <v>0</v>
+      </c>
       <c r="D456" s="5"/>
       <c r="E456" t="s">
         <v>9</v>
@@ -9282,7 +9540,9 @@
       <c r="A457" s="1">
         <v>42271</v>
       </c>
-      <c r="B457" s="5"/>
+      <c r="B457" s="6">
+        <v>0</v>
+      </c>
       <c r="D457" s="5"/>
       <c r="E457" t="s">
         <v>11</v>
@@ -9295,7 +9555,9 @@
       <c r="A458" s="1">
         <v>42271</v>
       </c>
-      <c r="B458" s="5"/>
+      <c r="B458" s="6">
+        <v>0</v>
+      </c>
       <c r="D458" s="5"/>
       <c r="E458" t="s">
         <v>13</v>
@@ -9308,7 +9570,9 @@
       <c r="A459" s="1">
         <v>42271</v>
       </c>
-      <c r="B459" s="5"/>
+      <c r="B459" s="6">
+        <v>0</v>
+      </c>
       <c r="D459" s="5"/>
       <c r="E459" t="s">
         <v>15</v>
@@ -9321,7 +9585,9 @@
       <c r="A460" s="1">
         <v>42271</v>
       </c>
-      <c r="B460" s="5"/>
+      <c r="B460" s="6">
+        <v>0</v>
+      </c>
       <c r="D460" s="5"/>
       <c r="E460" t="s">
         <v>16</v>
@@ -9334,7 +9600,9 @@
       <c r="A461" s="1">
         <v>42271</v>
       </c>
-      <c r="B461" s="5"/>
+      <c r="B461" s="6">
+        <v>0</v>
+      </c>
       <c r="D461" s="5"/>
       <c r="E461" t="s">
         <v>17</v>
@@ -9347,7 +9615,9 @@
       <c r="A462" s="1">
         <v>42271</v>
       </c>
-      <c r="B462" s="5"/>
+      <c r="B462" s="6">
+        <v>0</v>
+      </c>
       <c r="D462" s="5"/>
       <c r="E462" t="s">
         <v>18</v>
@@ -9360,7 +9630,9 @@
       <c r="A463" s="1">
         <v>42271</v>
       </c>
-      <c r="B463" s="5"/>
+      <c r="B463" s="6">
+        <v>0</v>
+      </c>
       <c r="D463" s="5"/>
       <c r="E463" t="s">
         <v>19</v>
@@ -9373,7 +9645,9 @@
       <c r="A464" s="1">
         <v>42271</v>
       </c>
-      <c r="B464" s="5"/>
+      <c r="B464" s="6">
+        <v>0</v>
+      </c>
       <c r="D464" s="5"/>
       <c r="E464" t="s">
         <v>20</v>
@@ -9386,7 +9660,9 @@
       <c r="A465" s="1">
         <v>42271</v>
       </c>
-      <c r="B465" s="5"/>
+      <c r="B465" s="6">
+        <v>0</v>
+      </c>
       <c r="D465" s="5"/>
       <c r="E465" t="s">
         <v>21</v>
@@ -9399,7 +9675,9 @@
       <c r="A466" s="1">
         <v>42271</v>
       </c>
-      <c r="B466" s="5"/>
+      <c r="B466" s="6">
+        <v>0</v>
+      </c>
       <c r="D466" s="5"/>
       <c r="E466" t="s">
         <v>22</v>
@@ -9412,7 +9690,9 @@
       <c r="A467" s="1">
         <v>42271</v>
       </c>
-      <c r="B467" s="5"/>
+      <c r="B467" s="6">
+        <v>0</v>
+      </c>
       <c r="D467" s="5"/>
       <c r="E467" t="s">
         <v>23</v>
@@ -9425,7 +9705,9 @@
       <c r="A468" s="1">
         <v>42271</v>
       </c>
-      <c r="B468" s="5"/>
+      <c r="B468" s="6">
+        <v>0</v>
+      </c>
       <c r="D468" s="5"/>
       <c r="E468" t="s">
         <v>25</v>
@@ -9438,7 +9720,9 @@
       <c r="A469" s="1">
         <v>42271</v>
       </c>
-      <c r="B469" s="5"/>
+      <c r="B469" s="6">
+        <v>0</v>
+      </c>
       <c r="D469" s="5"/>
       <c r="E469" t="s">
         <v>26</v>
@@ -9451,7 +9735,9 @@
       <c r="A470" s="1">
         <v>42271</v>
       </c>
-      <c r="B470" s="5"/>
+      <c r="B470" s="6">
+        <v>0</v>
+      </c>
       <c r="D470" s="5"/>
       <c r="E470" t="s">
         <v>27</v>
@@ -9464,7 +9750,9 @@
       <c r="A471" s="1">
         <v>42271</v>
       </c>
-      <c r="B471" s="5"/>
+      <c r="B471" s="6">
+        <v>0</v>
+      </c>
       <c r="D471" s="5"/>
       <c r="E471" t="s">
         <v>28</v>
@@ -9477,7 +9765,9 @@
       <c r="A472" s="1">
         <v>42271</v>
       </c>
-      <c r="B472" s="5"/>
+      <c r="B472" s="6">
+        <v>0</v>
+      </c>
       <c r="D472" s="5"/>
       <c r="E472" t="s">
         <v>29</v>
@@ -9490,7 +9780,9 @@
       <c r="A473" s="1">
         <v>42271</v>
       </c>
-      <c r="B473" s="5"/>
+      <c r="B473" s="6">
+        <v>0</v>
+      </c>
       <c r="D473" s="5"/>
       <c r="E473" t="s">
         <v>30</v>
@@ -9503,7 +9795,9 @@
       <c r="A474" s="1">
         <v>42271</v>
       </c>
-      <c r="B474" s="5"/>
+      <c r="B474" s="6">
+        <v>0</v>
+      </c>
       <c r="D474" s="5"/>
       <c r="E474" t="s">
         <v>5</v>
@@ -9516,7 +9810,9 @@
       <c r="A475" s="1">
         <v>42271</v>
       </c>
-      <c r="B475" s="5"/>
+      <c r="B475" s="6">
+        <v>0</v>
+      </c>
       <c r="D475" s="5"/>
       <c r="E475" t="s">
         <v>24</v>
@@ -9529,7 +9825,9 @@
       <c r="A476" s="1">
         <v>42271</v>
       </c>
-      <c r="B476" s="5"/>
+      <c r="B476" s="6">
+        <v>0</v>
+      </c>
       <c r="D476" s="5"/>
       <c r="E476" t="s">
         <v>8</v>
@@ -9542,7 +9840,9 @@
       <c r="A477" s="1">
         <v>42271</v>
       </c>
-      <c r="B477" s="5"/>
+      <c r="B477" s="6">
+        <v>0</v>
+      </c>
       <c r="D477" s="5"/>
       <c r="E477" t="s">
         <v>10</v>
@@ -9555,7 +9855,9 @@
       <c r="A478" s="1">
         <v>42271</v>
       </c>
-      <c r="B478" s="5"/>
+      <c r="B478" s="6">
+        <v>0</v>
+      </c>
       <c r="D478" s="5"/>
       <c r="E478" t="s">
         <v>12</v>
@@ -9568,7 +9870,9 @@
       <c r="A479" s="1">
         <v>42271</v>
       </c>
-      <c r="B479" s="5"/>
+      <c r="B479" s="6">
+        <v>0</v>
+      </c>
       <c r="D479" s="5"/>
       <c r="E479" t="s">
         <v>14</v>
@@ -10166,7 +10470,9 @@
       <c r="A515" s="1">
         <v>42275</v>
       </c>
-      <c r="B515" s="5"/>
+      <c r="B515" s="6">
+        <v>0</v>
+      </c>
       <c r="D515" s="5"/>
       <c r="E515" t="s">
         <v>1</v>
@@ -10179,7 +10485,9 @@
       <c r="A516" s="1">
         <v>42275</v>
       </c>
-      <c r="B516" s="5"/>
+      <c r="B516" s="6">
+        <v>0</v>
+      </c>
       <c r="D516" s="5"/>
       <c r="E516" t="s">
         <v>2</v>
@@ -10192,7 +10500,9 @@
       <c r="A517" s="1">
         <v>42275</v>
       </c>
-      <c r="B517" s="5"/>
+      <c r="B517" s="6">
+        <v>0</v>
+      </c>
       <c r="D517" s="5"/>
       <c r="E517" t="s">
         <v>3</v>
@@ -10205,7 +10515,9 @@
       <c r="A518" s="1">
         <v>42275</v>
       </c>
-      <c r="B518" s="5"/>
+      <c r="B518" s="6">
+        <v>0</v>
+      </c>
       <c r="D518" s="5"/>
       <c r="E518" t="s">
         <v>4</v>
@@ -10218,7 +10530,9 @@
       <c r="A519" s="1">
         <v>42275</v>
       </c>
-      <c r="B519" s="5"/>
+      <c r="B519" s="6">
+        <v>0</v>
+      </c>
       <c r="D519" s="5"/>
       <c r="E519" t="s">
         <v>6</v>
@@ -10231,7 +10545,9 @@
       <c r="A520" s="1">
         <v>42275</v>
       </c>
-      <c r="B520" s="5"/>
+      <c r="B520" s="6">
+        <v>0</v>
+      </c>
       <c r="D520" s="5"/>
       <c r="E520" t="s">
         <v>7</v>
@@ -10244,7 +10560,9 @@
       <c r="A521" s="1">
         <v>42275</v>
       </c>
-      <c r="B521" s="5"/>
+      <c r="B521" s="6">
+        <v>0</v>
+      </c>
       <c r="D521" s="5"/>
       <c r="E521" t="s">
         <v>9</v>
@@ -10257,7 +10575,9 @@
       <c r="A522" s="1">
         <v>42275</v>
       </c>
-      <c r="B522" s="5"/>
+      <c r="B522" s="6">
+        <v>0</v>
+      </c>
       <c r="D522" s="5"/>
       <c r="E522" t="s">
         <v>11</v>
@@ -10270,7 +10590,9 @@
       <c r="A523" s="1">
         <v>42275</v>
       </c>
-      <c r="B523" s="5"/>
+      <c r="B523" s="6">
+        <v>0</v>
+      </c>
       <c r="D523" s="5"/>
       <c r="E523" t="s">
         <v>13</v>
@@ -10283,7 +10605,9 @@
       <c r="A524" s="1">
         <v>42275</v>
       </c>
-      <c r="B524" s="5"/>
+      <c r="B524" s="6">
+        <v>0</v>
+      </c>
       <c r="D524" s="5"/>
       <c r="E524" t="s">
         <v>15</v>
@@ -10296,7 +10620,9 @@
       <c r="A525" s="1">
         <v>42275</v>
       </c>
-      <c r="B525" s="5"/>
+      <c r="B525" s="6">
+        <v>0</v>
+      </c>
       <c r="D525" s="5"/>
       <c r="E525" t="s">
         <v>16</v>
@@ -10309,7 +10635,9 @@
       <c r="A526" s="1">
         <v>42275</v>
       </c>
-      <c r="B526" s="5"/>
+      <c r="B526" s="6">
+        <v>0</v>
+      </c>
       <c r="D526" s="5"/>
       <c r="E526" t="s">
         <v>17</v>
@@ -10322,7 +10650,9 @@
       <c r="A527" s="1">
         <v>42275</v>
       </c>
-      <c r="B527" s="5"/>
+      <c r="B527" s="6">
+        <v>0</v>
+      </c>
       <c r="D527" s="5"/>
       <c r="E527" t="s">
         <v>18</v>
@@ -10335,7 +10665,9 @@
       <c r="A528" s="1">
         <v>42275</v>
       </c>
-      <c r="B528" s="5"/>
+      <c r="B528" s="6">
+        <v>0</v>
+      </c>
       <c r="D528" s="5"/>
       <c r="E528" t="s">
         <v>19</v>
@@ -10348,7 +10680,9 @@
       <c r="A529" s="1">
         <v>42275</v>
       </c>
-      <c r="B529" s="5"/>
+      <c r="B529" s="6">
+        <v>0</v>
+      </c>
       <c r="D529" s="5"/>
       <c r="E529" t="s">
         <v>20</v>
@@ -10361,7 +10695,9 @@
       <c r="A530" s="1">
         <v>42275</v>
       </c>
-      <c r="B530" s="5"/>
+      <c r="B530" s="6">
+        <v>0</v>
+      </c>
       <c r="D530" s="5"/>
       <c r="E530" t="s">
         <v>21</v>
@@ -10374,7 +10710,9 @@
       <c r="A531" s="1">
         <v>42275</v>
       </c>
-      <c r="B531" s="5"/>
+      <c r="B531" s="6">
+        <v>0</v>
+      </c>
       <c r="D531" s="5"/>
       <c r="E531" t="s">
         <v>22</v>
@@ -10387,7 +10725,9 @@
       <c r="A532" s="1">
         <v>42275</v>
       </c>
-      <c r="B532" s="5"/>
+      <c r="B532" s="6">
+        <v>0</v>
+      </c>
       <c r="D532" s="5"/>
       <c r="E532" t="s">
         <v>23</v>
@@ -10400,7 +10740,9 @@
       <c r="A533" s="1">
         <v>42275</v>
       </c>
-      <c r="B533" s="5"/>
+      <c r="B533" s="6">
+        <v>0</v>
+      </c>
       <c r="D533" s="5"/>
       <c r="E533" t="s">
         <v>25</v>
@@ -10413,7 +10755,9 @@
       <c r="A534" s="1">
         <v>42275</v>
       </c>
-      <c r="B534" s="5"/>
+      <c r="B534" s="6">
+        <v>0</v>
+      </c>
       <c r="D534" s="5"/>
       <c r="E534" t="s">
         <v>26</v>
@@ -10426,7 +10770,9 @@
       <c r="A535" s="1">
         <v>42275</v>
       </c>
-      <c r="B535" s="5"/>
+      <c r="B535" s="6">
+        <v>0</v>
+      </c>
       <c r="D535" s="5"/>
       <c r="E535" t="s">
         <v>27</v>
@@ -10439,7 +10785,9 @@
       <c r="A536" s="1">
         <v>42275</v>
       </c>
-      <c r="B536" s="5"/>
+      <c r="B536" s="6">
+        <v>0</v>
+      </c>
       <c r="D536" s="5"/>
       <c r="E536" t="s">
         <v>28</v>
@@ -10452,7 +10800,9 @@
       <c r="A537" s="1">
         <v>42275</v>
       </c>
-      <c r="B537" s="5"/>
+      <c r="B537" s="6">
+        <v>0</v>
+      </c>
       <c r="D537" s="5"/>
       <c r="E537" t="s">
         <v>29</v>
@@ -10465,7 +10815,9 @@
       <c r="A538" s="1">
         <v>42275</v>
       </c>
-      <c r="B538" s="5"/>
+      <c r="B538" s="6">
+        <v>0</v>
+      </c>
       <c r="D538" s="5"/>
       <c r="E538" t="s">
         <v>30</v>
@@ -10478,7 +10830,9 @@
       <c r="A539" s="1">
         <v>42275</v>
       </c>
-      <c r="B539" s="5"/>
+      <c r="B539" s="6">
+        <v>0</v>
+      </c>
       <c r="D539" s="5"/>
       <c r="E539" t="s">
         <v>5</v>
@@ -10491,7 +10845,9 @@
       <c r="A540" s="1">
         <v>42275</v>
       </c>
-      <c r="B540" s="5"/>
+      <c r="B540" s="6">
+        <v>0</v>
+      </c>
       <c r="D540" s="5"/>
       <c r="E540" t="s">
         <v>24</v>
@@ -10504,7 +10860,9 @@
       <c r="A541" s="1">
         <v>42275</v>
       </c>
-      <c r="B541" s="5"/>
+      <c r="B541" s="6">
+        <v>0</v>
+      </c>
       <c r="D541" s="5"/>
       <c r="E541" t="s">
         <v>8</v>
@@ -10517,7 +10875,9 @@
       <c r="A542" s="1">
         <v>42275</v>
       </c>
-      <c r="B542" s="5"/>
+      <c r="B542" s="6">
+        <v>0</v>
+      </c>
       <c r="D542" s="5"/>
       <c r="E542" t="s">
         <v>10</v>
@@ -10530,7 +10890,9 @@
       <c r="A543" s="1">
         <v>42275</v>
       </c>
-      <c r="B543" s="5"/>
+      <c r="B543" s="6">
+        <v>0</v>
+      </c>
       <c r="D543" s="5"/>
       <c r="E543" t="s">
         <v>12</v>
@@ -10543,7 +10905,9 @@
       <c r="A544" s="1">
         <v>42275</v>
       </c>
-      <c r="B544" s="5"/>
+      <c r="B544" s="6">
+        <v>0</v>
+      </c>
       <c r="D544" s="5"/>
       <c r="E544" t="s">
         <v>14</v>
@@ -11742,7 +12106,9 @@
       <c r="A616" s="1">
         <v>42282</v>
       </c>
-      <c r="B616" s="5"/>
+      <c r="B616" s="6">
+        <v>0</v>
+      </c>
       <c r="D616" s="5"/>
       <c r="E616" t="s">
         <v>1</v>
@@ -11755,7 +12121,9 @@
       <c r="A617" s="1">
         <v>42282</v>
       </c>
-      <c r="B617" s="5"/>
+      <c r="B617" s="6">
+        <v>0</v>
+      </c>
       <c r="D617" s="5"/>
       <c r="E617" t="s">
         <v>2</v>
@@ -11768,7 +12136,9 @@
       <c r="A618" s="1">
         <v>42282</v>
       </c>
-      <c r="B618" s="5"/>
+      <c r="B618" s="6">
+        <v>0</v>
+      </c>
       <c r="D618" s="5"/>
       <c r="E618" t="s">
         <v>3</v>
@@ -11781,7 +12151,9 @@
       <c r="A619" s="1">
         <v>42282</v>
       </c>
-      <c r="B619" s="5"/>
+      <c r="B619" s="6">
+        <v>0</v>
+      </c>
       <c r="D619" s="5"/>
       <c r="E619" t="s">
         <v>4</v>
@@ -11794,7 +12166,9 @@
       <c r="A620" s="1">
         <v>42282</v>
       </c>
-      <c r="B620" s="5"/>
+      <c r="B620" s="6">
+        <v>0</v>
+      </c>
       <c r="D620" s="5"/>
       <c r="E620" t="s">
         <v>6</v>
@@ -11807,7 +12181,9 @@
       <c r="A621" s="1">
         <v>42282</v>
       </c>
-      <c r="B621" s="5"/>
+      <c r="B621" s="6">
+        <v>0</v>
+      </c>
       <c r="D621" s="5"/>
       <c r="E621" t="s">
         <v>7</v>
@@ -11820,7 +12196,9 @@
       <c r="A622" s="1">
         <v>42282</v>
       </c>
-      <c r="B622" s="5"/>
+      <c r="B622" s="6">
+        <v>0</v>
+      </c>
       <c r="D622" s="5"/>
       <c r="E622" t="s">
         <v>9</v>
@@ -11833,7 +12211,9 @@
       <c r="A623" s="1">
         <v>42282</v>
       </c>
-      <c r="B623" s="5"/>
+      <c r="B623" s="6">
+        <v>0</v>
+      </c>
       <c r="D623" s="5"/>
       <c r="E623" t="s">
         <v>11</v>
@@ -11846,7 +12226,9 @@
       <c r="A624" s="1">
         <v>42282</v>
       </c>
-      <c r="B624" s="5"/>
+      <c r="B624" s="6">
+        <v>0</v>
+      </c>
       <c r="D624" s="5"/>
       <c r="E624" t="s">
         <v>13</v>
@@ -11859,7 +12241,9 @@
       <c r="A625" s="1">
         <v>42282</v>
       </c>
-      <c r="B625" s="5"/>
+      <c r="B625" s="6">
+        <v>0</v>
+      </c>
       <c r="D625" s="5"/>
       <c r="E625" t="s">
         <v>15</v>
@@ -11872,7 +12256,9 @@
       <c r="A626" s="1">
         <v>42282</v>
       </c>
-      <c r="B626" s="5"/>
+      <c r="B626" s="6">
+        <v>0</v>
+      </c>
       <c r="D626" s="5"/>
       <c r="E626" t="s">
         <v>16</v>
@@ -11885,7 +12271,9 @@
       <c r="A627" s="1">
         <v>42282</v>
       </c>
-      <c r="B627" s="5"/>
+      <c r="B627" s="6">
+        <v>0</v>
+      </c>
       <c r="D627" s="5"/>
       <c r="E627" t="s">
         <v>17</v>
@@ -11898,7 +12286,9 @@
       <c r="A628" s="1">
         <v>42282</v>
       </c>
-      <c r="B628" s="5"/>
+      <c r="B628" s="6">
+        <v>0</v>
+      </c>
       <c r="D628" s="5"/>
       <c r="E628" t="s">
         <v>18</v>
@@ -11911,7 +12301,9 @@
       <c r="A629" s="1">
         <v>42282</v>
       </c>
-      <c r="B629" s="5"/>
+      <c r="B629" s="6">
+        <v>0</v>
+      </c>
       <c r="D629" s="5"/>
       <c r="E629" t="s">
         <v>19</v>
@@ -11924,7 +12316,9 @@
       <c r="A630" s="1">
         <v>42282</v>
       </c>
-      <c r="B630" s="5"/>
+      <c r="B630" s="6">
+        <v>0</v>
+      </c>
       <c r="D630" s="5"/>
       <c r="E630" t="s">
         <v>20</v>
@@ -11937,7 +12331,9 @@
       <c r="A631" s="1">
         <v>42282</v>
       </c>
-      <c r="B631" s="5"/>
+      <c r="B631" s="6">
+        <v>0</v>
+      </c>
       <c r="D631" s="5"/>
       <c r="E631" t="s">
         <v>21</v>
@@ -11950,7 +12346,9 @@
       <c r="A632" s="1">
         <v>42282</v>
       </c>
-      <c r="B632" s="5"/>
+      <c r="B632" s="6">
+        <v>0</v>
+      </c>
       <c r="D632" s="5"/>
       <c r="E632" t="s">
         <v>22</v>
@@ -11963,7 +12361,9 @@
       <c r="A633" s="1">
         <v>42282</v>
       </c>
-      <c r="B633" s="5"/>
+      <c r="B633" s="6">
+        <v>0</v>
+      </c>
       <c r="D633" s="5"/>
       <c r="E633" t="s">
         <v>23</v>
@@ -11976,7 +12376,9 @@
       <c r="A634" s="1">
         <v>42282</v>
       </c>
-      <c r="B634" s="5"/>
+      <c r="B634" s="6">
+        <v>0</v>
+      </c>
       <c r="D634" s="5"/>
       <c r="E634" t="s">
         <v>25</v>
@@ -11989,7 +12391,9 @@
       <c r="A635" s="1">
         <v>42282</v>
       </c>
-      <c r="B635" s="5"/>
+      <c r="B635" s="6">
+        <v>0</v>
+      </c>
       <c r="D635" s="5"/>
       <c r="E635" t="s">
         <v>26</v>
@@ -12002,7 +12406,9 @@
       <c r="A636" s="1">
         <v>42282</v>
       </c>
-      <c r="B636" s="5"/>
+      <c r="B636" s="6">
+        <v>0</v>
+      </c>
       <c r="D636" s="5"/>
       <c r="E636" t="s">
         <v>27</v>
@@ -12015,7 +12421,9 @@
       <c r="A637" s="1">
         <v>42282</v>
       </c>
-      <c r="B637" s="5"/>
+      <c r="B637" s="6">
+        <v>0</v>
+      </c>
       <c r="D637" s="5"/>
       <c r="E637" t="s">
         <v>28</v>
@@ -12028,7 +12436,9 @@
       <c r="A638" s="1">
         <v>42282</v>
       </c>
-      <c r="B638" s="5"/>
+      <c r="B638" s="6">
+        <v>0</v>
+      </c>
       <c r="D638" s="5"/>
       <c r="E638" t="s">
         <v>29</v>
@@ -12041,7 +12451,9 @@
       <c r="A639" s="1">
         <v>42282</v>
       </c>
-      <c r="B639" s="5"/>
+      <c r="B639" s="6">
+        <v>0</v>
+      </c>
       <c r="D639" s="5"/>
       <c r="E639" t="s">
         <v>30</v>
@@ -12054,7 +12466,9 @@
       <c r="A640" s="1">
         <v>42282</v>
       </c>
-      <c r="B640" s="5"/>
+      <c r="B640" s="6">
+        <v>0</v>
+      </c>
       <c r="D640" s="5"/>
       <c r="E640" t="s">
         <v>5</v>
@@ -12067,7 +12481,9 @@
       <c r="A641" s="1">
         <v>42282</v>
       </c>
-      <c r="B641" s="5"/>
+      <c r="B641" s="6">
+        <v>0</v>
+      </c>
       <c r="D641" s="5"/>
       <c r="E641" t="s">
         <v>24</v>
@@ -12080,7 +12496,9 @@
       <c r="A642" s="1">
         <v>42282</v>
       </c>
-      <c r="B642" s="5"/>
+      <c r="B642" s="6">
+        <v>0</v>
+      </c>
       <c r="D642" s="5"/>
       <c r="E642" t="s">
         <v>8</v>
@@ -12093,7 +12511,9 @@
       <c r="A643" s="1">
         <v>42282</v>
       </c>
-      <c r="B643" s="5"/>
+      <c r="B643" s="6">
+        <v>0</v>
+      </c>
       <c r="D643" s="5"/>
       <c r="E643" t="s">
         <v>10</v>
@@ -12106,7 +12526,9 @@
       <c r="A644" s="1">
         <v>42282</v>
       </c>
-      <c r="B644" s="5"/>
+      <c r="B644" s="6">
+        <v>0</v>
+      </c>
       <c r="D644" s="5"/>
       <c r="E644" t="s">
         <v>12</v>
@@ -12119,7 +12541,9 @@
       <c r="A645" s="1">
         <v>42282</v>
       </c>
-      <c r="B645" s="5"/>
+      <c r="B645" s="6">
+        <v>0</v>
+      </c>
       <c r="D645" s="5"/>
       <c r="E645" t="s">
         <v>14</v>
@@ -12731,7 +13155,9 @@
       <c r="A682" s="1">
         <v>42289</v>
       </c>
-      <c r="B682" s="5"/>
+      <c r="B682" s="6">
+        <v>0</v>
+      </c>
       <c r="D682" s="5"/>
       <c r="E682" t="s">
         <v>1</v>
@@ -12744,7 +13170,9 @@
       <c r="A683" s="1">
         <v>42289</v>
       </c>
-      <c r="B683" s="5"/>
+      <c r="B683" s="6">
+        <v>0</v>
+      </c>
       <c r="D683" s="5"/>
       <c r="E683" t="s">
         <v>2</v>
@@ -12757,7 +13185,9 @@
       <c r="A684" s="1">
         <v>42289</v>
       </c>
-      <c r="B684" s="5"/>
+      <c r="B684" s="6">
+        <v>0</v>
+      </c>
       <c r="D684" s="5"/>
       <c r="E684" t="s">
         <v>3</v>
@@ -12770,7 +13200,9 @@
       <c r="A685" s="1">
         <v>42289</v>
       </c>
-      <c r="B685" s="5"/>
+      <c r="B685" s="6">
+        <v>0</v>
+      </c>
       <c r="D685" s="5"/>
       <c r="E685" t="s">
         <v>4</v>
@@ -12783,7 +13215,9 @@
       <c r="A686" s="1">
         <v>42289</v>
       </c>
-      <c r="B686" s="5"/>
+      <c r="B686" s="6">
+        <v>0</v>
+      </c>
       <c r="D686" s="5"/>
       <c r="E686" t="s">
         <v>6</v>
@@ -12796,7 +13230,9 @@
       <c r="A687" s="1">
         <v>42289</v>
       </c>
-      <c r="B687" s="5"/>
+      <c r="B687" s="6">
+        <v>0</v>
+      </c>
       <c r="D687" s="5"/>
       <c r="E687" t="s">
         <v>7</v>
@@ -12809,7 +13245,9 @@
       <c r="A688" s="1">
         <v>42289</v>
       </c>
-      <c r="B688" s="5"/>
+      <c r="B688" s="6">
+        <v>0</v>
+      </c>
       <c r="D688" s="5"/>
       <c r="E688" t="s">
         <v>9</v>
@@ -12822,7 +13260,9 @@
       <c r="A689" s="1">
         <v>42289</v>
       </c>
-      <c r="B689" s="5"/>
+      <c r="B689" s="6">
+        <v>0</v>
+      </c>
       <c r="D689" s="5"/>
       <c r="E689" t="s">
         <v>11</v>
@@ -12835,7 +13275,9 @@
       <c r="A690" s="1">
         <v>42289</v>
       </c>
-      <c r="B690" s="5"/>
+      <c r="B690" s="6">
+        <v>0</v>
+      </c>
       <c r="D690" s="5"/>
       <c r="E690" t="s">
         <v>13</v>
@@ -12848,7 +13290,9 @@
       <c r="A691" s="1">
         <v>42289</v>
       </c>
-      <c r="B691" s="5"/>
+      <c r="B691" s="6">
+        <v>0</v>
+      </c>
       <c r="D691" s="5"/>
       <c r="E691" t="s">
         <v>15</v>
@@ -12861,7 +13305,9 @@
       <c r="A692" s="1">
         <v>42289</v>
       </c>
-      <c r="B692" s="5"/>
+      <c r="B692" s="6">
+        <v>0</v>
+      </c>
       <c r="D692" s="5"/>
       <c r="E692" t="s">
         <v>16</v>
@@ -12874,7 +13320,9 @@
       <c r="A693" s="1">
         <v>42289</v>
       </c>
-      <c r="B693" s="5"/>
+      <c r="B693" s="6">
+        <v>0</v>
+      </c>
       <c r="D693" s="5"/>
       <c r="E693" t="s">
         <v>17</v>
@@ -12887,7 +13335,9 @@
       <c r="A694" s="1">
         <v>42289</v>
       </c>
-      <c r="B694" s="5"/>
+      <c r="B694" s="6">
+        <v>0</v>
+      </c>
       <c r="D694" s="5"/>
       <c r="E694" t="s">
         <v>18</v>
@@ -12900,7 +13350,9 @@
       <c r="A695" s="1">
         <v>42289</v>
       </c>
-      <c r="B695" s="5"/>
+      <c r="B695" s="6">
+        <v>0</v>
+      </c>
       <c r="D695" s="5"/>
       <c r="E695" t="s">
         <v>19</v>
@@ -12913,7 +13365,9 @@
       <c r="A696" s="1">
         <v>42289</v>
       </c>
-      <c r="B696" s="5"/>
+      <c r="B696" s="6">
+        <v>0</v>
+      </c>
       <c r="D696" s="5"/>
       <c r="E696" t="s">
         <v>20</v>
@@ -12926,7 +13380,9 @@
       <c r="A697" s="1">
         <v>42289</v>
       </c>
-      <c r="B697" s="5"/>
+      <c r="B697" s="6">
+        <v>0</v>
+      </c>
       <c r="D697" s="5"/>
       <c r="E697" t="s">
         <v>21</v>
@@ -12939,7 +13395,9 @@
       <c r="A698" s="1">
         <v>42289</v>
       </c>
-      <c r="B698" s="5"/>
+      <c r="B698" s="6">
+        <v>0</v>
+      </c>
       <c r="D698" s="5"/>
       <c r="E698" t="s">
         <v>22</v>
@@ -12952,7 +13410,9 @@
       <c r="A699" s="1">
         <v>42289</v>
       </c>
-      <c r="B699" s="5"/>
+      <c r="B699" s="6">
+        <v>0</v>
+      </c>
       <c r="D699" s="5"/>
       <c r="E699" t="s">
         <v>23</v>
@@ -12965,7 +13425,9 @@
       <c r="A700" s="1">
         <v>42289</v>
       </c>
-      <c r="B700" s="5"/>
+      <c r="B700" s="6">
+        <v>0</v>
+      </c>
       <c r="D700" s="5"/>
       <c r="E700" t="s">
         <v>25</v>
@@ -12978,7 +13440,9 @@
       <c r="A701" s="1">
         <v>42289</v>
       </c>
-      <c r="B701" s="5"/>
+      <c r="B701" s="6">
+        <v>0</v>
+      </c>
       <c r="D701" s="5"/>
       <c r="E701" t="s">
         <v>26</v>
@@ -12991,7 +13455,9 @@
       <c r="A702" s="1">
         <v>42289</v>
       </c>
-      <c r="B702" s="5"/>
+      <c r="B702" s="6">
+        <v>0</v>
+      </c>
       <c r="D702" s="5"/>
       <c r="E702" t="s">
         <v>27</v>
@@ -13004,7 +13470,9 @@
       <c r="A703" s="1">
         <v>42289</v>
       </c>
-      <c r="B703" s="5"/>
+      <c r="B703" s="6">
+        <v>0</v>
+      </c>
       <c r="D703" s="5"/>
       <c r="E703" t="s">
         <v>28</v>
@@ -13017,7 +13485,9 @@
       <c r="A704" s="1">
         <v>42289</v>
       </c>
-      <c r="B704" s="5"/>
+      <c r="B704" s="6">
+        <v>0</v>
+      </c>
       <c r="D704" s="5"/>
       <c r="E704" t="s">
         <v>29</v>
@@ -13030,7 +13500,9 @@
       <c r="A705" s="1">
         <v>42289</v>
       </c>
-      <c r="B705" s="5"/>
+      <c r="B705" s="6">
+        <v>0</v>
+      </c>
       <c r="D705" s="5"/>
       <c r="E705" t="s">
         <v>30</v>
@@ -13043,7 +13515,9 @@
       <c r="A706" s="1">
         <v>42289</v>
       </c>
-      <c r="B706" s="5"/>
+      <c r="B706" s="6">
+        <v>0</v>
+      </c>
       <c r="D706" s="5"/>
       <c r="E706" t="s">
         <v>5</v>
@@ -13056,7 +13530,9 @@
       <c r="A707" s="1">
         <v>42289</v>
       </c>
-      <c r="B707" s="5"/>
+      <c r="B707" s="6">
+        <v>0</v>
+      </c>
       <c r="D707" s="5"/>
       <c r="E707" t="s">
         <v>24</v>
@@ -13069,7 +13545,9 @@
       <c r="A708" s="1">
         <v>42289</v>
       </c>
-      <c r="B708" s="5"/>
+      <c r="B708" s="6">
+        <v>0</v>
+      </c>
       <c r="D708" s="5"/>
       <c r="E708" t="s">
         <v>8</v>
@@ -13082,7 +13560,9 @@
       <c r="A709" s="1">
         <v>42289</v>
       </c>
-      <c r="B709" s="5"/>
+      <c r="B709" s="6">
+        <v>0</v>
+      </c>
       <c r="D709" s="5"/>
       <c r="E709" t="s">
         <v>10</v>
@@ -13095,7 +13575,9 @@
       <c r="A710" s="1">
         <v>42289</v>
       </c>
-      <c r="B710" s="5"/>
+      <c r="B710" s="6">
+        <v>0</v>
+      </c>
       <c r="D710" s="5"/>
       <c r="E710" t="s">
         <v>12</v>
@@ -13108,7 +13590,9 @@
       <c r="A711" s="1">
         <v>42289</v>
       </c>
-      <c r="B711" s="5"/>
+      <c r="B711" s="6">
+        <v>0</v>
+      </c>
       <c r="D711" s="5"/>
       <c r="E711" t="s">
         <v>14</v>
@@ -13709,7 +14193,9 @@
       <c r="A747" s="1">
         <v>42296</v>
       </c>
-      <c r="B747" s="5"/>
+      <c r="B747" s="6">
+        <v>0</v>
+      </c>
       <c r="E747" t="s">
         <v>1</v>
       </c>
@@ -13721,7 +14207,9 @@
       <c r="A748" s="1">
         <v>42296</v>
       </c>
-      <c r="B748" s="5"/>
+      <c r="B748" s="6">
+        <v>0</v>
+      </c>
       <c r="E748" t="s">
         <v>2</v>
       </c>
@@ -13733,7 +14221,9 @@
       <c r="A749" s="1">
         <v>42296</v>
       </c>
-      <c r="B749" s="5"/>
+      <c r="B749" s="6">
+        <v>0</v>
+      </c>
       <c r="E749" t="s">
         <v>3</v>
       </c>
@@ -13745,7 +14235,9 @@
       <c r="A750" s="1">
         <v>42296</v>
       </c>
-      <c r="B750" s="5"/>
+      <c r="B750" s="6">
+        <v>0</v>
+      </c>
       <c r="E750" t="s">
         <v>4</v>
       </c>
@@ -13757,7 +14249,9 @@
       <c r="A751" s="1">
         <v>42296</v>
       </c>
-      <c r="B751" s="5"/>
+      <c r="B751" s="6">
+        <v>0</v>
+      </c>
       <c r="E751" t="s">
         <v>6</v>
       </c>
@@ -13769,7 +14263,9 @@
       <c r="A752" s="1">
         <v>42296</v>
       </c>
-      <c r="B752" s="5"/>
+      <c r="B752" s="6">
+        <v>0</v>
+      </c>
       <c r="E752" t="s">
         <v>7</v>
       </c>
@@ -13781,7 +14277,9 @@
       <c r="A753" s="1">
         <v>42296</v>
       </c>
-      <c r="B753" s="5"/>
+      <c r="B753" s="6">
+        <v>0</v>
+      </c>
       <c r="E753" t="s">
         <v>9</v>
       </c>
@@ -13793,7 +14291,9 @@
       <c r="A754" s="1">
         <v>42296</v>
       </c>
-      <c r="B754" s="5"/>
+      <c r="B754" s="6">
+        <v>0</v>
+      </c>
       <c r="E754" t="s">
         <v>11</v>
       </c>
@@ -13805,7 +14305,9 @@
       <c r="A755" s="1">
         <v>42296</v>
       </c>
-      <c r="B755" s="5"/>
+      <c r="B755" s="6">
+        <v>0</v>
+      </c>
       <c r="E755" t="s">
         <v>13</v>
       </c>
@@ -13817,7 +14319,9 @@
       <c r="A756" s="1">
         <v>42296</v>
       </c>
-      <c r="B756" s="5"/>
+      <c r="B756" s="6">
+        <v>0</v>
+      </c>
       <c r="E756" t="s">
         <v>15</v>
       </c>
@@ -13829,7 +14333,9 @@
       <c r="A757" s="1">
         <v>42296</v>
       </c>
-      <c r="B757" s="5"/>
+      <c r="B757" s="6">
+        <v>0</v>
+      </c>
       <c r="E757" t="s">
         <v>16</v>
       </c>
@@ -13841,7 +14347,9 @@
       <c r="A758" s="1">
         <v>42296</v>
       </c>
-      <c r="B758" s="5"/>
+      <c r="B758" s="6">
+        <v>0</v>
+      </c>
       <c r="E758" t="s">
         <v>17</v>
       </c>
@@ -13853,7 +14361,9 @@
       <c r="A759" s="1">
         <v>42296</v>
       </c>
-      <c r="B759" s="5"/>
+      <c r="B759" s="6">
+        <v>0</v>
+      </c>
       <c r="E759" t="s">
         <v>18</v>
       </c>
@@ -13865,7 +14375,9 @@
       <c r="A760" s="1">
         <v>42296</v>
       </c>
-      <c r="B760" s="5"/>
+      <c r="B760" s="6">
+        <v>0</v>
+      </c>
       <c r="E760" t="s">
         <v>19</v>
       </c>
@@ -13877,7 +14389,9 @@
       <c r="A761" s="1">
         <v>42296</v>
       </c>
-      <c r="B761" s="5"/>
+      <c r="B761" s="6">
+        <v>0</v>
+      </c>
       <c r="E761" t="s">
         <v>20</v>
       </c>
@@ -13889,7 +14403,9 @@
       <c r="A762" s="1">
         <v>42296</v>
       </c>
-      <c r="B762" s="5"/>
+      <c r="B762" s="6">
+        <v>0</v>
+      </c>
       <c r="E762" t="s">
         <v>21</v>
       </c>
@@ -13901,7 +14417,9 @@
       <c r="A763" s="1">
         <v>42296</v>
       </c>
-      <c r="B763" s="5"/>
+      <c r="B763" s="6">
+        <v>0</v>
+      </c>
       <c r="E763" t="s">
         <v>22</v>
       </c>
@@ -13913,7 +14431,9 @@
       <c r="A764" s="1">
         <v>42296</v>
       </c>
-      <c r="B764" s="5"/>
+      <c r="B764" s="6">
+        <v>0</v>
+      </c>
       <c r="E764" t="s">
         <v>23</v>
       </c>
@@ -13925,7 +14445,9 @@
       <c r="A765" s="1">
         <v>42296</v>
       </c>
-      <c r="B765" s="5"/>
+      <c r="B765" s="6">
+        <v>0</v>
+      </c>
       <c r="E765" t="s">
         <v>25</v>
       </c>
@@ -13937,7 +14459,9 @@
       <c r="A766" s="1">
         <v>42296</v>
       </c>
-      <c r="B766" s="5"/>
+      <c r="B766" s="6">
+        <v>0</v>
+      </c>
       <c r="E766" t="s">
         <v>26</v>
       </c>
@@ -13949,7 +14473,9 @@
       <c r="A767" s="1">
         <v>42296</v>
       </c>
-      <c r="B767" s="5"/>
+      <c r="B767" s="6">
+        <v>0</v>
+      </c>
       <c r="E767" t="s">
         <v>27</v>
       </c>
@@ -13961,7 +14487,9 @@
       <c r="A768" s="1">
         <v>42296</v>
       </c>
-      <c r="B768" s="5"/>
+      <c r="B768" s="6">
+        <v>0</v>
+      </c>
       <c r="E768" t="s">
         <v>28</v>
       </c>
@@ -13973,7 +14501,9 @@
       <c r="A769" s="1">
         <v>42296</v>
       </c>
-      <c r="B769" s="5"/>
+      <c r="B769" s="6">
+        <v>0</v>
+      </c>
       <c r="E769" t="s">
         <v>29</v>
       </c>
@@ -13985,7 +14515,9 @@
       <c r="A770" s="1">
         <v>42296</v>
       </c>
-      <c r="B770" s="5"/>
+      <c r="B770" s="6">
+        <v>0</v>
+      </c>
       <c r="E770" t="s">
         <v>30</v>
       </c>
@@ -13997,7 +14529,9 @@
       <c r="A771" s="1">
         <v>42296</v>
       </c>
-      <c r="B771" s="5"/>
+      <c r="B771" s="6">
+        <v>0</v>
+      </c>
       <c r="E771" t="s">
         <v>5</v>
       </c>
@@ -14009,7 +14543,9 @@
       <c r="A772" s="1">
         <v>42296</v>
       </c>
-      <c r="B772" s="5"/>
+      <c r="B772" s="6">
+        <v>0</v>
+      </c>
       <c r="E772" t="s">
         <v>24</v>
       </c>
@@ -14021,7 +14557,9 @@
       <c r="A773" s="1">
         <v>42296</v>
       </c>
-      <c r="B773" s="5"/>
+      <c r="B773" s="6">
+        <v>0</v>
+      </c>
       <c r="E773" t="s">
         <v>8</v>
       </c>
@@ -14033,7 +14571,9 @@
       <c r="A774" s="1">
         <v>42296</v>
       </c>
-      <c r="B774" s="5"/>
+      <c r="B774" s="6">
+        <v>0</v>
+      </c>
       <c r="E774" t="s">
         <v>10</v>
       </c>
@@ -14045,7 +14585,9 @@
       <c r="A775" s="1">
         <v>42296</v>
       </c>
-      <c r="B775" s="5"/>
+      <c r="B775" s="6">
+        <v>0</v>
+      </c>
       <c r="E775" t="s">
         <v>12</v>
       </c>
@@ -14057,7 +14599,9 @@
       <c r="A776" s="1">
         <v>42296</v>
       </c>
-      <c r="B776" s="5"/>
+      <c r="B776" s="6">
+        <v>0</v>
+      </c>
       <c r="E776" t="s">
         <v>14</v>
       </c>
@@ -14694,7 +15238,9 @@
       <c r="A814" s="1">
         <v>42303</v>
       </c>
-      <c r="B814" s="5"/>
+      <c r="B814" s="6">
+        <v>0</v>
+      </c>
       <c r="E814" t="s">
         <v>1</v>
       </c>
@@ -14706,7 +15252,9 @@
       <c r="A815" s="1">
         <v>42303</v>
       </c>
-      <c r="B815" s="5"/>
+      <c r="B815" s="6">
+        <v>0</v>
+      </c>
       <c r="E815" t="s">
         <v>2</v>
       </c>
@@ -14718,7 +15266,9 @@
       <c r="A816" s="1">
         <v>42303</v>
       </c>
-      <c r="B816" s="5"/>
+      <c r="B816" s="6">
+        <v>0</v>
+      </c>
       <c r="E816" t="s">
         <v>3</v>
       </c>
@@ -14730,7 +15280,9 @@
       <c r="A817" s="1">
         <v>42303</v>
       </c>
-      <c r="B817" s="5"/>
+      <c r="B817" s="6">
+        <v>0</v>
+      </c>
       <c r="E817" t="s">
         <v>4</v>
       </c>
@@ -14742,7 +15294,9 @@
       <c r="A818" s="1">
         <v>42303</v>
       </c>
-      <c r="B818" s="5"/>
+      <c r="B818" s="6">
+        <v>0</v>
+      </c>
       <c r="E818" t="s">
         <v>6</v>
       </c>
@@ -14754,7 +15308,9 @@
       <c r="A819" s="1">
         <v>42303</v>
       </c>
-      <c r="B819" s="5"/>
+      <c r="B819" s="6">
+        <v>0</v>
+      </c>
       <c r="E819" t="s">
         <v>7</v>
       </c>
@@ -14766,7 +15322,9 @@
       <c r="A820" s="1">
         <v>42303</v>
       </c>
-      <c r="B820" s="5"/>
+      <c r="B820" s="6">
+        <v>0</v>
+      </c>
       <c r="E820" t="s">
         <v>9</v>
       </c>
@@ -14778,7 +15336,9 @@
       <c r="A821" s="1">
         <v>42303</v>
       </c>
-      <c r="B821" s="5"/>
+      <c r="B821" s="6">
+        <v>0</v>
+      </c>
       <c r="E821" t="s">
         <v>11</v>
       </c>
@@ -14790,7 +15350,9 @@
       <c r="A822" s="1">
         <v>42303</v>
       </c>
-      <c r="B822" s="5"/>
+      <c r="B822" s="6">
+        <v>0</v>
+      </c>
       <c r="E822" t="s">
         <v>13</v>
       </c>
@@ -14802,7 +15364,9 @@
       <c r="A823" s="1">
         <v>42303</v>
       </c>
-      <c r="B823" s="5"/>
+      <c r="B823" s="6">
+        <v>0</v>
+      </c>
       <c r="E823" t="s">
         <v>15</v>
       </c>
@@ -14814,7 +15378,9 @@
       <c r="A824" s="1">
         <v>42303</v>
       </c>
-      <c r="B824" s="5"/>
+      <c r="B824" s="6">
+        <v>0</v>
+      </c>
       <c r="E824" t="s">
         <v>16</v>
       </c>
@@ -14826,7 +15392,9 @@
       <c r="A825" s="1">
         <v>42303</v>
       </c>
-      <c r="B825" s="5"/>
+      <c r="B825" s="6">
+        <v>0</v>
+      </c>
       <c r="E825" t="s">
         <v>17</v>
       </c>
@@ -14838,7 +15406,9 @@
       <c r="A826" s="1">
         <v>42303</v>
       </c>
-      <c r="B826" s="5"/>
+      <c r="B826" s="6">
+        <v>0</v>
+      </c>
       <c r="E826" t="s">
         <v>18</v>
       </c>
@@ -14850,7 +15420,9 @@
       <c r="A827" s="1">
         <v>42303</v>
       </c>
-      <c r="B827" s="5"/>
+      <c r="B827" s="6">
+        <v>0</v>
+      </c>
       <c r="E827" t="s">
         <v>19</v>
       </c>
@@ -14862,7 +15434,9 @@
       <c r="A828" s="1">
         <v>42303</v>
       </c>
-      <c r="B828" s="5"/>
+      <c r="B828" s="6">
+        <v>0</v>
+      </c>
       <c r="E828" t="s">
         <v>20</v>
       </c>
@@ -14874,7 +15448,9 @@
       <c r="A829" s="1">
         <v>42303</v>
       </c>
-      <c r="B829" s="5"/>
+      <c r="B829" s="6">
+        <v>0</v>
+      </c>
       <c r="E829" t="s">
         <v>21</v>
       </c>
@@ -14886,7 +15462,9 @@
       <c r="A830" s="1">
         <v>42303</v>
       </c>
-      <c r="B830" s="5"/>
+      <c r="B830" s="6">
+        <v>0</v>
+      </c>
       <c r="E830" t="s">
         <v>22</v>
       </c>
@@ -14898,7 +15476,9 @@
       <c r="A831" s="1">
         <v>42303</v>
       </c>
-      <c r="B831" s="5"/>
+      <c r="B831" s="6">
+        <v>0</v>
+      </c>
       <c r="E831" t="s">
         <v>23</v>
       </c>
@@ -14910,7 +15490,9 @@
       <c r="A832" s="1">
         <v>42303</v>
       </c>
-      <c r="B832" s="5"/>
+      <c r="B832" s="6">
+        <v>0</v>
+      </c>
       <c r="E832" t="s">
         <v>25</v>
       </c>
@@ -14922,7 +15504,9 @@
       <c r="A833" s="1">
         <v>42303</v>
       </c>
-      <c r="B833" s="5"/>
+      <c r="B833" s="6">
+        <v>0</v>
+      </c>
       <c r="E833" t="s">
         <v>26</v>
       </c>
@@ -14934,7 +15518,9 @@
       <c r="A834" s="1">
         <v>42303</v>
       </c>
-      <c r="B834" s="5"/>
+      <c r="B834" s="6">
+        <v>0</v>
+      </c>
       <c r="E834" t="s">
         <v>27</v>
       </c>
@@ -14946,7 +15532,9 @@
       <c r="A835" s="1">
         <v>42303</v>
       </c>
-      <c r="B835" s="5"/>
+      <c r="B835" s="6">
+        <v>0</v>
+      </c>
       <c r="E835" t="s">
         <v>28</v>
       </c>
@@ -14958,7 +15546,9 @@
       <c r="A836" s="1">
         <v>42303</v>
       </c>
-      <c r="B836" s="5"/>
+      <c r="B836" s="6">
+        <v>0</v>
+      </c>
       <c r="E836" t="s">
         <v>29</v>
       </c>
@@ -14970,7 +15560,9 @@
       <c r="A837" s="1">
         <v>42303</v>
       </c>
-      <c r="B837" s="5"/>
+      <c r="B837" s="6">
+        <v>0</v>
+      </c>
       <c r="E837" t="s">
         <v>30</v>
       </c>
@@ -14982,7 +15574,9 @@
       <c r="A838" s="1">
         <v>42303</v>
       </c>
-      <c r="B838" s="5"/>
+      <c r="B838" s="6">
+        <v>0</v>
+      </c>
       <c r="E838" t="s">
         <v>5</v>
       </c>
@@ -14994,7 +15588,9 @@
       <c r="A839" s="1">
         <v>42303</v>
       </c>
-      <c r="B839" s="5"/>
+      <c r="B839" s="6">
+        <v>0</v>
+      </c>
       <c r="E839" t="s">
         <v>24</v>
       </c>
@@ -15006,7 +15602,9 @@
       <c r="A840" s="1">
         <v>42303</v>
       </c>
-      <c r="B840" s="5"/>
+      <c r="B840" s="6">
+        <v>0</v>
+      </c>
       <c r="E840" t="s">
         <v>8</v>
       </c>
@@ -15018,7 +15616,9 @@
       <c r="A841" s="1">
         <v>42303</v>
       </c>
-      <c r="B841" s="5"/>
+      <c r="B841" s="6">
+        <v>0</v>
+      </c>
       <c r="E841" t="s">
         <v>10</v>
       </c>
@@ -15030,7 +15630,9 @@
       <c r="A842" s="1">
         <v>42303</v>
       </c>
-      <c r="B842" s="5"/>
+      <c r="B842" s="6">
+        <v>0</v>
+      </c>
       <c r="E842" t="s">
         <v>12</v>
       </c>
@@ -15042,7 +15644,9 @@
       <c r="A843" s="1">
         <v>42303</v>
       </c>
-      <c r="B843" s="5"/>
+      <c r="B843" s="6">
+        <v>0</v>
+      </c>
       <c r="E843" t="s">
         <v>14</v>
       </c>
@@ -15690,7 +16294,9 @@
       <c r="A880" s="1">
         <v>42310</v>
       </c>
-      <c r="B880" s="5"/>
+      <c r="B880" s="6">
+        <v>0</v>
+      </c>
       <c r="E880" t="s">
         <v>1</v>
       </c>
@@ -15702,7 +16308,9 @@
       <c r="A881" s="1">
         <v>42310</v>
       </c>
-      <c r="B881" s="5"/>
+      <c r="B881" s="6">
+        <v>0</v>
+      </c>
       <c r="E881" t="s">
         <v>2</v>
       </c>
@@ -15714,7 +16322,9 @@
       <c r="A882" s="1">
         <v>42310</v>
       </c>
-      <c r="B882" s="5"/>
+      <c r="B882" s="6">
+        <v>0</v>
+      </c>
       <c r="E882" t="s">
         <v>3</v>
       </c>
@@ -15726,7 +16336,9 @@
       <c r="A883" s="1">
         <v>42310</v>
       </c>
-      <c r="B883" s="5"/>
+      <c r="B883" s="6">
+        <v>0</v>
+      </c>
       <c r="E883" t="s">
         <v>4</v>
       </c>
@@ -15738,7 +16350,9 @@
       <c r="A884" s="1">
         <v>42310</v>
       </c>
-      <c r="B884" s="5"/>
+      <c r="B884" s="6">
+        <v>0</v>
+      </c>
       <c r="E884" t="s">
         <v>6</v>
       </c>
@@ -15750,7 +16364,9 @@
       <c r="A885" s="1">
         <v>42310</v>
       </c>
-      <c r="B885" s="5"/>
+      <c r="B885" s="6">
+        <v>0</v>
+      </c>
       <c r="E885" t="s">
         <v>7</v>
       </c>
@@ -15762,7 +16378,9 @@
       <c r="A886" s="1">
         <v>42310</v>
       </c>
-      <c r="B886" s="5"/>
+      <c r="B886" s="6">
+        <v>0</v>
+      </c>
       <c r="E886" t="s">
         <v>9</v>
       </c>
@@ -15774,7 +16392,9 @@
       <c r="A887" s="1">
         <v>42310</v>
       </c>
-      <c r="B887" s="5"/>
+      <c r="B887" s="6">
+        <v>0</v>
+      </c>
       <c r="E887" t="s">
         <v>11</v>
       </c>
@@ -15786,7 +16406,9 @@
       <c r="A888" s="1">
         <v>42310</v>
       </c>
-      <c r="B888" s="5"/>
+      <c r="B888" s="6">
+        <v>0</v>
+      </c>
       <c r="E888" t="s">
         <v>13</v>
       </c>
@@ -15798,7 +16420,9 @@
       <c r="A889" s="1">
         <v>42310</v>
       </c>
-      <c r="B889" s="5"/>
+      <c r="B889" s="6">
+        <v>0</v>
+      </c>
       <c r="E889" t="s">
         <v>15</v>
       </c>
@@ -15810,7 +16434,9 @@
       <c r="A890" s="1">
         <v>42310</v>
       </c>
-      <c r="B890" s="5"/>
+      <c r="B890" s="6">
+        <v>0</v>
+      </c>
       <c r="E890" t="s">
         <v>16</v>
       </c>
@@ -15822,7 +16448,9 @@
       <c r="A891" s="1">
         <v>42310</v>
       </c>
-      <c r="B891" s="5"/>
+      <c r="B891" s="6">
+        <v>0</v>
+      </c>
       <c r="E891" t="s">
         <v>17</v>
       </c>
@@ -15834,7 +16462,9 @@
       <c r="A892" s="1">
         <v>42310</v>
       </c>
-      <c r="B892" s="5"/>
+      <c r="B892" s="6">
+        <v>0</v>
+      </c>
       <c r="E892" t="s">
         <v>18</v>
       </c>
@@ -15846,7 +16476,9 @@
       <c r="A893" s="1">
         <v>42310</v>
       </c>
-      <c r="B893" s="5"/>
+      <c r="B893" s="6">
+        <v>0</v>
+      </c>
       <c r="E893" t="s">
         <v>19</v>
       </c>
@@ -15858,7 +16490,9 @@
       <c r="A894" s="1">
         <v>42310</v>
       </c>
-      <c r="B894" s="5"/>
+      <c r="B894" s="6">
+        <v>0</v>
+      </c>
       <c r="E894" t="s">
         <v>20</v>
       </c>
@@ -15870,7 +16504,9 @@
       <c r="A895" s="1">
         <v>42310</v>
       </c>
-      <c r="B895" s="5"/>
+      <c r="B895" s="6">
+        <v>0</v>
+      </c>
       <c r="E895" t="s">
         <v>21</v>
       </c>
@@ -15882,7 +16518,9 @@
       <c r="A896" s="1">
         <v>42310</v>
       </c>
-      <c r="B896" s="5"/>
+      <c r="B896" s="6">
+        <v>0</v>
+      </c>
       <c r="E896" t="s">
         <v>22</v>
       </c>
@@ -15894,7 +16532,9 @@
       <c r="A897" s="1">
         <v>42310</v>
       </c>
-      <c r="B897" s="5"/>
+      <c r="B897" s="6">
+        <v>0</v>
+      </c>
       <c r="E897" t="s">
         <v>23</v>
       </c>
@@ -15906,7 +16546,9 @@
       <c r="A898" s="1">
         <v>42310</v>
       </c>
-      <c r="B898" s="5"/>
+      <c r="B898" s="6">
+        <v>0</v>
+      </c>
       <c r="E898" t="s">
         <v>25</v>
       </c>
@@ -15918,7 +16560,9 @@
       <c r="A899" s="1">
         <v>42310</v>
       </c>
-      <c r="B899" s="5"/>
+      <c r="B899" s="6">
+        <v>0</v>
+      </c>
       <c r="E899" t="s">
         <v>26</v>
       </c>
@@ -15930,7 +16574,9 @@
       <c r="A900" s="1">
         <v>42310</v>
       </c>
-      <c r="B900" s="5"/>
+      <c r="B900" s="6">
+        <v>0</v>
+      </c>
       <c r="E900" t="s">
         <v>27</v>
       </c>
@@ -15942,7 +16588,9 @@
       <c r="A901" s="1">
         <v>42310</v>
       </c>
-      <c r="B901" s="5"/>
+      <c r="B901" s="6">
+        <v>0</v>
+      </c>
       <c r="E901" t="s">
         <v>28</v>
       </c>
@@ -15954,7 +16602,9 @@
       <c r="A902" s="1">
         <v>42310</v>
       </c>
-      <c r="B902" s="5"/>
+      <c r="B902" s="6">
+        <v>0</v>
+      </c>
       <c r="E902" t="s">
         <v>29</v>
       </c>
@@ -15966,7 +16616,9 @@
       <c r="A903" s="1">
         <v>42310</v>
       </c>
-      <c r="B903" s="5"/>
+      <c r="B903" s="6">
+        <v>0</v>
+      </c>
       <c r="E903" t="s">
         <v>30</v>
       </c>
@@ -15978,7 +16630,9 @@
       <c r="A904" s="1">
         <v>42310</v>
       </c>
-      <c r="B904" s="5"/>
+      <c r="B904" s="6">
+        <v>0</v>
+      </c>
       <c r="E904" t="s">
         <v>5</v>
       </c>
@@ -15990,7 +16644,9 @@
       <c r="A905" s="1">
         <v>42310</v>
       </c>
-      <c r="B905" s="5"/>
+      <c r="B905" s="6">
+        <v>0</v>
+      </c>
       <c r="E905" t="s">
         <v>24</v>
       </c>
@@ -16002,7 +16658,9 @@
       <c r="A906" s="1">
         <v>42310</v>
       </c>
-      <c r="B906" s="5"/>
+      <c r="B906" s="6">
+        <v>0</v>
+      </c>
       <c r="E906" t="s">
         <v>8</v>
       </c>
@@ -16014,7 +16672,9 @@
       <c r="A907" s="1">
         <v>42310</v>
       </c>
-      <c r="B907" s="5"/>
+      <c r="B907" s="6">
+        <v>0</v>
+      </c>
       <c r="E907" t="s">
         <v>10</v>
       </c>
@@ -16026,7 +16686,9 @@
       <c r="A908" s="1">
         <v>42310</v>
       </c>
-      <c r="B908" s="5"/>
+      <c r="B908" s="6">
+        <v>0</v>
+      </c>
       <c r="E908" t="s">
         <v>12</v>
       </c>
@@ -16038,7 +16700,9 @@
       <c r="A909" s="1">
         <v>42310</v>
       </c>
-      <c r="B909" s="5"/>
+      <c r="B909" s="6">
+        <v>0</v>
+      </c>
       <c r="E909" t="s">
         <v>14</v>
       </c>
@@ -16673,7 +17337,9 @@
       <c r="A946" s="1">
         <v>42317</v>
       </c>
-      <c r="B946" s="5"/>
+      <c r="B946" s="6">
+        <v>0</v>
+      </c>
       <c r="D946" s="5"/>
       <c r="E946" t="s">
         <v>1</v>
@@ -16686,7 +17352,9 @@
       <c r="A947" s="1">
         <v>42317</v>
       </c>
-      <c r="B947" s="5"/>
+      <c r="B947" s="6">
+        <v>0</v>
+      </c>
       <c r="D947" s="5"/>
       <c r="E947" t="s">
         <v>2</v>
@@ -16699,7 +17367,9 @@
       <c r="A948" s="1">
         <v>42317</v>
       </c>
-      <c r="B948" s="5"/>
+      <c r="B948" s="6">
+        <v>0</v>
+      </c>
       <c r="D948" s="5"/>
       <c r="E948" t="s">
         <v>3</v>
@@ -16712,7 +17382,9 @@
       <c r="A949" s="1">
         <v>42317</v>
       </c>
-      <c r="B949" s="5"/>
+      <c r="B949" s="6">
+        <v>0</v>
+      </c>
       <c r="D949" s="5"/>
       <c r="E949" t="s">
         <v>4</v>
@@ -16725,7 +17397,9 @@
       <c r="A950" s="1">
         <v>42317</v>
       </c>
-      <c r="B950" s="5"/>
+      <c r="B950" s="6">
+        <v>0</v>
+      </c>
       <c r="D950" s="5"/>
       <c r="E950" t="s">
         <v>6</v>
@@ -16738,7 +17412,9 @@
       <c r="A951" s="1">
         <v>42317</v>
       </c>
-      <c r="B951" s="5"/>
+      <c r="B951" s="6">
+        <v>0</v>
+      </c>
       <c r="D951" s="5"/>
       <c r="E951" t="s">
         <v>7</v>
@@ -16751,7 +17427,9 @@
       <c r="A952" s="1">
         <v>42317</v>
       </c>
-      <c r="B952" s="5"/>
+      <c r="B952" s="6">
+        <v>0</v>
+      </c>
       <c r="D952" s="5"/>
       <c r="E952" t="s">
         <v>9</v>
@@ -16764,7 +17442,9 @@
       <c r="A953" s="1">
         <v>42317</v>
       </c>
-      <c r="B953" s="5"/>
+      <c r="B953" s="6">
+        <v>0</v>
+      </c>
       <c r="D953" s="5"/>
       <c r="E953" t="s">
         <v>11</v>
@@ -16777,7 +17457,9 @@
       <c r="A954" s="1">
         <v>42317</v>
       </c>
-      <c r="B954" s="5"/>
+      <c r="B954" s="6">
+        <v>0</v>
+      </c>
       <c r="D954" s="5"/>
       <c r="E954" t="s">
         <v>13</v>
@@ -16790,7 +17472,9 @@
       <c r="A955" s="1">
         <v>42317</v>
       </c>
-      <c r="B955" s="5"/>
+      <c r="B955" s="6">
+        <v>0</v>
+      </c>
       <c r="D955" s="5"/>
       <c r="E955" t="s">
         <v>15</v>
@@ -16803,7 +17487,9 @@
       <c r="A956" s="1">
         <v>42317</v>
       </c>
-      <c r="B956" s="5"/>
+      <c r="B956" s="6">
+        <v>0</v>
+      </c>
       <c r="D956" s="5"/>
       <c r="E956" t="s">
         <v>16</v>
@@ -16816,7 +17502,9 @@
       <c r="A957" s="1">
         <v>42317</v>
       </c>
-      <c r="B957" s="5"/>
+      <c r="B957" s="6">
+        <v>0</v>
+      </c>
       <c r="D957" s="5"/>
       <c r="E957" t="s">
         <v>17</v>
@@ -16829,7 +17517,9 @@
       <c r="A958" s="1">
         <v>42317</v>
       </c>
-      <c r="B958" s="5"/>
+      <c r="B958" s="6">
+        <v>0</v>
+      </c>
       <c r="D958" s="5"/>
       <c r="E958" t="s">
         <v>18</v>
@@ -16842,7 +17532,9 @@
       <c r="A959" s="1">
         <v>42317</v>
       </c>
-      <c r="B959" s="5"/>
+      <c r="B959" s="6">
+        <v>0</v>
+      </c>
       <c r="D959" s="5"/>
       <c r="E959" t="s">
         <v>19</v>
@@ -16855,7 +17547,9 @@
       <c r="A960" s="1">
         <v>42317</v>
       </c>
-      <c r="B960" s="5"/>
+      <c r="B960" s="6">
+        <v>0</v>
+      </c>
       <c r="D960" s="5"/>
       <c r="E960" t="s">
         <v>20</v>
@@ -16868,7 +17562,9 @@
       <c r="A961" s="1">
         <v>42317</v>
       </c>
-      <c r="B961" s="5"/>
+      <c r="B961" s="6">
+        <v>0</v>
+      </c>
       <c r="D961" s="5"/>
       <c r="E961" t="s">
         <v>21</v>
@@ -16881,7 +17577,9 @@
       <c r="A962" s="1">
         <v>42317</v>
       </c>
-      <c r="B962" s="5"/>
+      <c r="B962" s="6">
+        <v>0</v>
+      </c>
       <c r="D962" s="5"/>
       <c r="E962" t="s">
         <v>22</v>
@@ -16894,7 +17592,9 @@
       <c r="A963" s="1">
         <v>42317</v>
       </c>
-      <c r="B963" s="5"/>
+      <c r="B963" s="6">
+        <v>0</v>
+      </c>
       <c r="D963" s="5"/>
       <c r="E963" t="s">
         <v>23</v>
@@ -16907,7 +17607,9 @@
       <c r="A964" s="1">
         <v>42317</v>
       </c>
-      <c r="B964" s="5"/>
+      <c r="B964" s="6">
+        <v>0</v>
+      </c>
       <c r="D964" s="5"/>
       <c r="E964" t="s">
         <v>25</v>
@@ -16920,7 +17622,9 @@
       <c r="A965" s="1">
         <v>42317</v>
       </c>
-      <c r="B965" s="5"/>
+      <c r="B965" s="6">
+        <v>0</v>
+      </c>
       <c r="D965" s="5"/>
       <c r="E965" t="s">
         <v>26</v>
@@ -16933,7 +17637,9 @@
       <c r="A966" s="1">
         <v>42317</v>
       </c>
-      <c r="B966" s="5"/>
+      <c r="B966" s="6">
+        <v>0</v>
+      </c>
       <c r="D966" s="5"/>
       <c r="E966" t="s">
         <v>27</v>
@@ -16946,7 +17652,9 @@
       <c r="A967" s="1">
         <v>42317</v>
       </c>
-      <c r="B967" s="5"/>
+      <c r="B967" s="6">
+        <v>0</v>
+      </c>
       <c r="D967" s="5"/>
       <c r="E967" t="s">
         <v>28</v>
@@ -16959,7 +17667,9 @@
       <c r="A968" s="1">
         <v>42317</v>
       </c>
-      <c r="B968" s="5"/>
+      <c r="B968" s="6">
+        <v>0</v>
+      </c>
       <c r="D968" s="5"/>
       <c r="E968" t="s">
         <v>29</v>
@@ -16972,7 +17682,9 @@
       <c r="A969" s="1">
         <v>42317</v>
       </c>
-      <c r="B969" s="5"/>
+      <c r="B969" s="6">
+        <v>0</v>
+      </c>
       <c r="D969" s="5"/>
       <c r="E969" t="s">
         <v>30</v>
@@ -16985,7 +17697,9 @@
       <c r="A970" s="1">
         <v>42317</v>
       </c>
-      <c r="B970" s="5"/>
+      <c r="B970" s="6">
+        <v>0</v>
+      </c>
       <c r="D970" s="5"/>
       <c r="E970" t="s">
         <v>5</v>
@@ -16998,7 +17712,9 @@
       <c r="A971" s="1">
         <v>42317</v>
       </c>
-      <c r="B971" s="5"/>
+      <c r="B971" s="6">
+        <v>0</v>
+      </c>
       <c r="D971" s="5"/>
       <c r="E971" t="s">
         <v>24</v>
@@ -17011,7 +17727,9 @@
       <c r="A972" s="1">
         <v>42317</v>
       </c>
-      <c r="B972" s="5"/>
+      <c r="B972" s="6">
+        <v>0</v>
+      </c>
       <c r="D972" s="5"/>
       <c r="E972" t="s">
         <v>8</v>
@@ -17024,7 +17742,9 @@
       <c r="A973" s="1">
         <v>42317</v>
       </c>
-      <c r="B973" s="5"/>
+      <c r="B973" s="6">
+        <v>0</v>
+      </c>
       <c r="D973" s="5"/>
       <c r="E973" t="s">
         <v>10</v>
@@ -17037,7 +17757,9 @@
       <c r="A974" s="1">
         <v>42317</v>
       </c>
-      <c r="B974" s="5"/>
+      <c r="B974" s="6">
+        <v>0</v>
+      </c>
       <c r="D974" s="5"/>
       <c r="E974" t="s">
         <v>12</v>
@@ -17050,7 +17772,9 @@
       <c r="A975" s="1">
         <v>42317</v>
       </c>
-      <c r="B975" s="5"/>
+      <c r="B975" s="6">
+        <v>0</v>
+      </c>
       <c r="D975" s="5"/>
       <c r="E975" t="s">
         <v>14</v>
@@ -17797,7 +18521,9 @@
       <c r="A1018" s="1">
         <v>42327</v>
       </c>
-      <c r="B1018" s="5"/>
+      <c r="B1018" s="6">
+        <v>0</v>
+      </c>
       <c r="E1018" t="s">
         <v>1</v>
       </c>
@@ -17809,7 +18535,9 @@
       <c r="A1019" s="1">
         <v>42327</v>
       </c>
-      <c r="B1019" s="5"/>
+      <c r="B1019" s="6">
+        <v>0</v>
+      </c>
       <c r="E1019" t="s">
         <v>2</v>
       </c>
@@ -17821,7 +18549,9 @@
       <c r="A1020" s="1">
         <v>42327</v>
       </c>
-      <c r="B1020" s="5"/>
+      <c r="B1020" s="6">
+        <v>0</v>
+      </c>
       <c r="E1020" t="s">
         <v>3</v>
       </c>
@@ -17833,7 +18563,9 @@
       <c r="A1021" s="1">
         <v>42327</v>
       </c>
-      <c r="B1021" s="5"/>
+      <c r="B1021" s="6">
+        <v>0</v>
+      </c>
       <c r="E1021" t="s">
         <v>4</v>
       </c>
@@ -17845,7 +18577,9 @@
       <c r="A1022" s="1">
         <v>42327</v>
       </c>
-      <c r="B1022" s="5"/>
+      <c r="B1022" s="6">
+        <v>0</v>
+      </c>
       <c r="E1022" t="s">
         <v>6</v>
       </c>
@@ -17857,7 +18591,9 @@
       <c r="A1023" s="1">
         <v>42327</v>
       </c>
-      <c r="B1023" s="5"/>
+      <c r="B1023" s="6">
+        <v>0</v>
+      </c>
       <c r="E1023" t="s">
         <v>7</v>
       </c>
@@ -17869,7 +18605,9 @@
       <c r="A1024" s="1">
         <v>42327</v>
       </c>
-      <c r="B1024" s="5"/>
+      <c r="B1024" s="6">
+        <v>0</v>
+      </c>
       <c r="E1024" t="s">
         <v>9</v>
       </c>
@@ -17881,7 +18619,9 @@
       <c r="A1025" s="1">
         <v>42327</v>
       </c>
-      <c r="B1025" s="5"/>
+      <c r="B1025" s="6">
+        <v>0</v>
+      </c>
       <c r="E1025" t="s">
         <v>11</v>
       </c>
@@ -17893,7 +18633,9 @@
       <c r="A1026" s="1">
         <v>42327</v>
       </c>
-      <c r="B1026" s="5"/>
+      <c r="B1026" s="6">
+        <v>0</v>
+      </c>
       <c r="E1026" t="s">
         <v>13</v>
       </c>
@@ -17905,7 +18647,9 @@
       <c r="A1027" s="1">
         <v>42327</v>
       </c>
-      <c r="B1027" s="5"/>
+      <c r="B1027" s="6">
+        <v>0</v>
+      </c>
       <c r="E1027" t="s">
         <v>15</v>
       </c>
@@ -17917,7 +18661,9 @@
       <c r="A1028" s="1">
         <v>42327</v>
       </c>
-      <c r="B1028" s="5"/>
+      <c r="B1028" s="6">
+        <v>0</v>
+      </c>
       <c r="E1028" t="s">
         <v>16</v>
       </c>
@@ -17929,7 +18675,9 @@
       <c r="A1029" s="1">
         <v>42327</v>
       </c>
-      <c r="B1029" s="5"/>
+      <c r="B1029" s="6">
+        <v>0</v>
+      </c>
       <c r="E1029" t="s">
         <v>17</v>
       </c>
@@ -17941,7 +18689,9 @@
       <c r="A1030" s="1">
         <v>42327</v>
       </c>
-      <c r="B1030" s="5"/>
+      <c r="B1030" s="6">
+        <v>0</v>
+      </c>
       <c r="E1030" t="s">
         <v>18</v>
       </c>
@@ -17953,7 +18703,9 @@
       <c r="A1031" s="1">
         <v>42327</v>
       </c>
-      <c r="B1031" s="5"/>
+      <c r="B1031" s="6">
+        <v>0</v>
+      </c>
       <c r="E1031" t="s">
         <v>19</v>
       </c>
@@ -17965,7 +18717,9 @@
       <c r="A1032" s="1">
         <v>42327</v>
       </c>
-      <c r="B1032" s="5"/>
+      <c r="B1032" s="6">
+        <v>0</v>
+      </c>
       <c r="E1032" t="s">
         <v>20</v>
       </c>
@@ -17977,7 +18731,9 @@
       <c r="A1033" s="1">
         <v>42327</v>
       </c>
-      <c r="B1033" s="5"/>
+      <c r="B1033" s="6">
+        <v>0</v>
+      </c>
       <c r="E1033" t="s">
         <v>21</v>
       </c>
@@ -17989,7 +18745,9 @@
       <c r="A1034" s="1">
         <v>42327</v>
       </c>
-      <c r="B1034" s="5"/>
+      <c r="B1034" s="6">
+        <v>0</v>
+      </c>
       <c r="E1034" t="s">
         <v>22</v>
       </c>
@@ -18001,7 +18759,9 @@
       <c r="A1035" s="1">
         <v>42327</v>
       </c>
-      <c r="B1035" s="5"/>
+      <c r="B1035" s="6">
+        <v>0</v>
+      </c>
       <c r="E1035" t="s">
         <v>23</v>
       </c>
@@ -18013,7 +18773,9 @@
       <c r="A1036" s="1">
         <v>42327</v>
       </c>
-      <c r="B1036" s="5"/>
+      <c r="B1036" s="6">
+        <v>0</v>
+      </c>
       <c r="E1036" t="s">
         <v>25</v>
       </c>
@@ -18025,7 +18787,9 @@
       <c r="A1037" s="1">
         <v>42327</v>
       </c>
-      <c r="B1037" s="5"/>
+      <c r="B1037" s="6">
+        <v>0</v>
+      </c>
       <c r="E1037" t="s">
         <v>26</v>
       </c>
@@ -18037,7 +18801,9 @@
       <c r="A1038" s="1">
         <v>42327</v>
       </c>
-      <c r="B1038" s="5"/>
+      <c r="B1038" s="6">
+        <v>0</v>
+      </c>
       <c r="E1038" t="s">
         <v>27</v>
       </c>
@@ -18049,7 +18815,9 @@
       <c r="A1039" s="1">
         <v>42327</v>
       </c>
-      <c r="B1039" s="5"/>
+      <c r="B1039" s="6">
+        <v>0</v>
+      </c>
       <c r="E1039" t="s">
         <v>28</v>
       </c>
@@ -18061,7 +18829,9 @@
       <c r="A1040" s="1">
         <v>42327</v>
       </c>
-      <c r="B1040" s="5"/>
+      <c r="B1040" s="6">
+        <v>0</v>
+      </c>
       <c r="E1040" t="s">
         <v>29</v>
       </c>
@@ -18073,7 +18843,9 @@
       <c r="A1041" s="1">
         <v>42327</v>
       </c>
-      <c r="B1041" s="5"/>
+      <c r="B1041" s="6">
+        <v>0</v>
+      </c>
       <c r="E1041" t="s">
         <v>30</v>
       </c>
@@ -18085,7 +18857,9 @@
       <c r="A1042" s="1">
         <v>42327</v>
       </c>
-      <c r="B1042" s="5"/>
+      <c r="B1042" s="6">
+        <v>0</v>
+      </c>
       <c r="E1042" t="s">
         <v>5</v>
       </c>
@@ -18097,7 +18871,9 @@
       <c r="A1043" s="1">
         <v>42327</v>
       </c>
-      <c r="B1043" s="5"/>
+      <c r="B1043" s="6">
+        <v>0</v>
+      </c>
       <c r="E1043" t="s">
         <v>24</v>
       </c>
@@ -18109,7 +18885,9 @@
       <c r="A1044" s="1">
         <v>42327</v>
       </c>
-      <c r="B1044" s="5"/>
+      <c r="B1044" s="6">
+        <v>0</v>
+      </c>
       <c r="E1044" t="s">
         <v>8</v>
       </c>
@@ -18121,7 +18899,9 @@
       <c r="A1045" s="1">
         <v>42327</v>
       </c>
-      <c r="B1045" s="5"/>
+      <c r="B1045" s="6">
+        <v>0</v>
+      </c>
       <c r="E1045" t="s">
         <v>10</v>
       </c>
@@ -18133,7 +18913,9 @@
       <c r="A1046" s="1">
         <v>42327</v>
       </c>
-      <c r="B1046" s="5"/>
+      <c r="B1046" s="6">
+        <v>0</v>
+      </c>
       <c r="E1046" t="s">
         <v>12</v>
       </c>
@@ -18145,7 +18927,9 @@
       <c r="A1047" s="1">
         <v>42327</v>
       </c>
-      <c r="B1047" s="5"/>
+      <c r="B1047" s="6">
+        <v>0</v>
+      </c>
       <c r="E1047" t="s">
         <v>14</v>
       </c>
@@ -18771,7 +19555,9 @@
       <c r="A1084" s="1">
         <v>42332</v>
       </c>
-      <c r="B1084" s="5"/>
+      <c r="B1084" s="6">
+        <v>0</v>
+      </c>
       <c r="E1084" t="s">
         <v>1</v>
       </c>
@@ -18783,7 +19569,9 @@
       <c r="A1085" s="1">
         <v>42332</v>
       </c>
-      <c r="B1085" s="5"/>
+      <c r="B1085" s="6">
+        <v>0</v>
+      </c>
       <c r="E1085" t="s">
         <v>2</v>
       </c>
@@ -18795,7 +19583,9 @@
       <c r="A1086" s="1">
         <v>42332</v>
       </c>
-      <c r="B1086" s="5"/>
+      <c r="B1086" s="6">
+        <v>0</v>
+      </c>
       <c r="E1086" t="s">
         <v>3</v>
       </c>
@@ -18807,7 +19597,9 @@
       <c r="A1087" s="1">
         <v>42332</v>
       </c>
-      <c r="B1087" s="5"/>
+      <c r="B1087" s="6">
+        <v>0</v>
+      </c>
       <c r="E1087" t="s">
         <v>4</v>
       </c>
@@ -18819,7 +19611,9 @@
       <c r="A1088" s="1">
         <v>42332</v>
       </c>
-      <c r="B1088" s="5"/>
+      <c r="B1088" s="6">
+        <v>0</v>
+      </c>
       <c r="E1088" t="s">
         <v>6</v>
       </c>
@@ -18831,7 +19625,9 @@
       <c r="A1089" s="1">
         <v>42332</v>
       </c>
-      <c r="B1089" s="5"/>
+      <c r="B1089" s="6">
+        <v>0</v>
+      </c>
       <c r="E1089" t="s">
         <v>7</v>
       </c>
@@ -18843,7 +19639,9 @@
       <c r="A1090" s="1">
         <v>42332</v>
       </c>
-      <c r="B1090" s="5"/>
+      <c r="B1090" s="6">
+        <v>0</v>
+      </c>
       <c r="E1090" t="s">
         <v>9</v>
       </c>
@@ -18855,7 +19653,9 @@
       <c r="A1091" s="1">
         <v>42332</v>
       </c>
-      <c r="B1091" s="5"/>
+      <c r="B1091" s="6">
+        <v>0</v>
+      </c>
       <c r="E1091" t="s">
         <v>11</v>
       </c>
@@ -18867,7 +19667,9 @@
       <c r="A1092" s="1">
         <v>42332</v>
       </c>
-      <c r="B1092" s="5"/>
+      <c r="B1092" s="6">
+        <v>0</v>
+      </c>
       <c r="E1092" t="s">
         <v>13</v>
       </c>
@@ -18879,7 +19681,9 @@
       <c r="A1093" s="1">
         <v>42332</v>
       </c>
-      <c r="B1093" s="5"/>
+      <c r="B1093" s="6">
+        <v>0</v>
+      </c>
       <c r="E1093" t="s">
         <v>15</v>
       </c>
@@ -18891,7 +19695,9 @@
       <c r="A1094" s="1">
         <v>42332</v>
       </c>
-      <c r="B1094" s="5"/>
+      <c r="B1094" s="6">
+        <v>0</v>
+      </c>
       <c r="E1094" t="s">
         <v>16</v>
       </c>
@@ -18903,7 +19709,9 @@
       <c r="A1095" s="1">
         <v>42332</v>
       </c>
-      <c r="B1095" s="5"/>
+      <c r="B1095" s="6">
+        <v>0</v>
+      </c>
       <c r="E1095" t="s">
         <v>17</v>
       </c>
@@ -18915,7 +19723,9 @@
       <c r="A1096" s="1">
         <v>42332</v>
       </c>
-      <c r="B1096" s="5"/>
+      <c r="B1096" s="6">
+        <v>0</v>
+      </c>
       <c r="E1096" t="s">
         <v>18</v>
       </c>
@@ -18927,7 +19737,9 @@
       <c r="A1097" s="1">
         <v>42332</v>
       </c>
-      <c r="B1097" s="5"/>
+      <c r="B1097" s="6">
+        <v>0</v>
+      </c>
       <c r="E1097" t="s">
         <v>19</v>
       </c>
@@ -18939,7 +19751,9 @@
       <c r="A1098" s="1">
         <v>42332</v>
       </c>
-      <c r="B1098" s="5"/>
+      <c r="B1098" s="6">
+        <v>0</v>
+      </c>
       <c r="E1098" t="s">
         <v>20</v>
       </c>
@@ -18951,7 +19765,9 @@
       <c r="A1099" s="1">
         <v>42332</v>
       </c>
-      <c r="B1099" s="5"/>
+      <c r="B1099" s="6">
+        <v>0</v>
+      </c>
       <c r="E1099" t="s">
         <v>21</v>
       </c>
@@ -18963,7 +19779,9 @@
       <c r="A1100" s="1">
         <v>42332</v>
       </c>
-      <c r="B1100" s="5"/>
+      <c r="B1100" s="6">
+        <v>0</v>
+      </c>
       <c r="E1100" t="s">
         <v>22</v>
       </c>
@@ -18975,7 +19793,9 @@
       <c r="A1101" s="1">
         <v>42332</v>
       </c>
-      <c r="B1101" s="5"/>
+      <c r="B1101" s="6">
+        <v>0</v>
+      </c>
       <c r="E1101" t="s">
         <v>23</v>
       </c>
@@ -18987,7 +19807,9 @@
       <c r="A1102" s="1">
         <v>42332</v>
       </c>
-      <c r="B1102" s="5"/>
+      <c r="B1102" s="6">
+        <v>0</v>
+      </c>
       <c r="E1102" t="s">
         <v>25</v>
       </c>
@@ -18999,7 +19821,9 @@
       <c r="A1103" s="1">
         <v>42332</v>
       </c>
-      <c r="B1103" s="5"/>
+      <c r="B1103" s="6">
+        <v>0</v>
+      </c>
       <c r="E1103" t="s">
         <v>26</v>
       </c>
@@ -19011,7 +19835,9 @@
       <c r="A1104" s="1">
         <v>42332</v>
       </c>
-      <c r="B1104" s="5"/>
+      <c r="B1104" s="6">
+        <v>0</v>
+      </c>
       <c r="E1104" t="s">
         <v>27</v>
       </c>
@@ -19023,7 +19849,9 @@
       <c r="A1105" s="1">
         <v>42332</v>
       </c>
-      <c r="B1105" s="5"/>
+      <c r="B1105" s="6">
+        <v>0</v>
+      </c>
       <c r="E1105" t="s">
         <v>28</v>
       </c>
@@ -19035,7 +19863,9 @@
       <c r="A1106" s="1">
         <v>42332</v>
       </c>
-      <c r="B1106" s="5"/>
+      <c r="B1106" s="6">
+        <v>0</v>
+      </c>
       <c r="E1106" t="s">
         <v>29</v>
       </c>
@@ -19047,7 +19877,9 @@
       <c r="A1107" s="1">
         <v>42332</v>
       </c>
-      <c r="B1107" s="5"/>
+      <c r="B1107" s="6">
+        <v>0</v>
+      </c>
       <c r="E1107" t="s">
         <v>30</v>
       </c>
@@ -19059,7 +19891,9 @@
       <c r="A1108" s="1">
         <v>42332</v>
       </c>
-      <c r="B1108" s="5"/>
+      <c r="B1108" s="6">
+        <v>0</v>
+      </c>
       <c r="E1108" t="s">
         <v>5</v>
       </c>
@@ -19071,7 +19905,9 @@
       <c r="A1109" s="1">
         <v>42332</v>
       </c>
-      <c r="B1109" s="5"/>
+      <c r="B1109" s="6">
+        <v>0</v>
+      </c>
       <c r="E1109" t="s">
         <v>24</v>
       </c>
@@ -19083,7 +19919,9 @@
       <c r="A1110" s="1">
         <v>42332</v>
       </c>
-      <c r="B1110" s="5"/>
+      <c r="B1110" s="6">
+        <v>0</v>
+      </c>
       <c r="E1110" t="s">
         <v>8</v>
       </c>
@@ -19095,7 +19933,9 @@
       <c r="A1111" s="1">
         <v>42332</v>
       </c>
-      <c r="B1111" s="5"/>
+      <c r="B1111" s="6">
+        <v>0</v>
+      </c>
       <c r="E1111" t="s">
         <v>10</v>
       </c>
@@ -19107,7 +19947,9 @@
       <c r="A1112" s="1">
         <v>42332</v>
       </c>
-      <c r="B1112" s="5"/>
+      <c r="B1112" s="6">
+        <v>0</v>
+      </c>
       <c r="E1112" t="s">
         <v>12</v>
       </c>
@@ -19119,7 +19961,9 @@
       <c r="A1113" s="1">
         <v>42332</v>
       </c>
-      <c r="B1113" s="5"/>
+      <c r="B1113" s="6">
+        <v>0</v>
+      </c>
       <c r="E1113" t="s">
         <v>14</v>
       </c>
@@ -19753,6 +20597,9 @@
       <c r="A1150" s="1">
         <v>42346</v>
       </c>
+      <c r="B1150" s="6">
+        <v>0</v>
+      </c>
       <c r="C1150"/>
       <c r="E1150" s="8" t="s">
         <v>1</v>
@@ -19765,6 +20612,9 @@
       <c r="A1151" s="1">
         <v>42346</v>
       </c>
+      <c r="B1151" s="6">
+        <v>0</v>
+      </c>
       <c r="C1151"/>
       <c r="E1151" s="8" t="s">
         <v>2</v>
@@ -19777,6 +20627,9 @@
       <c r="A1152" s="1">
         <v>42346</v>
       </c>
+      <c r="B1152" s="6">
+        <v>0</v>
+      </c>
       <c r="C1152"/>
       <c r="E1152" s="8" t="s">
         <v>3</v>
@@ -19789,6 +20642,9 @@
       <c r="A1153" s="1">
         <v>42346</v>
       </c>
+      <c r="B1153" s="6">
+        <v>0</v>
+      </c>
       <c r="C1153"/>
       <c r="E1153" s="8" t="s">
         <v>4</v>
@@ -19801,6 +20657,9 @@
       <c r="A1154" s="1">
         <v>42346</v>
       </c>
+      <c r="B1154" s="6">
+        <v>0</v>
+      </c>
       <c r="C1154"/>
       <c r="E1154" s="8" t="s">
         <v>6</v>
@@ -19813,6 +20672,9 @@
       <c r="A1155" s="1">
         <v>42346</v>
       </c>
+      <c r="B1155" s="6">
+        <v>0</v>
+      </c>
       <c r="C1155"/>
       <c r="E1155" s="8" t="s">
         <v>7</v>
@@ -19825,6 +20687,9 @@
       <c r="A1156" s="1">
         <v>42346</v>
       </c>
+      <c r="B1156" s="6">
+        <v>0</v>
+      </c>
       <c r="C1156"/>
       <c r="E1156" s="8" t="s">
         <v>9</v>
@@ -19837,6 +20702,9 @@
       <c r="A1157" s="1">
         <v>42346</v>
       </c>
+      <c r="B1157" s="6">
+        <v>0</v>
+      </c>
       <c r="C1157"/>
       <c r="E1157" s="8" t="s">
         <v>11</v>
@@ -19849,6 +20717,9 @@
       <c r="A1158" s="1">
         <v>42346</v>
       </c>
+      <c r="B1158" s="6">
+        <v>0</v>
+      </c>
       <c r="C1158"/>
       <c r="E1158" t="s">
         <v>13</v>
@@ -19861,6 +20732,9 @@
       <c r="A1159" s="1">
         <v>42346</v>
       </c>
+      <c r="B1159" s="6">
+        <v>0</v>
+      </c>
       <c r="C1159"/>
       <c r="E1159" t="s">
         <v>15</v>
@@ -19873,6 +20747,9 @@
       <c r="A1160" s="1">
         <v>42346</v>
       </c>
+      <c r="B1160" s="6">
+        <v>0</v>
+      </c>
       <c r="C1160"/>
       <c r="E1160" t="s">
         <v>16</v>
@@ -19885,6 +20762,9 @@
       <c r="A1161" s="1">
         <v>42346</v>
       </c>
+      <c r="B1161" s="6">
+        <v>0</v>
+      </c>
       <c r="C1161"/>
       <c r="E1161" t="s">
         <v>17</v>
@@ -19897,6 +20777,9 @@
       <c r="A1162" s="1">
         <v>42346</v>
       </c>
+      <c r="B1162" s="6">
+        <v>0</v>
+      </c>
       <c r="C1162"/>
       <c r="E1162" t="s">
         <v>18</v>
@@ -19909,6 +20792,9 @@
       <c r="A1163" s="1">
         <v>42346</v>
       </c>
+      <c r="B1163" s="6">
+        <v>0</v>
+      </c>
       <c r="C1163"/>
       <c r="E1163" t="s">
         <v>19</v>
@@ -19921,6 +20807,9 @@
       <c r="A1164" s="1">
         <v>42346</v>
       </c>
+      <c r="B1164" s="6">
+        <v>0</v>
+      </c>
       <c r="C1164"/>
       <c r="E1164" t="s">
         <v>20</v>
@@ -19933,6 +20822,9 @@
       <c r="A1165" s="1">
         <v>42346</v>
       </c>
+      <c r="B1165" s="6">
+        <v>0</v>
+      </c>
       <c r="C1165"/>
       <c r="E1165" t="s">
         <v>21</v>
@@ -19945,6 +20837,9 @@
       <c r="A1166" s="1">
         <v>42346</v>
       </c>
+      <c r="B1166" s="6">
+        <v>0</v>
+      </c>
       <c r="C1166"/>
       <c r="E1166" t="s">
         <v>22</v>
@@ -19957,6 +20852,9 @@
       <c r="A1167" s="1">
         <v>42346</v>
       </c>
+      <c r="B1167" s="6">
+        <v>0</v>
+      </c>
       <c r="C1167"/>
       <c r="E1167" t="s">
         <v>23</v>
@@ -19969,6 +20867,9 @@
       <c r="A1168" s="1">
         <v>42346</v>
       </c>
+      <c r="B1168" s="6">
+        <v>0</v>
+      </c>
       <c r="C1168"/>
       <c r="E1168" t="s">
         <v>25</v>
@@ -19981,6 +20882,9 @@
       <c r="A1169" s="1">
         <v>42346</v>
       </c>
+      <c r="B1169" s="6">
+        <v>0</v>
+      </c>
       <c r="C1169"/>
       <c r="E1169" t="s">
         <v>26</v>
@@ -19993,6 +20897,9 @@
       <c r="A1170" s="1">
         <v>42346</v>
       </c>
+      <c r="B1170" s="6">
+        <v>0</v>
+      </c>
       <c r="C1170"/>
       <c r="E1170" t="s">
         <v>27</v>
@@ -20005,6 +20912,9 @@
       <c r="A1171" s="1">
         <v>42346</v>
       </c>
+      <c r="B1171" s="6">
+        <v>0</v>
+      </c>
       <c r="C1171"/>
       <c r="E1171" t="s">
         <v>28</v>
@@ -20017,6 +20927,9 @@
       <c r="A1172" s="1">
         <v>42346</v>
       </c>
+      <c r="B1172" s="6">
+        <v>0</v>
+      </c>
       <c r="C1172"/>
       <c r="E1172" t="s">
         <v>29</v>
@@ -20029,6 +20942,9 @@
       <c r="A1173" s="1">
         <v>42346</v>
       </c>
+      <c r="B1173" s="6">
+        <v>0</v>
+      </c>
       <c r="C1173"/>
       <c r="E1173" t="s">
         <v>30</v>
@@ -20041,6 +20957,9 @@
       <c r="A1174" s="1">
         <v>42346</v>
       </c>
+      <c r="B1174" s="6">
+        <v>0</v>
+      </c>
       <c r="C1174"/>
       <c r="E1174" t="s">
         <v>5</v>
@@ -20053,6 +20972,9 @@
       <c r="A1175" s="1">
         <v>42346</v>
       </c>
+      <c r="B1175" s="6">
+        <v>0</v>
+      </c>
       <c r="C1175"/>
       <c r="E1175" t="s">
         <v>24</v>
@@ -20065,6 +20987,9 @@
       <c r="A1176" s="1">
         <v>42346</v>
       </c>
+      <c r="B1176" s="6">
+        <v>0</v>
+      </c>
       <c r="C1176"/>
       <c r="E1176" t="s">
         <v>8</v>
@@ -20077,6 +21002,9 @@
       <c r="A1177" s="1">
         <v>42346</v>
       </c>
+      <c r="B1177" s="6">
+        <v>0</v>
+      </c>
       <c r="C1177"/>
       <c r="E1177" t="s">
         <v>10</v>
@@ -20089,6 +21017,9 @@
       <c r="A1178" s="1">
         <v>42346</v>
       </c>
+      <c r="B1178" s="6">
+        <v>0</v>
+      </c>
       <c r="C1178"/>
       <c r="E1178" t="s">
         <v>12</v>
@@ -20100,6 +21031,9 @@
     <row r="1179" spans="1:6">
       <c r="A1179" s="1">
         <v>42346</v>
+      </c>
+      <c r="B1179" s="6">
+        <v>0</v>
       </c>
       <c r="C1179"/>
       <c r="E1179" t="s">

</xml_diff>

<commit_message>
Make CoreData.xlsx match the treatments.csv file
</commit_message>
<xml_diff>
--- a/data/CoreData.xlsx
+++ b/data/CoreData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24680" windowHeight="15600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24680" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="treatments.csv" sheetId="2" r:id="rId1"/>
@@ -351,8 +351,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="273">
+  <cellStyleXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -649,7 +651,7 @@
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="273">
+  <cellStyles count="275">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -786,6 +788,7 @@
     <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -922,6 +925,7 @@
     <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1223,9 +1227,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1265,7 +1269,7 @@
         <v>32</v>
       </c>
       <c r="C4">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1309,7 +1313,7 @@
         <v>33</v>
       </c>
       <c r="C8">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1331,7 +1335,7 @@
         <v>33</v>
       </c>
       <c r="C10">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1342,7 +1346,7 @@
         <v>35</v>
       </c>
       <c r="C11">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1353,7 +1357,7 @@
         <v>35</v>
       </c>
       <c r="C12">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1375,7 +1379,7 @@
         <v>33</v>
       </c>
       <c r="C14">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1386,7 +1390,7 @@
         <v>32</v>
       </c>
       <c r="C15">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1397,7 +1401,7 @@
         <v>33</v>
       </c>
       <c r="C16">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1408,7 +1412,7 @@
         <v>35</v>
       </c>
       <c r="C17">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1441,7 +1445,7 @@
         <v>35</v>
       </c>
       <c r="C20">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1452,7 +1456,7 @@
         <v>35</v>
       </c>
       <c r="C21">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1474,7 +1478,7 @@
         <v>32</v>
       </c>
       <c r="C23">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1496,7 +1500,7 @@
         <v>33</v>
       </c>
       <c r="C25">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1507,7 +1511,7 @@
         <v>32</v>
       </c>
       <c r="C26">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1518,7 +1522,7 @@
         <v>32</v>
       </c>
       <c r="C27">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1529,7 +1533,7 @@
         <v>32</v>
       </c>
       <c r="C28">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1540,7 +1544,7 @@
         <v>35</v>
       </c>
       <c r="C29">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1573,7 +1577,7 @@
         <v>33</v>
       </c>
       <c r="C32">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1584,7 +1588,7 @@
         <v>40</v>
       </c>
       <c r="C33">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1616,9 +1620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1215"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A405" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E427" sqref="E427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>